<commit_message>
data: add endpoint metric calculation for combining tools
</commit_message>
<xml_diff>
--- a/merged_results/complete_results.xlsx
+++ b/merged_results/complete_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/Documents/Own/Papers_and_Projects/comparison_ArchRec_tools/GitHub_SARbenchmarks/merged_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EA89DC-35B6-A44C-86EF-4B7F4D4746D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0EEA3F-7E49-4C46-9D66-151C8E236125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26840" xr2:uid="{21E6DDBE-06EB-864D-8BE4-57F9A90E46C0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" xr2:uid="{21E6DDBE-06EB-864D-8BE4-57F9A90E46C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Complete Results" sheetId="1" r:id="rId1"/>
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3289" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3292" uniqueCount="508">
   <si>
     <t xml:space="preserve"> RAD</t>
   </si>
@@ -1803,6 +1803,9 @@
   </si>
   <si>
     <t>RAS</t>
+  </si>
+  <si>
+    <t>This is done manually (checking each FP for overlaps)</t>
   </si>
 </sst>
 </file>
@@ -1985,7 +1988,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1993,6 +1996,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2032,6 +2036,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2432,11 +2437,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E181CEDB-9761-A944-9A62-062C9F034F3F}">
-  <dimension ref="A1:Y602"/>
+  <dimension ref="A1:Y600"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A549" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P595" sqref="P595"/>
+      <pane ySplit="2" topLeftCell="A573" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M597" sqref="M597"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2450,26 +2455,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="8" t="s">
         <v>469</v>
       </c>
-      <c r="L1" s="7"/>
+      <c r="L1" s="8"/>
       <c r="M1" s="2" t="s">
         <v>474</v>
       </c>
       <c r="N1" s="2"/>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="8" t="s">
         <v>472</v>
       </c>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7" t="s">
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8" t="s">
         <v>473</v>
       </c>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7" t="s">
+      <c r="R1" s="8"/>
+      <c r="S1" s="8" t="s">
         <v>475</v>
       </c>
-      <c r="T1" s="7"/>
+      <c r="T1" s="8"/>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
@@ -2479,55 +2484,55 @@
       <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>501</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="34" t="s">
         <v>502</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="34" t="s">
         <v>503</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="34" t="s">
         <v>504</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="35" t="s">
         <v>505</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="36" t="s">
         <v>506</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="9" t="s">
         <v>470</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="9" t="s">
         <v>471</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="9" t="s">
         <v>470</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="9" t="s">
         <v>471</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="9" t="s">
         <v>470</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="9" t="s">
         <v>471</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="9" t="s">
         <v>470</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="R2" s="9" t="s">
         <v>471</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="9" t="s">
         <v>470</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="9" t="s">
         <v>471</v>
       </c>
     </row>
@@ -2711,20 +2716,20 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="13"/>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
         <v>TP</v>
@@ -3940,22 +3945,22 @@
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H30" s="11"/>
-      <c r="I30" s="12"/>
+      <c r="C30" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="12"/>
+      <c r="I30" s="13"/>
       <c r="K30" t="str">
         <f t="shared" si="0"/>
         <v>TP</v>
@@ -4007,7 +4012,7 @@
       <c r="D31" t="s">
         <v>2</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I31" s="5" t="s">
@@ -4064,7 +4069,7 @@
       <c r="D32" t="s">
         <v>2</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I32" s="5" t="s">
@@ -7211,24 +7216,24 @@
       </c>
     </row>
     <row r="87" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B87" s="11" t="s">
+      <c r="B87" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C87" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D87" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E87" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F87" s="11"/>
-      <c r="G87" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H87" s="11"/>
-      <c r="I87" s="12"/>
+      <c r="C87" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E87" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F87" s="12"/>
+      <c r="G87" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H87" s="12"/>
+      <c r="I87" s="13"/>
       <c r="K87" t="str">
         <f t="shared" si="12"/>
         <v>TP</v>
@@ -7283,7 +7288,7 @@
       <c r="E88" t="s">
         <v>4</v>
       </c>
-      <c r="G88" s="10" t="s">
+      <c r="G88" s="11" t="s">
         <v>4</v>
       </c>
       <c r="H88" t="s">
@@ -7346,7 +7351,7 @@
       <c r="E89" t="s">
         <v>2</v>
       </c>
-      <c r="G89" s="10" t="s">
+      <c r="G89" s="11" t="s">
         <v>4</v>
       </c>
       <c r="H89" t="s">
@@ -9824,24 +9829,24 @@
       </c>
     </row>
     <row r="129" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B129" s="11" t="s">
+      <c r="B129" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="C129" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D129" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E129" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F129" s="11"/>
-      <c r="G129" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H129" s="11"/>
-      <c r="I129" s="12"/>
+      <c r="C129" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D129" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E129" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F129" s="12"/>
+      <c r="G129" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H129" s="12"/>
+      <c r="I129" s="13"/>
       <c r="K129" t="str">
         <f t="shared" si="12"/>
         <v>TP</v>
@@ -9896,7 +9901,7 @@
       <c r="E130" t="s">
         <v>2</v>
       </c>
-      <c r="G130" s="10" t="s">
+      <c r="G130" s="11" t="s">
         <v>4</v>
       </c>
       <c r="H130" t="s">
@@ -9959,7 +9964,7 @@
       <c r="E131" t="s">
         <v>2</v>
       </c>
-      <c r="G131" s="10" t="s">
+      <c r="G131" s="11" t="s">
         <v>4</v>
       </c>
       <c r="H131" t="s">
@@ -11011,26 +11016,26 @@
       </c>
     </row>
     <row r="148" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B148" s="11" t="s">
+      <c r="B148" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="C148" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D148" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E148" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F148" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G148" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H148" s="11"/>
-      <c r="I148" s="12"/>
+      <c r="C148" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D148" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E148" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F148" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G148" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H148" s="12"/>
+      <c r="I148" s="13"/>
       <c r="K148" t="str">
         <f t="shared" si="22"/>
         <v>TP</v>
@@ -11085,7 +11090,7 @@
       <c r="E149" t="s">
         <v>2</v>
       </c>
-      <c r="G149" s="10" t="s">
+      <c r="G149" s="11" t="s">
         <v>4</v>
       </c>
       <c r="H149" t="s">
@@ -11148,7 +11153,7 @@
       <c r="E150" t="s">
         <v>4</v>
       </c>
-      <c r="G150" s="10" t="s">
+      <c r="G150" s="11" t="s">
         <v>4</v>
       </c>
       <c r="H150" t="s">
@@ -11211,7 +11216,7 @@
       <c r="E151" t="s">
         <v>4</v>
       </c>
-      <c r="G151" s="10" t="s">
+      <c r="G151" s="11" t="s">
         <v>4</v>
       </c>
       <c r="H151" t="s">
@@ -11274,7 +11279,7 @@
       <c r="E152" t="s">
         <v>2</v>
       </c>
-      <c r="G152" s="10" t="s">
+      <c r="G152" s="11" t="s">
         <v>4</v>
       </c>
       <c r="H152" t="s">
@@ -12568,26 +12573,26 @@
       </c>
     </row>
     <row r="173" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B173" s="11" t="s">
+      <c r="B173" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C173" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D173" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E173" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F173" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G173" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H173" s="11"/>
-      <c r="I173" s="12"/>
+      <c r="C173" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D173" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E173" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F173" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G173" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H173" s="12"/>
+      <c r="I173" s="13"/>
       <c r="K173" t="str">
         <f t="shared" si="22"/>
         <v>TP</v>
@@ -15188,24 +15193,24 @@
       </c>
     </row>
     <row r="217" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B217" s="11" t="s">
+      <c r="B217" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="C217" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D217" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E217" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F217" s="11"/>
-      <c r="G217" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H217" s="11"/>
-      <c r="I217" s="12"/>
+      <c r="C217" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D217" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E217" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F217" s="12"/>
+      <c r="G217" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H217" s="12"/>
+      <c r="I217" s="13"/>
       <c r="K217" t="str">
         <f t="shared" si="32"/>
         <v>TP</v>
@@ -18323,24 +18328,24 @@
       </c>
     </row>
     <row r="268" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B268" s="11" t="s">
+      <c r="B268" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C268" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D268" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E268" s="11"/>
-      <c r="F268" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G268" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H268" s="11"/>
-      <c r="I268" s="12"/>
+      <c r="C268" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D268" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E268" s="12"/>
+      <c r="F268" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G268" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H268" s="12"/>
+      <c r="I268" s="13"/>
       <c r="K268" t="str">
         <f t="shared" si="42"/>
         <v>TP</v>
@@ -20917,20 +20922,20 @@
       </c>
     </row>
     <row r="313" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B313" s="11" t="s">
+      <c r="B313" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="C313" s="11"/>
-      <c r="D313" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E313" s="11"/>
-      <c r="F313" s="11"/>
-      <c r="G313" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H313" s="11"/>
-      <c r="I313" s="12"/>
+      <c r="C313" s="12"/>
+      <c r="D313" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E313" s="12"/>
+      <c r="F313" s="12"/>
+      <c r="G313" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H313" s="12"/>
+      <c r="I313" s="13"/>
       <c r="K313" t="str">
         <f t="shared" si="42"/>
         <v>TP</v>
@@ -21785,20 +21790,20 @@
       </c>
     </row>
     <row r="331" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B331" s="11" t="s">
+      <c r="B331" s="12" t="s">
         <v>310</v>
       </c>
-      <c r="C331" s="11"/>
-      <c r="D331" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E331" s="11"/>
-      <c r="F331" s="11"/>
-      <c r="G331" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H331" s="11"/>
-      <c r="I331" s="12"/>
+      <c r="C331" s="12"/>
+      <c r="D331" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E331" s="12"/>
+      <c r="F331" s="12"/>
+      <c r="G331" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H331" s="12"/>
+      <c r="I331" s="13"/>
       <c r="K331" t="str">
         <f t="shared" si="52"/>
         <v>TP</v>
@@ -22714,24 +22719,24 @@
       </c>
     </row>
     <row r="348" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B348" s="11" t="s">
+      <c r="B348" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C348" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D348" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E348" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F348" s="11"/>
-      <c r="G348" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H348" s="11"/>
-      <c r="I348" s="12"/>
+      <c r="C348" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D348" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E348" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F348" s="12"/>
+      <c r="G348" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H348" s="12"/>
+      <c r="I348" s="13"/>
       <c r="K348" t="str">
         <f t="shared" si="52"/>
         <v>TP</v>
@@ -24780,20 +24785,20 @@
       </c>
     </row>
     <row r="385" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B385" s="11" t="s">
+      <c r="B385" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C385" s="11"/>
-      <c r="D385" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E385" s="11"/>
-      <c r="F385" s="11"/>
-      <c r="G385" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H385" s="11"/>
-      <c r="I385" s="12"/>
+      <c r="C385" s="12"/>
+      <c r="D385" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E385" s="12"/>
+      <c r="F385" s="12"/>
+      <c r="G385" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H385" s="12"/>
+      <c r="I385" s="13"/>
       <c r="K385" t="str">
         <f t="shared" si="52"/>
         <v>TP</v>
@@ -26239,24 +26244,24 @@
       </c>
     </row>
     <row r="413" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B413" s="11" t="s">
+      <c r="B413" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="C413" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D413" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E413" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F413" s="11"/>
-      <c r="G413" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H413" s="11"/>
-      <c r="I413" s="12"/>
+      <c r="C413" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D413" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E413" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F413" s="12"/>
+      <c r="G413" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H413" s="12"/>
+      <c r="I413" s="13"/>
       <c r="K413" t="str">
         <f t="shared" si="62"/>
         <v>TP</v>
@@ -28625,24 +28630,24 @@
       </c>
     </row>
     <row r="453" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B453" s="11" t="s">
+      <c r="B453" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C453" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D453" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E453" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F453" s="11"/>
-      <c r="G453" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H453" s="11"/>
-      <c r="I453" s="12"/>
+      <c r="C453" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D453" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E453" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F453" s="12"/>
+      <c r="G453" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H453" s="12"/>
+      <c r="I453" s="13"/>
       <c r="K453" t="str">
         <f t="shared" si="72"/>
         <v>TP</v>
@@ -30873,26 +30878,26 @@
       </c>
     </row>
     <row r="489" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B489" s="11" t="s">
+      <c r="B489" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C489" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D489" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E489" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F489" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G489" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H489" s="11"/>
-      <c r="I489" s="12"/>
+      <c r="C489" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D489" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E489" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F489" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G489" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H489" s="12"/>
+      <c r="I489" s="13"/>
       <c r="K489" t="str">
         <f t="shared" si="72"/>
         <v>TP</v>
@@ -33080,22 +33085,22 @@
       </c>
     </row>
     <row r="526" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B526" s="11" t="s">
+      <c r="B526" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C526" s="11"/>
-      <c r="D526" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E526" s="11"/>
-      <c r="F526" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G526" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H526" s="11"/>
-      <c r="I526" s="12"/>
+      <c r="C526" s="12"/>
+      <c r="D526" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E526" s="12"/>
+      <c r="F526" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G526" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H526" s="12"/>
+      <c r="I526" s="13"/>
       <c r="K526" t="str">
         <f t="shared" si="82"/>
         <v>TP</v>
@@ -34491,24 +34496,24 @@
       </c>
     </row>
     <row r="553" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B553" s="11" t="s">
+      <c r="B553" s="12" t="s">
         <v>452</v>
       </c>
-      <c r="C553" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D553" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E553" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F553" s="11"/>
-      <c r="G553" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H553" s="11"/>
-      <c r="I553" s="12"/>
+      <c r="C553" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D553" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E553" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F553" s="12"/>
+      <c r="G553" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H553" s="12"/>
+      <c r="I553" s="13"/>
       <c r="K553" t="str">
         <f t="shared" si="82"/>
         <v>TP</v>
@@ -34991,7 +34996,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="561" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B561" t="s">
         <v>459</v>
       </c>
@@ -35054,7 +35059,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="562" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B562" t="s">
         <v>460</v>
       </c>
@@ -35117,7 +35122,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="563" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B563" t="s">
         <v>461</v>
       </c>
@@ -35180,7 +35185,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="564" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B564" t="s">
         <v>462</v>
       </c>
@@ -35243,7 +35248,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="565" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B565" t="s">
         <v>463</v>
       </c>
@@ -35306,7 +35311,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="566" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="566" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B566" t="s">
         <v>464</v>
       </c>
@@ -35369,7 +35374,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="567" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="567" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B567" t="s">
         <v>465</v>
       </c>
@@ -35432,7 +35437,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="568" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="568" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B568" t="s">
         <v>466</v>
       </c>
@@ -35495,7 +35500,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="569" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A569" s="4"/>
       <c r="B569" s="3" t="s">
         <v>467</v>
@@ -35560,246 +35565,461 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="572" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B572" s="17" t="s">
+    <row r="572" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B572" s="18" t="s">
         <v>476</v>
       </c>
-      <c r="C572" s="9">
-        <f>COUNTIF(C3:C569, " TP")</f>
+      <c r="C572" s="10">
+        <f>COUNTIF(C3:C569, " TP") + C593</f>
         <v>402</v>
       </c>
-      <c r="D572" s="9">
-        <f t="shared" ref="D572:I572" si="92">COUNTIF(D3:D569, " TP")</f>
-        <v>498</v>
-      </c>
-      <c r="E572" s="9">
+      <c r="D572" s="10">
+        <f t="shared" ref="D572:I572" si="92">COUNTIF(D3:D569, " TP") + D593</f>
+        <v>576</v>
+      </c>
+      <c r="E572" s="10">
         <f t="shared" si="92"/>
         <v>208</v>
       </c>
-      <c r="F572" s="9">
+      <c r="F572" s="10">
         <f t="shared" si="92"/>
         <v>32</v>
       </c>
-      <c r="G572" s="9">
+      <c r="G572" s="10">
         <f t="shared" si="92"/>
         <v>31</v>
       </c>
-      <c r="H572" s="9"/>
-      <c r="I572" s="23">
+      <c r="H572" s="10">
         <f t="shared" si="92"/>
-        <v>7</v>
-      </c>
-      <c r="K572">
-        <f>COUNTIF(K3:K569, "TP")</f>
-        <v>553</v>
-      </c>
-      <c r="L572">
-        <f t="shared" ref="L572:S572" si="93">COUNTIF(L3:L569, "TP")</f>
-        <v>24</v>
-      </c>
-      <c r="M572">
+        <v>90</v>
+      </c>
+      <c r="I572" s="24">
+        <f t="shared" si="92"/>
+        <v>92</v>
+      </c>
+      <c r="K572" s="11">
+        <f>COUNTIF(K3:K569, "TP") + K593</f>
+        <v>684</v>
+      </c>
+      <c r="L572" s="11">
+        <f>COUNTIF(L3:L569, "TP") + L593</f>
+        <v>76</v>
+      </c>
+      <c r="M572" s="11">
+        <f t="shared" ref="L572:S572" si="93">COUNTIF(M3:M569, "TP")</f>
+        <v>552</v>
+      </c>
+      <c r="N572" s="11">
+        <f t="shared" si="93"/>
+        <v>353</v>
+      </c>
+      <c r="O572" s="11">
         <f t="shared" si="93"/>
         <v>552</v>
       </c>
-      <c r="N572">
-        <f t="shared" si="93"/>
-        <v>353</v>
-      </c>
-      <c r="O572">
-        <f t="shared" si="93"/>
-        <v>552</v>
-      </c>
-      <c r="P572">
+      <c r="P572" s="11">
         <f t="shared" si="93"/>
         <v>437</v>
       </c>
-      <c r="Q572">
+      <c r="Q572" s="11">
         <f t="shared" si="93"/>
         <v>407</v>
       </c>
-      <c r="R572">
+      <c r="R572" s="11">
         <f t="shared" si="93"/>
         <v>203</v>
       </c>
-      <c r="S572">
+      <c r="S572" s="11">
         <f t="shared" si="93"/>
         <v>509</v>
       </c>
-      <c r="T572">
+      <c r="T572" s="11">
         <f>COUNTIF(T3:T569, "TP")</f>
         <v>372</v>
       </c>
     </row>
-    <row r="573" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B573" s="18" t="s">
+    <row r="573" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B573" s="19" t="s">
         <v>477</v>
       </c>
-      <c r="C573" s="13">
-        <f>COUNTIF(C3:C569, " FN")</f>
+      <c r="C573" s="14">
+        <f>COUNTIF(C3:C569, " FN") + C594</f>
         <v>66</v>
       </c>
-      <c r="D573" s="13">
-        <f>COUNTIF(D3:D569, " FN")</f>
-        <v>69</v>
-      </c>
-      <c r="E573" s="13">
-        <f>COUNTIF(E3:E569, " FN")</f>
+      <c r="D573" s="14">
+        <f t="shared" ref="D573:I573" si="94">COUNTIF(D3:D569, " FN") + D594</f>
+        <v>141</v>
+      </c>
+      <c r="E573" s="14">
+        <f t="shared" si="94"/>
         <v>147</v>
       </c>
-      <c r="F573" s="13">
-        <f>COUNTIF(F3:F569, " FN")</f>
+      <c r="F573" s="14">
+        <f t="shared" si="94"/>
         <v>25</v>
       </c>
-      <c r="G573" s="13">
-        <f>COUNTIF(G3:G569, " FN")</f>
+      <c r="G573" s="14">
+        <f t="shared" si="94"/>
         <v>536</v>
       </c>
-      <c r="H573" s="13">
-        <f>COUNTIF(H3:H569, " FN")</f>
-        <v>259</v>
-      </c>
-      <c r="I573" s="24">
-        <f>COUNTIF(I3:I569, " FN")</f>
-        <v>378</v>
-      </c>
-    </row>
-    <row r="574" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B574" s="19" t="s">
+      <c r="H573" s="14">
+        <f t="shared" si="94"/>
+        <v>291</v>
+      </c>
+      <c r="I573" s="25">
+        <f t="shared" si="94"/>
+        <v>443</v>
+      </c>
+      <c r="K573" s="14">
+        <f>COUNTIF(K3:K569, "FN") + K594</f>
+        <v>32</v>
+      </c>
+      <c r="L573" s="14">
+        <f>COUNTIF(L3:L569, "FN") + L594</f>
+        <v>640</v>
+      </c>
+      <c r="M573" s="14">
+        <f t="shared" ref="L573:T573" si="95">COUNTIF(M3:M569, "FN")</f>
+        <v>15</v>
+      </c>
+      <c r="N573" s="14">
+        <f t="shared" si="95"/>
+        <v>214</v>
+      </c>
+      <c r="O573" s="14">
+        <f t="shared" si="95"/>
+        <v>15</v>
+      </c>
+      <c r="P573" s="14">
+        <f t="shared" si="95"/>
+        <v>130</v>
+      </c>
+      <c r="Q573" s="14">
+        <f t="shared" si="95"/>
+        <v>62</v>
+      </c>
+      <c r="R573" s="14">
+        <f t="shared" si="95"/>
+        <v>266</v>
+      </c>
+      <c r="S573" s="14">
+        <f>COUNTIF(S3:S569, "FN")</f>
+        <v>58</v>
+      </c>
+      <c r="T573" s="14">
+        <f t="shared" si="95"/>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="574" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B574" s="20" t="s">
         <v>480</v>
       </c>
-      <c r="C574" s="14">
+      <c r="C574" s="15">
         <v>436</v>
       </c>
-      <c r="D574" s="14">
+      <c r="D574" s="15">
         <v>54</v>
       </c>
-      <c r="E574" s="14">
-        <v>2</v>
-      </c>
-      <c r="F574" s="14">
+      <c r="E574" s="15">
+        <v>2</v>
+      </c>
+      <c r="F574" s="15">
         <v>1</v>
       </c>
-      <c r="G574" s="14">
+      <c r="G574" s="15">
         <v>22</v>
       </c>
-      <c r="H574" s="14">
-        <v>2</v>
-      </c>
-      <c r="I574" s="25">
+      <c r="H574" s="15">
+        <v>2</v>
+      </c>
+      <c r="I574" s="26">
         <v>16</v>
       </c>
-    </row>
-    <row r="575" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B575" s="20" t="s">
+      <c r="J574" s="11"/>
+      <c r="K574" s="7">
+        <f>K581+K588+K595</f>
+        <v>517</v>
+      </c>
+      <c r="L574" s="7">
+        <v>2</v>
+      </c>
+      <c r="M574" s="7">
+        <f>M581+M588</f>
+        <v>458</v>
+      </c>
+      <c r="N574" s="7">
+        <v>0</v>
+      </c>
+      <c r="O574" s="7">
+        <f>O581+O588</f>
+        <v>458</v>
+      </c>
+      <c r="P574" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q574" s="7">
+        <f>Q581+Q588</f>
+        <v>437</v>
+      </c>
+      <c r="R574" s="7">
+        <v>0</v>
+      </c>
+      <c r="S574" s="7">
+        <f>S581+S588</f>
+        <v>34</v>
+      </c>
+      <c r="T574" s="11">
+        <v>0</v>
+      </c>
+      <c r="V574" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="575" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B575" s="21" t="s">
         <v>478</v>
       </c>
-      <c r="C575" s="28">
+      <c r="C575" s="29">
         <f>C572/(C572+C574)</f>
         <v>0.47971360381861577</v>
       </c>
-      <c r="D575" s="28">
-        <f t="shared" ref="D575:I575" si="94">D572/(D572+D574)</f>
-        <v>0.90217391304347827</v>
-      </c>
-      <c r="E575" s="28">
-        <f t="shared" si="94"/>
+      <c r="D575" s="29">
+        <f t="shared" ref="D575:I575" si="96">D572/(D572+D574)</f>
+        <v>0.91428571428571426</v>
+      </c>
+      <c r="E575" s="29">
+        <f t="shared" si="96"/>
         <v>0.99047619047619051</v>
       </c>
-      <c r="F575" s="28">
-        <f t="shared" si="94"/>
+      <c r="F575" s="29">
+        <f t="shared" si="96"/>
         <v>0.96969696969696972</v>
       </c>
-      <c r="G575" s="28">
-        <f t="shared" si="94"/>
+      <c r="G575" s="29">
+        <f t="shared" si="96"/>
         <v>0.58490566037735847</v>
       </c>
-      <c r="H575" s="28">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="I575" s="29">
-        <f t="shared" si="94"/>
-        <v>0.30434782608695654</v>
-      </c>
-    </row>
-    <row r="576" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B576" s="20" t="s">
+      <c r="H575" s="29">
+        <f t="shared" si="96"/>
+        <v>0.97826086956521741</v>
+      </c>
+      <c r="I575" s="30">
+        <f t="shared" si="96"/>
+        <v>0.85185185185185186</v>
+      </c>
+      <c r="J575" s="37"/>
+      <c r="K575" s="37">
+        <f>K572/(K572+K574)</f>
+        <v>0.56952539550374692</v>
+      </c>
+      <c r="L575" s="37">
+        <f t="shared" ref="L575" si="97">L572/(L572+L574)</f>
+        <v>0.97435897435897434</v>
+      </c>
+      <c r="M575" s="37">
+        <f t="shared" ref="M575" si="98">M572/(M572+M574)</f>
+        <v>0.54653465346534658</v>
+      </c>
+      <c r="N575" s="37">
+        <f t="shared" ref="N575" si="99">N572/(N572+N574)</f>
+        <v>1</v>
+      </c>
+      <c r="O575" s="37">
+        <f t="shared" ref="O575" si="100">O572/(O572+O574)</f>
+        <v>0.54653465346534658</v>
+      </c>
+      <c r="P575" s="37">
+        <f t="shared" ref="P575" si="101">P572/(P572+P574)</f>
+        <v>1</v>
+      </c>
+      <c r="Q575" s="37">
+        <f t="shared" ref="Q575" si="102">Q572/(Q572+Q574)</f>
+        <v>0.48222748815165878</v>
+      </c>
+      <c r="R575" s="37">
+        <f t="shared" ref="R575" si="103">R572/(R572+R574)</f>
+        <v>1</v>
+      </c>
+      <c r="S575" s="37">
+        <f>S572/(S572+S574)</f>
+        <v>0.93738489871086561</v>
+      </c>
+      <c r="T575" s="37">
+        <f t="shared" ref="T575" si="104">T572/(T572+T574)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="576" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B576" s="21" t="s">
         <v>479</v>
       </c>
-      <c r="C576" s="28">
+      <c r="C576" s="29">
         <f>C572/(C572+C573)</f>
         <v>0.85897435897435892</v>
       </c>
-      <c r="D576" s="28">
+      <c r="D576" s="29">
         <f>D572/(D572+D573)</f>
-        <v>0.87830687830687826</v>
-      </c>
-      <c r="E576" s="28">
+        <v>0.80334728033472802</v>
+      </c>
+      <c r="E576" s="29">
         <f>E572/(E572+E573)</f>
         <v>0.58591549295774648</v>
       </c>
-      <c r="F576" s="28">
+      <c r="F576" s="29">
         <f>F572/(F572+F573)</f>
         <v>0.56140350877192979</v>
       </c>
-      <c r="G576" s="28">
+      <c r="G576" s="29">
         <f>G572/(G572+G573)</f>
         <v>5.4673721340388004E-2</v>
       </c>
-      <c r="H576" s="28">
+      <c r="H576" s="29">
         <f>H572/(H572+H573)</f>
-        <v>0</v>
-      </c>
-      <c r="I576" s="30">
+        <v>0.23622047244094488</v>
+      </c>
+      <c r="I576" s="31">
         <f>I572/(I572+I573)</f>
-        <v>1.8181818181818181E-2</v>
-      </c>
-    </row>
-    <row r="577" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B577" s="21" t="s">
+        <v>0.17196261682242991</v>
+      </c>
+      <c r="J576" s="37"/>
+      <c r="K576" s="37">
+        <f t="shared" ref="J576:T576" si="105">K572/(K572+K573)</f>
+        <v>0.95530726256983245</v>
+      </c>
+      <c r="L576" s="37">
+        <f t="shared" si="105"/>
+        <v>0.10614525139664804</v>
+      </c>
+      <c r="M576" s="37">
+        <f t="shared" si="105"/>
+        <v>0.97354497354497349</v>
+      </c>
+      <c r="N576" s="37">
+        <f t="shared" si="105"/>
+        <v>0.62257495590828926</v>
+      </c>
+      <c r="O576" s="37">
+        <f t="shared" si="105"/>
+        <v>0.97354497354497349</v>
+      </c>
+      <c r="P576" s="37">
+        <f t="shared" si="105"/>
+        <v>0.7707231040564374</v>
+      </c>
+      <c r="Q576" s="37">
+        <f t="shared" si="105"/>
+        <v>0.86780383795309168</v>
+      </c>
+      <c r="R576" s="37">
+        <f t="shared" si="105"/>
+        <v>0.43283582089552236</v>
+      </c>
+      <c r="S576" s="37">
+        <f t="shared" si="105"/>
+        <v>0.89770723104056438</v>
+      </c>
+      <c r="T576" s="37">
+        <f t="shared" si="105"/>
+        <v>0.65608465608465605</v>
+      </c>
+    </row>
+    <row r="577" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B577" s="22" t="s">
         <v>491</v>
       </c>
-      <c r="C577" s="31">
+      <c r="C577" s="32">
         <f>(2*C572)/((2*C572)+C574+C573)</f>
         <v>0.61562021439509951</v>
       </c>
-      <c r="D577" s="31">
+      <c r="D577" s="32">
         <f>(2*D572)/((2*D572)+D574+D573)</f>
-        <v>0.89008042895442363</v>
-      </c>
-      <c r="E577" s="31">
-        <f t="shared" ref="D577:I577" si="95">(2*E572)/((2*E572)+E574+E573)</f>
+        <v>0.85523385300668153</v>
+      </c>
+      <c r="E577" s="32">
+        <f t="shared" ref="D577:I577" si="106">(2*E572)/((2*E572)+E574+E573)</f>
         <v>0.73628318584070795</v>
       </c>
-      <c r="F577" s="31">
-        <f t="shared" si="95"/>
+      <c r="F577" s="32">
+        <f t="shared" si="106"/>
         <v>0.71111111111111114</v>
       </c>
-      <c r="G577" s="31">
-        <f t="shared" si="95"/>
+      <c r="G577" s="32">
+        <f t="shared" si="106"/>
         <v>0.1</v>
       </c>
-      <c r="H577" s="31">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
-      <c r="I577" s="32">
-        <f t="shared" si="95"/>
-        <v>3.4313725490196081E-2</v>
-      </c>
-    </row>
-    <row r="578" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B578" s="16"/>
-      <c r="C578" s="16"/>
-      <c r="D578" s="16"/>
-      <c r="E578" s="16"/>
-      <c r="F578" s="16"/>
-      <c r="G578" s="16"/>
-      <c r="H578" s="16"/>
-      <c r="I578" s="16"/>
-    </row>
-    <row r="579" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B579" s="17" t="s">
+      <c r="H577" s="32">
+        <f t="shared" si="106"/>
+        <v>0.38054968287526425</v>
+      </c>
+      <c r="I577" s="33">
+        <f t="shared" si="106"/>
+        <v>0.28615863141524106</v>
+      </c>
+      <c r="J577" s="37"/>
+      <c r="K577" s="37">
+        <f t="shared" ref="J577:T577" si="107">(2*K572)/((2*K572)+K574+K573)</f>
+        <v>0.71361502347417838</v>
+      </c>
+      <c r="L577" s="37">
+        <f t="shared" si="107"/>
+        <v>0.19143576826196473</v>
+      </c>
+      <c r="M577" s="37">
+        <f t="shared" si="107"/>
+        <v>0.70006341154090046</v>
+      </c>
+      <c r="N577" s="37">
+        <f t="shared" si="107"/>
+        <v>0.7673913043478261</v>
+      </c>
+      <c r="O577" s="37">
+        <f t="shared" si="107"/>
+        <v>0.70006341154090046</v>
+      </c>
+      <c r="P577" s="37">
+        <f t="shared" si="107"/>
+        <v>0.87051792828685259</v>
+      </c>
+      <c r="Q577" s="37">
+        <f t="shared" si="107"/>
+        <v>0.61995430312262001</v>
+      </c>
+      <c r="R577" s="37">
+        <f t="shared" si="107"/>
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="S577" s="37">
+        <f t="shared" si="107"/>
+        <v>0.91711711711711708</v>
+      </c>
+      <c r="T577" s="37">
+        <f t="shared" si="107"/>
+        <v>0.792332268370607</v>
+      </c>
+    </row>
+    <row r="578" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B578" s="17"/>
+      <c r="C578" s="17"/>
+      <c r="D578" s="17"/>
+      <c r="E578" s="17"/>
+      <c r="F578" s="17"/>
+      <c r="G578" s="17"/>
+      <c r="H578" s="17"/>
+      <c r="I578" s="17"/>
+      <c r="K578" s="11"/>
+      <c r="L578" s="11"/>
+      <c r="M578" s="11"/>
+      <c r="N578" s="11"/>
+      <c r="O578" s="11"/>
+      <c r="P578" s="11"/>
+      <c r="Q578" s="11"/>
+      <c r="R578" s="11"/>
+      <c r="S578" s="11"/>
+      <c r="T578" s="11"/>
+    </row>
+    <row r="579" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B579" s="18" t="s">
         <v>487</v>
       </c>
       <c r="C579" s="1">
@@ -35823,50 +36043,50 @@
         <v>27</v>
       </c>
       <c r="H579" s="1"/>
-      <c r="I579" s="23"/>
-      <c r="K579">
-        <f>COUNTIF(K3:K569, "FN")</f>
-        <v>14</v>
-      </c>
-      <c r="L579">
-        <f t="shared" ref="L579:S579" si="96">COUNTIF(L3:L569, "FN")</f>
-        <v>543</v>
-      </c>
-      <c r="M579">
-        <f t="shared" si="96"/>
-        <v>15</v>
-      </c>
-      <c r="N579">
-        <f t="shared" si="96"/>
-        <v>214</v>
-      </c>
-      <c r="O579">
-        <f t="shared" si="96"/>
-        <v>15</v>
-      </c>
-      <c r="P579">
-        <f t="shared" si="96"/>
-        <v>130</v>
-      </c>
-      <c r="Q579">
-        <f t="shared" si="96"/>
-        <v>62</v>
-      </c>
-      <c r="R579">
-        <f t="shared" si="96"/>
-        <v>266</v>
-      </c>
-      <c r="S579">
-        <f t="shared" si="96"/>
-        <v>58</v>
-      </c>
-      <c r="T579">
-        <f>COUNTIF(T3:T569, "FN")</f>
-        <v>195</v>
-      </c>
-    </row>
-    <row r="580" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B580" s="18" t="s">
+      <c r="I579" s="24"/>
+      <c r="K579" s="14">
+        <f>COUNTIF(K3:K7, "TP") + COUNTIF(K14:K30, "TP") + COUNTIF(K73:K87, "TP") + COUNTIF(K122:K129, "TP") + COUNTIF(K142:K148, "TP") + COUNTIF(K162:K173, "TP") + COUNTIF(K203:K217, "TP") + COUNTIF(K252:K268, "TP") + COUNTIF(K306:K313, "TP") + COUNTIF(K327:K331, "TP") + COUNTIF(K338:K348, "TP") + COUNTIF(K375:K385, "TP") + COUNTIF(K404:K413, "TP") + COUNTIF(K443:K453, "TP") + COUNTIF(K478:K489, "TP") + COUNTIF(K518:K526, "TP") + COUNTIF(K545:K553, "TP")</f>
+        <v>179</v>
+      </c>
+      <c r="L579" s="14">
+        <f t="shared" ref="L579:T579" si="108">COUNTIF(L3:L7, "TP") + COUNTIF(L14:L30, "TP") + COUNTIF(L73:L87, "TP") + COUNTIF(L122:L129, "TP") + COUNTIF(L142:L148, "TP") + COUNTIF(L162:L173, "TP") + COUNTIF(L203:L217, "TP") + COUNTIF(L252:L268, "TP") + COUNTIF(L306:L313, "TP") + COUNTIF(L327:L331, "TP") + COUNTIF(L338:L348, "TP") + COUNTIF(L375:L385, "TP") + COUNTIF(L404:L413, "TP") + COUNTIF(L443:L453, "TP") + COUNTIF(L478:L489, "TP") + COUNTIF(L518:L526, "TP") + COUNTIF(L545:L553, "TP")</f>
+        <v>24</v>
+      </c>
+      <c r="M579" s="14">
+        <f t="shared" si="108"/>
+        <v>179</v>
+      </c>
+      <c r="N579" s="14">
+        <f t="shared" si="108"/>
+        <v>145</v>
+      </c>
+      <c r="O579" s="14">
+        <f t="shared" si="108"/>
+        <v>179</v>
+      </c>
+      <c r="P579" s="14">
+        <f t="shared" si="108"/>
+        <v>158</v>
+      </c>
+      <c r="Q579" s="14">
+        <f t="shared" si="108"/>
+        <v>125</v>
+      </c>
+      <c r="R579" s="14">
+        <f t="shared" si="108"/>
+        <v>82</v>
+      </c>
+      <c r="S579" s="14">
+        <f t="shared" si="108"/>
+        <v>178</v>
+      </c>
+      <c r="T579" s="14">
+        <f t="shared" si="108"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="580" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B580" s="19" t="s">
         <v>484</v>
       </c>
       <c r="C580" s="1">
@@ -35890,122 +36110,325 @@
         <v>155</v>
       </c>
       <c r="H580" s="1"/>
-      <c r="I580" s="24"/>
-    </row>
-    <row r="581" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B581" s="19" t="s">
+      <c r="I580" s="25"/>
+      <c r="K580" s="14">
+        <f>COUNTIF(K3:K7, "FN") + COUNTIF(K14:K30, "FN") + COUNTIF(K73:K87, "FN") + COUNTIF(K122:K129, "FN") + COUNTIF(K142:K148, "FN") + COUNTIF(K162:K173, "FN") + COUNTIF(K203:K217, "FN") + COUNTIF(K252:K268, "FN") + COUNTIF(K306:K313, "FN") + COUNTIF(K327:K331, "FN") + COUNTIF(K338:K348, "FN") + COUNTIF(K375:K385, "FN") + COUNTIF(K404:K413, "FN") + COUNTIF(K443:K453, "FN") + COUNTIF(K478:K489, "FN") + COUNTIF(K518:K526, "FN") + COUNTIF(K545:K553, "FN")</f>
+        <v>3</v>
+      </c>
+      <c r="L580" s="14">
+        <f t="shared" ref="L580:T580" si="109">COUNTIF(L3:L7, "FN") + COUNTIF(L14:L30, "FN") + COUNTIF(L73:L87, "FN") + COUNTIF(L122:L129, "FN") + COUNTIF(L142:L148, "FN") + COUNTIF(L162:L173, "FN") + COUNTIF(L203:L217, "FN") + COUNTIF(L252:L268, "FN") + COUNTIF(L306:L313, "FN") + COUNTIF(L327:L331, "FN") + COUNTIF(L338:L348, "FN") + COUNTIF(L375:L385, "FN") + COUNTIF(L404:L413, "FN") + COUNTIF(L443:L453, "FN") + COUNTIF(L478:L489, "FN") + COUNTIF(L518:L526, "FN") + COUNTIF(L545:L553, "FN")</f>
+        <v>158</v>
+      </c>
+      <c r="M580" s="14">
+        <f t="shared" si="109"/>
+        <v>3</v>
+      </c>
+      <c r="N580" s="14">
+        <f t="shared" si="109"/>
+        <v>37</v>
+      </c>
+      <c r="O580" s="14">
+        <f t="shared" si="109"/>
+        <v>3</v>
+      </c>
+      <c r="P580" s="14">
+        <f t="shared" si="109"/>
+        <v>24</v>
+      </c>
+      <c r="Q580" s="14">
+        <f t="shared" si="109"/>
+        <v>19</v>
+      </c>
+      <c r="R580" s="14">
+        <f t="shared" si="109"/>
+        <v>62</v>
+      </c>
+      <c r="S580" s="14">
+        <f t="shared" si="109"/>
+        <v>4</v>
+      </c>
+      <c r="T580" s="14">
+        <f t="shared" si="109"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="581" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B581" s="20" t="s">
         <v>481</v>
       </c>
-      <c r="C581" s="14">
+      <c r="C581" s="15">
         <v>41</v>
       </c>
-      <c r="D581" s="14">
+      <c r="D581" s="15">
         <v>5</v>
       </c>
-      <c r="E581" s="14">
+      <c r="E581" s="15">
         <v>0</v>
       </c>
-      <c r="F581" s="14">
+      <c r="F581" s="15">
         <v>1</v>
       </c>
-      <c r="G581" s="14">
+      <c r="G581" s="15">
         <v>21</v>
       </c>
-      <c r="H581" s="14"/>
-      <c r="I581" s="25"/>
-    </row>
-    <row r="582" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B582" s="18" t="s">
+      <c r="H581" s="15"/>
+      <c r="I581" s="26"/>
+      <c r="K581" s="11">
+        <v>68</v>
+      </c>
+      <c r="L581" s="11">
+        <v>0</v>
+      </c>
+      <c r="M581" s="11">
+        <v>46</v>
+      </c>
+      <c r="N581" s="11">
+        <v>0</v>
+      </c>
+      <c r="O581" s="7">
+        <v>46</v>
+      </c>
+      <c r="P581" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q581" s="7">
+        <v>41</v>
+      </c>
+      <c r="R581" s="11">
+        <v>0</v>
+      </c>
+      <c r="S581" s="7">
+        <v>5</v>
+      </c>
+      <c r="T581" s="11">
+        <v>0</v>
+      </c>
+      <c r="V581" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="582" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B582" s="19" t="s">
         <v>493</v>
       </c>
-      <c r="C582" s="28">
+      <c r="C582" s="29">
         <f>C579/(C579+C581)</f>
         <v>0.75</v>
       </c>
-      <c r="D582" s="28">
-        <f t="shared" ref="D582:G582" si="97">D579/(D579+D581)</f>
+      <c r="D582" s="29">
+        <f t="shared" ref="D582:G582" si="110">D579/(D579+D581)</f>
         <v>0.97267759562841527</v>
       </c>
-      <c r="E582" s="28">
-        <f t="shared" si="97"/>
+      <c r="E582" s="29">
+        <f t="shared" si="110"/>
         <v>1</v>
       </c>
-      <c r="F582" s="28">
-        <f t="shared" si="97"/>
+      <c r="F582" s="29">
+        <f t="shared" si="110"/>
         <v>0.96969696969696972</v>
       </c>
-      <c r="G582" s="28">
-        <f t="shared" si="97"/>
+      <c r="G582" s="29">
+        <f t="shared" si="110"/>
         <v>0.5625</v>
       </c>
-      <c r="H582" s="13"/>
-      <c r="I582" s="24"/>
-    </row>
-    <row r="583" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B583" s="18" t="s">
+      <c r="H582" s="14"/>
+      <c r="I582" s="25"/>
+      <c r="K582" s="37">
+        <f t="shared" ref="K582" si="111">K579/(K579+K581)</f>
+        <v>0.7246963562753036</v>
+      </c>
+      <c r="L582" s="37">
+        <f t="shared" ref="L582" si="112">L579/(L579+L581)</f>
+        <v>1</v>
+      </c>
+      <c r="M582" s="37">
+        <f t="shared" ref="M582" si="113">M579/(M579+M581)</f>
+        <v>0.79555555555555557</v>
+      </c>
+      <c r="N582" s="37">
+        <f t="shared" ref="N582" si="114">N579/(N579+N581)</f>
+        <v>1</v>
+      </c>
+      <c r="O582" s="37">
+        <f t="shared" ref="O582" si="115">O579/(O579+O581)</f>
+        <v>0.79555555555555557</v>
+      </c>
+      <c r="P582" s="37">
+        <f t="shared" ref="P582" si="116">P579/(P579+P581)</f>
+        <v>1</v>
+      </c>
+      <c r="Q582" s="37">
+        <f t="shared" ref="Q582" si="117">Q579/(Q579+Q581)</f>
+        <v>0.75301204819277112</v>
+      </c>
+      <c r="R582" s="37">
+        <f t="shared" ref="R582" si="118">R579/(R579+R581)</f>
+        <v>1</v>
+      </c>
+      <c r="S582" s="37">
+        <f t="shared" ref="S582" si="119">S579/(S579+S581)</f>
+        <v>0.97267759562841527</v>
+      </c>
+      <c r="T582" s="37">
+        <f t="shared" ref="T582" si="120">T579/(T579+T581)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="583" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B583" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="C583" s="28">
+      <c r="C583" s="29">
         <f>C579/(C579+C580)</f>
         <v>0.85416666666666663</v>
       </c>
-      <c r="D583" s="28">
-        <f t="shared" ref="D583:I583" si="98">D579/(D579+D580)</f>
+      <c r="D583" s="29">
+        <f t="shared" ref="D583:I583" si="121">D579/(D579+D580)</f>
         <v>0.97802197802197799</v>
       </c>
-      <c r="E583" s="28">
-        <f t="shared" si="98"/>
+      <c r="E583" s="29">
+        <f t="shared" si="121"/>
         <v>0.76363636363636367</v>
       </c>
-      <c r="F583" s="28">
-        <f t="shared" si="98"/>
+      <c r="F583" s="29">
+        <f t="shared" si="121"/>
         <v>0.56140350877192979</v>
       </c>
-      <c r="G583" s="28">
+      <c r="G583" s="29">
         <f>G579/(G579+G580)</f>
         <v>0.14835164835164835</v>
       </c>
       <c r="I583" s="5"/>
-    </row>
-    <row r="584" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B584" s="22" t="s">
+      <c r="K583" s="37">
+        <f>K579/(K579+K580)</f>
+        <v>0.98351648351648346</v>
+      </c>
+      <c r="L583" s="37">
+        <f>L579/(L579+L580)</f>
+        <v>0.13186813186813187</v>
+      </c>
+      <c r="M583" s="37">
+        <f t="shared" ref="L583:T583" si="122">M579/(M579+M580)</f>
+        <v>0.98351648351648346</v>
+      </c>
+      <c r="N583" s="37">
+        <f t="shared" si="122"/>
+        <v>0.79670329670329665</v>
+      </c>
+      <c r="O583" s="37">
+        <f t="shared" si="122"/>
+        <v>0.98351648351648346</v>
+      </c>
+      <c r="P583" s="37">
+        <f t="shared" si="122"/>
+        <v>0.86813186813186816</v>
+      </c>
+      <c r="Q583" s="37">
+        <f t="shared" si="122"/>
+        <v>0.86805555555555558</v>
+      </c>
+      <c r="R583" s="37">
+        <f t="shared" si="122"/>
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="S583" s="37">
+        <f t="shared" si="122"/>
+        <v>0.97802197802197799</v>
+      </c>
+      <c r="T583" s="37">
+        <f t="shared" si="122"/>
+        <v>0.84065934065934067</v>
+      </c>
+    </row>
+    <row r="584" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B584" s="23" t="s">
         <v>494</v>
       </c>
-      <c r="C584" s="31">
+      <c r="C584" s="32">
         <f>(2*C579)/((2*C579)+C581+C580)</f>
         <v>0.79870129870129869</v>
       </c>
-      <c r="D584" s="31">
-        <f t="shared" ref="D584:G584" si="99">(2*D579)/((2*D579)+D581+D580)</f>
+      <c r="D584" s="32">
+        <f t="shared" ref="D584:G584" si="123">(2*D579)/((2*D579)+D581+D580)</f>
         <v>0.97534246575342465</v>
       </c>
-      <c r="E584" s="31">
-        <f t="shared" si="99"/>
+      <c r="E584" s="32">
+        <f t="shared" si="123"/>
         <v>0.865979381443299</v>
       </c>
-      <c r="F584" s="31">
-        <f t="shared" si="99"/>
+      <c r="F584" s="32">
+        <f t="shared" si="123"/>
         <v>0.71111111111111114</v>
       </c>
-      <c r="G584" s="31">
-        <f t="shared" si="99"/>
+      <c r="G584" s="32">
+        <f t="shared" si="123"/>
         <v>0.23478260869565218</v>
       </c>
-      <c r="H584" s="15"/>
-      <c r="I584" s="26"/>
-    </row>
-    <row r="585" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B585" s="16"/>
-      <c r="C585" s="16"/>
-      <c r="D585" s="16"/>
-      <c r="E585" s="16"/>
-      <c r="F585" s="16"/>
-      <c r="G585" s="16"/>
-      <c r="H585" s="16"/>
-      <c r="I585" s="16"/>
-    </row>
-    <row r="586" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B586" s="17" t="s">
+      <c r="H584" s="16"/>
+      <c r="I584" s="27"/>
+      <c r="K584" s="37">
+        <f t="shared" ref="K584:T584" si="124">(2*K579)/((2*K579)+K581+K580)</f>
+        <v>0.83449883449883455</v>
+      </c>
+      <c r="L584" s="37">
+        <f t="shared" si="124"/>
+        <v>0.23300970873786409</v>
+      </c>
+      <c r="M584" s="37">
+        <f>(2*M579)/((2*M579)+M581+M580)</f>
+        <v>0.87960687960687955</v>
+      </c>
+      <c r="N584" s="37">
+        <f t="shared" si="124"/>
+        <v>0.88685015290519875</v>
+      </c>
+      <c r="O584" s="37">
+        <f t="shared" si="124"/>
+        <v>0.87960687960687955</v>
+      </c>
+      <c r="P584" s="37">
+        <f t="shared" si="124"/>
+        <v>0.92941176470588238</v>
+      </c>
+      <c r="Q584" s="37">
+        <f t="shared" si="124"/>
+        <v>0.80645161290322576</v>
+      </c>
+      <c r="R584" s="37">
+        <f t="shared" si="124"/>
+        <v>0.72566371681415931</v>
+      </c>
+      <c r="S584" s="37">
+        <f t="shared" si="124"/>
+        <v>0.97534246575342465</v>
+      </c>
+      <c r="T584" s="37">
+        <f t="shared" si="124"/>
+        <v>0.91343283582089552</v>
+      </c>
+    </row>
+    <row r="585" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B585" s="17"/>
+      <c r="C585" s="17"/>
+      <c r="D585" s="17"/>
+      <c r="E585" s="17"/>
+      <c r="F585" s="17"/>
+      <c r="G585" s="17"/>
+      <c r="H585" s="17"/>
+      <c r="I585" s="17"/>
+      <c r="K585" s="11"/>
+      <c r="L585" s="11"/>
+      <c r="M585" s="11"/>
+      <c r="N585" s="11"/>
+      <c r="O585" s="11"/>
+      <c r="P585" s="11"/>
+      <c r="Q585" s="11"/>
+      <c r="R585" s="11"/>
+      <c r="S585" s="11"/>
+      <c r="T585" s="11"/>
+    </row>
+    <row r="586" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B586" s="18" t="s">
         <v>488</v>
       </c>
       <c r="C586" s="1">
@@ -36026,13 +36449,53 @@
         <v>4</v>
       </c>
       <c r="H586" s="1"/>
-      <c r="I586" s="23">
+      <c r="I586" s="24">
         <f>COUNTIF(I554:I569, " TP") + COUNTIF(I527:I544, " TP") + COUNTIF(I490:I517, " TP") + COUNTIF(I454:I477, " TP") + COUNTIF(I414:I442, " TP") + COUNTIF(I386:I403, " TP") + COUNTIF(I349:I374, " TP") + COUNTIF(I332:I337, " TP") + COUNTIF(I314:I326, " TP") + COUNTIF(I269:I305, " TP") + COUNTIF(I218:I251, " TP") + COUNTIF(I174:I202, " TP") + COUNTIF(I149:I161, " TP") + COUNTIF(I130:I141, " TP") + COUNTIF(I88:I121, " TP") + COUNTIF(I31:I72, " TP") + COUNTIF(I8:I13, " TP")</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="587" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B587" s="18" t="s">
+      <c r="K586" s="1">
+        <f>COUNTIF(K554:K569, "TP") + COUNTIF(K527:K544, "TP") + COUNTIF(K490:K517, "TP") + COUNTIF(K454:K477, "TP") + COUNTIF(K414:K442, "TP") + COUNTIF(K386:K403, "TP") + COUNTIF(K349:K374, "TP") + COUNTIF(K332:K337, "TP") + COUNTIF(K314:K326, "TP") + COUNTIF(K269:K305, "TP") + COUNTIF(K218:K251, "TP") + COUNTIF(K174:K202, "TP") + COUNTIF(K149:K161, "TP") + COUNTIF(K130:K141, "TP") + COUNTIF(K88:K121, "TP") + COUNTIF(K31:K72, "TP") + COUNTIF(K8:K13, "TP")</f>
+        <v>374</v>
+      </c>
+      <c r="L586" s="1">
+        <f t="shared" ref="L586:T586" si="125">COUNTIF(L554:L569, "TP") + COUNTIF(L527:L544, "TP") + COUNTIF(L490:L517, "TP") + COUNTIF(L454:L477, "TP") + COUNTIF(L414:L442, "TP") + COUNTIF(L386:L403, "TP") + COUNTIF(L349:L374, "TP") + COUNTIF(L332:L337, "TP") + COUNTIF(L314:L326, "TP") + COUNTIF(L269:L305, "TP") + COUNTIF(L218:L251, "TP") + COUNTIF(L174:L202, "TP") + COUNTIF(L149:L161, "TP") + COUNTIF(L130:L141, "TP") + COUNTIF(L88:L121, "TP") + COUNTIF(L31:L72, "TP") + COUNTIF(L8:L13, "TP")</f>
+        <v>0</v>
+      </c>
+      <c r="M586" s="1">
+        <f t="shared" si="125"/>
+        <v>373</v>
+      </c>
+      <c r="N586" s="1">
+        <f t="shared" si="125"/>
+        <v>208</v>
+      </c>
+      <c r="O586" s="1">
+        <f t="shared" si="125"/>
+        <v>373</v>
+      </c>
+      <c r="P586" s="1">
+        <f t="shared" si="125"/>
+        <v>279</v>
+      </c>
+      <c r="Q586" s="1">
+        <f t="shared" si="125"/>
+        <v>282</v>
+      </c>
+      <c r="R586" s="1">
+        <f t="shared" si="125"/>
+        <v>121</v>
+      </c>
+      <c r="S586" s="1">
+        <f t="shared" si="125"/>
+        <v>331</v>
+      </c>
+      <c r="T586" s="1">
+        <f t="shared" si="125"/>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="587" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B587" s="19" t="s">
         <v>485</v>
       </c>
       <c r="C587" s="1">
@@ -36056,121 +36519,324 @@
         <f>COUNTIF(H554:H569, " FN") + COUNTIF(H527:H544, " FN") + COUNTIF(H490:H517, " FN") + COUNTIF(H454:H477, " FN") + COUNTIF(H414:H442, " FN") + COUNTIF(H386:H403, " FN") + COUNTIF(H349:H374, " FN") + COUNTIF(H332:H337, " FN") + COUNTIF(H314:H326, " FN") + COUNTIF(H269:H305, " FN") + COUNTIF(H218:H251, " FN") + COUNTIF(H174:H202, " FN") + COUNTIF(H149:H161, " FN") + COUNTIF(H130:H141, " FN") + COUNTIF(H88:H121, " FN") + COUNTIF(H31:H72, " FN") + COUNTIF(H8:H13, " FN")</f>
         <v>259</v>
       </c>
-      <c r="I587" s="24">
+      <c r="I587" s="25">
         <f>COUNTIF(I554:I569, " FN") + COUNTIF(I527:I544, " FN") + COUNTIF(I490:I517, " FN") + COUNTIF(I454:I477, " FN") + COUNTIF(I414:I442, " FN") + COUNTIF(I386:I403, " FN") + COUNTIF(I349:I374, " FN") + COUNTIF(I332:I337, " FN") + COUNTIF(I314:I326, " FN") + COUNTIF(I269:I305, " FN") + COUNTIF(I218:I251, " FN") + COUNTIF(I174:I202, " FN") + COUNTIF(I149:I161, " FN") + COUNTIF(I130:I141, " FN") + COUNTIF(I88:I121, " FN") + COUNTIF(I31:I72, " FN") + COUNTIF(I8:I13, " FN")</f>
         <v>378</v>
       </c>
-    </row>
-    <row r="588" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B588" s="19" t="s">
+      <c r="K587" s="1">
+        <f>COUNTIF(K554:K569, "FN") + COUNTIF(K527:K544, "FN") + COUNTIF(K490:K517, "FN") + COUNTIF(K454:K477, "FN") + COUNTIF(K414:K442, "FN") + COUNTIF(K386:K403, "FN") + COUNTIF(K349:K374, "FN") + COUNTIF(K332:K337, "FN") + COUNTIF(K314:K326, "FN") + COUNTIF(K269:K305, "FN") + COUNTIF(K218:K251, "FN") + COUNTIF(K174:K202, "FN") + COUNTIF(K149:K161, "FN") + COUNTIF(K130:K141, "FN") + COUNTIF(K88:K121, "FN") + COUNTIF(K31:K72, "FN") + COUNTIF(K8:K13, "FN")</f>
+        <v>11</v>
+      </c>
+      <c r="L587" s="1">
+        <f t="shared" ref="L587:T587" si="126">COUNTIF(L554:L569, "FN") + COUNTIF(L527:L544, "FN") + COUNTIF(L490:L517, "FN") + COUNTIF(L454:L477, "FN") + COUNTIF(L414:L442, "FN") + COUNTIF(L386:L403, "FN") + COUNTIF(L349:L374, "FN") + COUNTIF(L332:L337, "FN") + COUNTIF(L314:L326, "FN") + COUNTIF(L269:L305, "FN") + COUNTIF(L218:L251, "FN") + COUNTIF(L174:L202, "FN") + COUNTIF(L149:L161, "FN") + COUNTIF(L130:L141, "FN") + COUNTIF(L88:L121, "FN") + COUNTIF(L31:L72, "FN") + COUNTIF(L8:L13, "FN")</f>
+        <v>385</v>
+      </c>
+      <c r="M587" s="1">
+        <f t="shared" si="126"/>
+        <v>12</v>
+      </c>
+      <c r="N587" s="1">
+        <f t="shared" si="126"/>
+        <v>177</v>
+      </c>
+      <c r="O587" s="1">
+        <f t="shared" si="126"/>
+        <v>12</v>
+      </c>
+      <c r="P587" s="1">
+        <f t="shared" si="126"/>
+        <v>106</v>
+      </c>
+      <c r="Q587" s="1">
+        <f t="shared" si="126"/>
+        <v>43</v>
+      </c>
+      <c r="R587" s="1">
+        <f t="shared" si="126"/>
+        <v>204</v>
+      </c>
+      <c r="S587" s="1">
+        <f t="shared" si="126"/>
+        <v>54</v>
+      </c>
+      <c r="T587" s="1">
+        <f t="shared" si="126"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="588" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B588" s="20" t="s">
         <v>483</v>
       </c>
-      <c r="C588" s="14">
+      <c r="C588" s="15">
         <v>395</v>
       </c>
-      <c r="D588" s="14">
+      <c r="D588" s="15">
         <v>27</v>
       </c>
-      <c r="E588" s="14">
-        <v>2</v>
-      </c>
-      <c r="F588" s="14"/>
-      <c r="G588" s="14">
+      <c r="E588" s="15">
+        <v>2</v>
+      </c>
+      <c r="F588" s="15"/>
+      <c r="G588" s="15">
         <v>1</v>
       </c>
-      <c r="H588" s="14"/>
-      <c r="I588" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="589" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B589" s="20" t="s">
+      <c r="H588" s="15"/>
+      <c r="I588" s="26">
+        <v>2</v>
+      </c>
+      <c r="K588" s="11">
+        <v>415</v>
+      </c>
+      <c r="L588" s="11">
+        <v>0</v>
+      </c>
+      <c r="M588" s="7">
+        <v>412</v>
+      </c>
+      <c r="N588" s="11">
+        <v>0</v>
+      </c>
+      <c r="O588" s="7">
+        <v>412</v>
+      </c>
+      <c r="P588" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q588" s="7">
+        <v>396</v>
+      </c>
+      <c r="R588" s="11">
+        <v>0</v>
+      </c>
+      <c r="S588" s="7">
+        <v>29</v>
+      </c>
+      <c r="T588" s="11">
+        <v>0</v>
+      </c>
+      <c r="V588" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="589" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B589" s="21" t="s">
         <v>495</v>
       </c>
-      <c r="C589" s="28">
+      <c r="C589" s="29">
         <f>C586/(C586+C588)</f>
         <v>0.41394658753709201</v>
       </c>
-      <c r="D589" s="28">
-        <f t="shared" ref="D589:I589" si="100">D586/(D586+D588)</f>
+      <c r="D589" s="29">
+        <f t="shared" ref="D589:K589" si="127">D586/(D586+D588)</f>
         <v>0.9221902017291066</v>
       </c>
-      <c r="E589" s="28">
-        <f t="shared" si="100"/>
+      <c r="E589" s="29">
+        <f t="shared" si="127"/>
         <v>0.98412698412698407</v>
       </c>
-      <c r="F589" s="28">
+      <c r="F589" s="29">
         <v>0</v>
       </c>
-      <c r="G589" s="28">
-        <f t="shared" si="100"/>
+      <c r="G589" s="29">
+        <f t="shared" si="127"/>
         <v>0.8</v>
       </c>
-      <c r="I589" s="27"/>
-    </row>
-    <row r="590" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B590" s="20" t="s">
+      <c r="I589" s="28"/>
+      <c r="K589" s="37">
+        <f t="shared" si="127"/>
+        <v>0.47401774397972118</v>
+      </c>
+      <c r="L589" s="37" t="e">
+        <f t="shared" ref="L589" si="128">L586/(L586+L588)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M589" s="37">
+        <f t="shared" ref="M589" si="129">M586/(M586+M588)</f>
+        <v>0.47515923566878981</v>
+      </c>
+      <c r="N589" s="37">
+        <f t="shared" ref="N589" si="130">N586/(N586+N588)</f>
+        <v>1</v>
+      </c>
+      <c r="O589" s="37">
+        <f t="shared" ref="O589" si="131">O586/(O586+O588)</f>
+        <v>0.47515923566878981</v>
+      </c>
+      <c r="P589" s="37">
+        <f t="shared" ref="P589" si="132">P586/(P586+P588)</f>
+        <v>1</v>
+      </c>
+      <c r="Q589" s="37">
+        <f t="shared" ref="Q589" si="133">Q586/(Q586+Q588)</f>
+        <v>0.41592920353982299</v>
+      </c>
+      <c r="R589" s="37">
+        <f t="shared" ref="R589" si="134">R586/(R586+R588)</f>
+        <v>1</v>
+      </c>
+      <c r="S589" s="37">
+        <f t="shared" ref="S589" si="135">S586/(S586+S588)</f>
+        <v>0.9194444444444444</v>
+      </c>
+      <c r="T589" s="37">
+        <f t="shared" ref="T589" si="136">T586/(T586+T588)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="590" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B590" s="21" t="s">
         <v>496</v>
       </c>
-      <c r="C590" s="28">
+      <c r="C590" s="29">
         <f>C586/(C586+C587)</f>
         <v>0.86111111111111116</v>
       </c>
-      <c r="D590" s="28">
-        <f t="shared" ref="D590:I590" si="101">D586/(D586+D587)</f>
+      <c r="D590" s="29">
+        <f t="shared" ref="D590:K590" si="137">D586/(D586+D587)</f>
         <v>0.83116883116883122</v>
       </c>
-      <c r="E590" s="28">
-        <f t="shared" si="101"/>
+      <c r="E590" s="29">
+        <f t="shared" si="137"/>
         <v>0.5061224489795918</v>
       </c>
-      <c r="F590" s="28">
+      <c r="F590" s="29">
         <v>0</v>
       </c>
-      <c r="G590" s="28">
-        <f t="shared" si="101"/>
+      <c r="G590" s="29">
+        <f t="shared" si="137"/>
         <v>1.038961038961039E-2</v>
       </c>
       <c r="I590" s="5"/>
-    </row>
-    <row r="591" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B591" s="21" t="s">
+      <c r="K590" s="37">
+        <f t="shared" si="137"/>
+        <v>0.97142857142857142</v>
+      </c>
+      <c r="L590" s="37">
+        <f t="shared" ref="L590:T590" si="138">L586/(L586+L587)</f>
+        <v>0</v>
+      </c>
+      <c r="M590" s="37">
+        <f t="shared" si="138"/>
+        <v>0.96883116883116882</v>
+      </c>
+      <c r="N590" s="37">
+        <f t="shared" si="138"/>
+        <v>0.54025974025974022</v>
+      </c>
+      <c r="O590" s="37">
+        <f t="shared" si="138"/>
+        <v>0.96883116883116882</v>
+      </c>
+      <c r="P590" s="37">
+        <f t="shared" si="138"/>
+        <v>0.72467532467532469</v>
+      </c>
+      <c r="Q590" s="37">
+        <f t="shared" si="138"/>
+        <v>0.86769230769230765</v>
+      </c>
+      <c r="R590" s="37">
+        <f t="shared" si="138"/>
+        <v>0.37230769230769228</v>
+      </c>
+      <c r="S590" s="37">
+        <f t="shared" si="138"/>
+        <v>0.85974025974025969</v>
+      </c>
+      <c r="T590" s="37">
+        <f t="shared" si="138"/>
+        <v>0.5688311688311688</v>
+      </c>
+    </row>
+    <row r="591" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B591" s="22" t="s">
         <v>497</v>
       </c>
-      <c r="C591" s="31">
+      <c r="C591" s="32">
         <f>(2*C586)/((2*C586)+C588+C587)</f>
         <v>0.5591182364729459</v>
       </c>
-      <c r="D591" s="31">
-        <f t="shared" ref="D591:I591" si="102">(2*D586)/((2*D586)+D588+D587)</f>
+      <c r="D591" s="32">
+        <f t="shared" ref="D591:K591" si="139">(2*D586)/((2*D586)+D588+D587)</f>
         <v>0.87431693989071035</v>
       </c>
-      <c r="E591" s="31">
-        <f t="shared" si="102"/>
+      <c r="E591" s="32">
+        <f t="shared" si="139"/>
         <v>0.66846361185983827</v>
       </c>
-      <c r="F591" s="31">
+      <c r="F591" s="32">
         <v>0</v>
       </c>
-      <c r="G591" s="31">
-        <f t="shared" si="102"/>
+      <c r="G591" s="32">
+        <f t="shared" si="139"/>
         <v>2.0512820512820513E-2</v>
       </c>
       <c r="H591" s="3"/>
       <c r="I591" s="6"/>
-    </row>
-    <row r="592" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B592" s="16"/>
-      <c r="C592" s="16"/>
-      <c r="D592" s="16"/>
-      <c r="E592" s="16"/>
-      <c r="F592" s="16"/>
-      <c r="G592" s="16"/>
-      <c r="H592" s="16"/>
-      <c r="I592" s="16"/>
+      <c r="K591" s="37">
+        <f t="shared" si="139"/>
+        <v>0.63713798977853497</v>
+      </c>
+      <c r="L591" s="37">
+        <f t="shared" ref="L591:T591" si="140">(2*L586)/((2*L586)+L588+L587)</f>
+        <v>0</v>
+      </c>
+      <c r="M591" s="37">
+        <f t="shared" si="140"/>
+        <v>0.63760683760683756</v>
+      </c>
+      <c r="N591" s="37">
+        <f t="shared" si="140"/>
+        <v>0.70151770657672852</v>
+      </c>
+      <c r="O591" s="37">
+        <f t="shared" si="140"/>
+        <v>0.63760683760683756</v>
+      </c>
+      <c r="P591" s="37">
+        <f t="shared" si="140"/>
+        <v>0.84036144578313254</v>
+      </c>
+      <c r="Q591" s="37">
+        <f t="shared" si="140"/>
+        <v>0.56231306081754739</v>
+      </c>
+      <c r="R591" s="37">
+        <f t="shared" si="140"/>
+        <v>0.54260089686098656</v>
+      </c>
+      <c r="S591" s="37">
+        <f t="shared" si="140"/>
+        <v>0.88859060402684564</v>
+      </c>
+      <c r="T591" s="37">
+        <f t="shared" si="140"/>
+        <v>0.72516556291390732</v>
+      </c>
+    </row>
+    <row r="592" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B592" s="17"/>
+      <c r="C592" s="17"/>
+      <c r="D592" s="17"/>
+      <c r="E592" s="17"/>
+      <c r="F592" s="17"/>
+      <c r="G592" s="17"/>
+      <c r="H592" s="17"/>
+      <c r="I592" s="17"/>
+      <c r="K592" s="11"/>
+      <c r="L592" s="11"/>
+      <c r="M592" s="11"/>
+      <c r="N592" s="11"/>
+      <c r="O592" s="11"/>
+      <c r="P592" s="11"/>
+      <c r="Q592" s="11"/>
+      <c r="R592" s="11"/>
+      <c r="S592" s="11"/>
+      <c r="T592" s="11"/>
     </row>
     <row r="593" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B593" s="17" t="s">
+      <c r="B593" s="18" t="s">
         <v>489</v>
       </c>
       <c r="C593" s="1"/>
@@ -36183,12 +36849,26 @@
       <c r="H593" s="1">
         <v>90</v>
       </c>
-      <c r="I593" s="23">
-        <v>14</v>
-      </c>
+      <c r="I593" s="24">
+        <v>85</v>
+      </c>
+      <c r="K593" s="7">
+        <v>131</v>
+      </c>
+      <c r="L593" s="7">
+        <v>52</v>
+      </c>
+      <c r="M593" s="11"/>
+      <c r="N593" s="11"/>
+      <c r="O593" s="11"/>
+      <c r="P593" s="11"/>
+      <c r="Q593" s="11"/>
+      <c r="R593" s="11"/>
+      <c r="S593" s="11"/>
+      <c r="T593" s="11"/>
     </row>
     <row r="594" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B594" s="18" t="s">
+      <c r="B594" s="19" t="s">
         <v>486</v>
       </c>
       <c r="C594" s="1"/>
@@ -36201,152 +36881,186 @@
       <c r="H594" s="1">
         <v>32</v>
       </c>
-      <c r="I594" s="24">
-        <v>64</v>
-      </c>
+      <c r="I594" s="25">
+        <v>65</v>
+      </c>
+      <c r="K594" s="7">
+        <v>18</v>
+      </c>
+      <c r="L594" s="7">
+        <v>97</v>
+      </c>
+      <c r="M594" s="11"/>
+      <c r="N594" s="11"/>
+      <c r="O594" s="11"/>
+      <c r="P594" s="11"/>
+      <c r="Q594" s="11"/>
+      <c r="R594" s="11"/>
+      <c r="S594" s="11"/>
+      <c r="T594" s="11"/>
     </row>
     <row r="595" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B595" s="19" t="s">
+      <c r="B595" s="20" t="s">
         <v>482</v>
       </c>
-      <c r="C595" s="14"/>
-      <c r="D595" s="14">
+      <c r="C595" s="15"/>
+      <c r="D595" s="15">
         <v>22</v>
       </c>
-      <c r="E595" s="14"/>
-      <c r="F595" s="14"/>
-      <c r="G595" s="14"/>
-      <c r="H595" s="14">
-        <v>2</v>
-      </c>
-      <c r="I595" s="25">
+      <c r="E595" s="15"/>
+      <c r="F595" s="15"/>
+      <c r="G595" s="15"/>
+      <c r="H595" s="15">
+        <v>2</v>
+      </c>
+      <c r="I595" s="26">
         <v>14</v>
       </c>
+      <c r="K595" s="11">
+        <v>34</v>
+      </c>
+      <c r="L595" s="7">
+        <v>2</v>
+      </c>
+      <c r="M595" s="7"/>
+      <c r="N595" s="7"/>
+      <c r="O595" s="11"/>
+      <c r="P595" s="7"/>
+      <c r="Q595" s="11"/>
+      <c r="R595" s="11"/>
+      <c r="S595" s="11"/>
+      <c r="T595" s="11"/>
     </row>
     <row r="596" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B596" s="18" t="s">
+      <c r="B596" s="19" t="s">
         <v>498</v>
       </c>
-      <c r="C596" s="13"/>
-      <c r="D596" s="28">
+      <c r="C596" s="14"/>
+      <c r="D596" s="29">
         <f>D593/(D593+D595)</f>
         <v>0.78</v>
       </c>
-      <c r="E596" s="28"/>
-      <c r="F596" s="28"/>
-      <c r="G596" s="28"/>
-      <c r="H596" s="28">
-        <f t="shared" ref="E596:I596" si="103">H593/(H593+H595)</f>
+      <c r="E596" s="29"/>
+      <c r="F596" s="29"/>
+      <c r="G596" s="29"/>
+      <c r="H596" s="29">
+        <f t="shared" ref="E596:K596" si="141">H593/(H593+H595)</f>
         <v>0.97826086956521741</v>
       </c>
-      <c r="I596" s="29">
-        <f t="shared" si="103"/>
-        <v>0.5</v>
-      </c>
+      <c r="I596" s="30">
+        <f t="shared" si="141"/>
+        <v>0.85858585858585856</v>
+      </c>
+      <c r="K596" s="37">
+        <f t="shared" si="141"/>
+        <v>0.79393939393939394</v>
+      </c>
+      <c r="L596" s="37">
+        <f t="shared" ref="L596" si="142">L593/(L593+L595)</f>
+        <v>0.96296296296296291</v>
+      </c>
+      <c r="M596" s="37"/>
+      <c r="N596" s="37"/>
+      <c r="O596" s="37"/>
+      <c r="P596" s="37"/>
+      <c r="Q596" s="37"/>
+      <c r="R596" s="37"/>
+      <c r="S596" s="37"/>
+      <c r="T596" s="37"/>
     </row>
     <row r="597" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B597" s="18" t="s">
+      <c r="B597" s="19" t="s">
         <v>499</v>
       </c>
-      <c r="C597" s="13"/>
-      <c r="D597" s="28">
+      <c r="C597" s="14"/>
+      <c r="D597" s="29">
         <f>D593/(D593+D594)</f>
         <v>0.52</v>
       </c>
-      <c r="E597" s="28"/>
-      <c r="F597" s="28"/>
-      <c r="G597" s="28"/>
-      <c r="H597" s="28">
-        <f t="shared" ref="E597:I597" si="104">H593/(H593+H594)</f>
+      <c r="E597" s="29"/>
+      <c r="F597" s="29"/>
+      <c r="G597" s="29"/>
+      <c r="H597" s="29">
+        <f t="shared" ref="E597:K597" si="143">H593/(H593+H594)</f>
         <v>0.73770491803278693</v>
       </c>
-      <c r="I597" s="30">
-        <f t="shared" si="104"/>
-        <v>0.17948717948717949</v>
-      </c>
+      <c r="I597" s="31">
+        <f t="shared" si="143"/>
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="K597" s="37">
+        <f t="shared" si="143"/>
+        <v>0.87919463087248317</v>
+      </c>
+      <c r="L597" s="37">
+        <f t="shared" ref="L597:T597" si="144">L593/(L593+L594)</f>
+        <v>0.34899328859060402</v>
+      </c>
+      <c r="M597" s="37"/>
+      <c r="N597" s="37"/>
+      <c r="O597" s="37"/>
+      <c r="P597" s="37"/>
+      <c r="Q597" s="37"/>
+      <c r="R597" s="37"/>
+      <c r="S597" s="37"/>
+      <c r="T597" s="37"/>
     </row>
     <row r="598" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B598" s="22" t="s">
+      <c r="B598" s="23" t="s">
         <v>500</v>
       </c>
-      <c r="C598" s="15"/>
-      <c r="D598" s="31">
+      <c r="C598" s="16"/>
+      <c r="D598" s="32">
         <f>(2*D593)/((2*D593)+D595+D594)</f>
         <v>0.624</v>
       </c>
-      <c r="E598" s="31"/>
-      <c r="F598" s="31"/>
-      <c r="G598" s="31"/>
-      <c r="H598" s="31">
-        <f t="shared" ref="E598:I598" si="105">(2*H593)/((2*H593)+H595+H594)</f>
+      <c r="E598" s="32"/>
+      <c r="F598" s="32"/>
+      <c r="G598" s="32"/>
+      <c r="H598" s="32">
+        <f t="shared" ref="E598:K598" si="145">(2*H593)/((2*H593)+H595+H594)</f>
         <v>0.84112149532710279</v>
       </c>
-      <c r="I598" s="32">
-        <f t="shared" si="105"/>
-        <v>0.26415094339622641</v>
-      </c>
+      <c r="I598" s="33">
+        <f t="shared" si="145"/>
+        <v>0.68273092369477917</v>
+      </c>
+      <c r="K598" s="37">
+        <f t="shared" si="145"/>
+        <v>0.83439490445859876</v>
+      </c>
+      <c r="L598" s="37">
+        <f t="shared" ref="L598:T598" si="146">(2*L593)/((2*L593)+L595+L594)</f>
+        <v>0.51231527093596063</v>
+      </c>
+      <c r="M598" s="37"/>
+      <c r="N598" s="37"/>
+      <c r="O598" s="37"/>
+      <c r="P598" s="37"/>
+      <c r="Q598" s="37"/>
+      <c r="R598" s="37"/>
+      <c r="S598" s="37"/>
+      <c r="T598" s="37"/>
     </row>
     <row r="599" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B599" s="10"/>
-      <c r="C599" s="10"/>
-      <c r="D599" s="10"/>
-      <c r="E599" s="10"/>
-      <c r="F599" s="10"/>
-      <c r="G599" s="10"/>
-      <c r="H599" s="10"/>
-      <c r="I599" s="10"/>
+      <c r="B599" s="11"/>
+      <c r="C599" s="11"/>
+      <c r="D599" s="11"/>
+      <c r="E599" s="11"/>
+      <c r="F599" s="11"/>
+      <c r="G599" s="11"/>
+      <c r="H599" s="11"/>
+      <c r="I599" s="11"/>
     </row>
     <row r="600" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B600" s="10"/>
-      <c r="C600" s="10"/>
-      <c r="D600" s="10"/>
-      <c r="E600" s="10"/>
-      <c r="F600" s="10"/>
-      <c r="G600" s="10"/>
-      <c r="H600" s="10"/>
-      <c r="I600" s="10"/>
-    </row>
-    <row r="602" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="K602">
-        <f>K572/(K572+K579)</f>
-        <v>0.97530864197530864</v>
-      </c>
-      <c r="L602">
-        <f t="shared" ref="L602:T602" si="106">L572/(L572+L579)</f>
-        <v>4.2328042328042326E-2</v>
-      </c>
-      <c r="M602">
-        <f t="shared" si="106"/>
-        <v>0.97354497354497349</v>
-      </c>
-      <c r="N602">
-        <f t="shared" si="106"/>
-        <v>0.62257495590828926</v>
-      </c>
-      <c r="O602">
-        <f t="shared" si="106"/>
-        <v>0.97354497354497349</v>
-      </c>
-      <c r="P602">
-        <f t="shared" si="106"/>
-        <v>0.7707231040564374</v>
-      </c>
-      <c r="Q602">
-        <f t="shared" si="106"/>
-        <v>0.86780383795309168</v>
-      </c>
-      <c r="R602">
-        <f t="shared" si="106"/>
-        <v>0.43283582089552236</v>
-      </c>
-      <c r="S602">
-        <f t="shared" si="106"/>
-        <v>0.89770723104056438</v>
-      </c>
-      <c r="T602">
-        <f t="shared" si="106"/>
-        <v>0.65608465608465605</v>
-      </c>
+      <c r="B600" s="11"/>
+      <c r="C600" s="11"/>
+      <c r="D600" s="11"/>
+      <c r="E600" s="11"/>
+      <c r="F600" s="11"/>
+      <c r="G600" s="11"/>
+      <c r="H600" s="11"/>
+      <c r="I600" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
data: endpoint metric calculation for tool combinations
</commit_message>
<xml_diff>
--- a/merged_results/complete_results.xlsx
+++ b/merged_results/complete_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/Documents/Own/Papers_and_Projects/comparison_ArchRec_tools/GitHub_SARbenchmarks/merged_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0EEA3F-7E49-4C46-9D66-151C8E236125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C205A821-5FE2-094D-BC68-5835C8899DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" xr2:uid="{21E6DDBE-06EB-864D-8BE4-57F9A90E46C0}"/>
   </bookViews>
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3292" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3304" uniqueCount="512">
   <si>
     <t xml:space="preserve"> RAD</t>
   </si>
@@ -1805,7 +1805,19 @@
     <t>RAS</t>
   </si>
   <si>
-    <t>This is done manually (checking each FP for overlaps)</t>
+    <t>RAD</t>
+  </si>
+  <si>
+    <t>All three</t>
+  </si>
+  <si>
+    <t>C2D + RAD</t>
+  </si>
+  <si>
+    <t>C2D + RAS</t>
+  </si>
+  <si>
+    <t>RAD + RAS</t>
   </si>
 </sst>
 </file>
@@ -1843,7 +1855,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1984,11 +1996,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2000,9 +2021,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -2037,6 +2062,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2437,11 +2486,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E181CEDB-9761-A944-9A62-062C9F034F3F}">
-  <dimension ref="A1:Y600"/>
+  <dimension ref="A1:Y603"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A573" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M597" sqref="M597"/>
+      <pane ySplit="2" topLeftCell="A580" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J601" sqref="J601"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2455,26 +2504,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="9" t="s">
         <v>469</v>
       </c>
-      <c r="L1" s="8"/>
+      <c r="L1" s="9"/>
       <c r="M1" s="2" t="s">
         <v>474</v>
       </c>
       <c r="N1" s="2"/>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="9" t="s">
         <v>472</v>
       </c>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8" t="s">
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9" t="s">
         <v>473</v>
       </c>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8" t="s">
+      <c r="R1" s="9"/>
+      <c r="S1" s="9" t="s">
         <v>475</v>
       </c>
-      <c r="T1" s="8"/>
+      <c r="T1" s="9"/>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
@@ -2484,55 +2533,55 @@
       <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="36" t="s">
         <v>501</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="36" t="s">
         <v>502</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="36" t="s">
         <v>503</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="36" t="s">
         <v>504</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="37" t="s">
         <v>505</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="38" t="s">
         <v>506</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="S2" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="T2" s="10" t="s">
         <v>471</v>
       </c>
     </row>
@@ -2716,20 +2765,20 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="15"/>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
         <v>TP</v>
@@ -3945,22 +3994,22 @@
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H30" s="12"/>
-      <c r="I30" s="13"/>
+      <c r="C30" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="14"/>
+      <c r="I30" s="15"/>
       <c r="K30" t="str">
         <f t="shared" si="0"/>
         <v>TP</v>
@@ -4012,7 +4061,7 @@
       <c r="D31" t="s">
         <v>2</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="13" t="s">
         <v>4</v>
       </c>
       <c r="I31" s="5" t="s">
@@ -4069,7 +4118,7 @@
       <c r="D32" t="s">
         <v>2</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="13" t="s">
         <v>4</v>
       </c>
       <c r="I32" s="5" t="s">
@@ -7216,24 +7265,24 @@
       </c>
     </row>
     <row r="87" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B87" s="12" t="s">
+      <c r="B87" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C87" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D87" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E87" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F87" s="12"/>
-      <c r="G87" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H87" s="12"/>
-      <c r="I87" s="13"/>
+      <c r="C87" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E87" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H87" s="14"/>
+      <c r="I87" s="15"/>
       <c r="K87" t="str">
         <f t="shared" si="12"/>
         <v>TP</v>
@@ -7288,7 +7337,7 @@
       <c r="E88" t="s">
         <v>4</v>
       </c>
-      <c r="G88" s="11" t="s">
+      <c r="G88" s="13" t="s">
         <v>4</v>
       </c>
       <c r="H88" t="s">
@@ -7351,7 +7400,7 @@
       <c r="E89" t="s">
         <v>2</v>
       </c>
-      <c r="G89" s="11" t="s">
+      <c r="G89" s="13" t="s">
         <v>4</v>
       </c>
       <c r="H89" t="s">
@@ -9829,24 +9878,24 @@
       </c>
     </row>
     <row r="129" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B129" s="12" t="s">
+      <c r="B129" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="C129" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D129" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E129" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F129" s="12"/>
-      <c r="G129" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H129" s="12"/>
-      <c r="I129" s="13"/>
+      <c r="C129" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D129" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E129" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F129" s="14"/>
+      <c r="G129" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H129" s="14"/>
+      <c r="I129" s="15"/>
       <c r="K129" t="str">
         <f t="shared" si="12"/>
         <v>TP</v>
@@ -9901,7 +9950,7 @@
       <c r="E130" t="s">
         <v>2</v>
       </c>
-      <c r="G130" s="11" t="s">
+      <c r="G130" s="13" t="s">
         <v>4</v>
       </c>
       <c r="H130" t="s">
@@ -9964,7 +10013,7 @@
       <c r="E131" t="s">
         <v>2</v>
       </c>
-      <c r="G131" s="11" t="s">
+      <c r="G131" s="13" t="s">
         <v>4</v>
       </c>
       <c r="H131" t="s">
@@ -11016,26 +11065,26 @@
       </c>
     </row>
     <row r="148" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B148" s="12" t="s">
+      <c r="B148" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C148" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D148" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E148" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F148" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="G148" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H148" s="12"/>
-      <c r="I148" s="13"/>
+      <c r="C148" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D148" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E148" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F148" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G148" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H148" s="14"/>
+      <c r="I148" s="15"/>
       <c r="K148" t="str">
         <f t="shared" si="22"/>
         <v>TP</v>
@@ -11090,7 +11139,7 @@
       <c r="E149" t="s">
         <v>2</v>
       </c>
-      <c r="G149" s="11" t="s">
+      <c r="G149" s="13" t="s">
         <v>4</v>
       </c>
       <c r="H149" t="s">
@@ -11153,7 +11202,7 @@
       <c r="E150" t="s">
         <v>4</v>
       </c>
-      <c r="G150" s="11" t="s">
+      <c r="G150" s="13" t="s">
         <v>4</v>
       </c>
       <c r="H150" t="s">
@@ -11216,7 +11265,7 @@
       <c r="E151" t="s">
         <v>4</v>
       </c>
-      <c r="G151" s="11" t="s">
+      <c r="G151" s="13" t="s">
         <v>4</v>
       </c>
       <c r="H151" t="s">
@@ -11279,7 +11328,7 @@
       <c r="E152" t="s">
         <v>2</v>
       </c>
-      <c r="G152" s="11" t="s">
+      <c r="G152" s="13" t="s">
         <v>4</v>
       </c>
       <c r="H152" t="s">
@@ -12573,26 +12622,26 @@
       </c>
     </row>
     <row r="173" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B173" s="12" t="s">
+      <c r="B173" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C173" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D173" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E173" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F173" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G173" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H173" s="12"/>
-      <c r="I173" s="13"/>
+      <c r="C173" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D173" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E173" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F173" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G173" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H173" s="14"/>
+      <c r="I173" s="15"/>
       <c r="K173" t="str">
         <f t="shared" si="22"/>
         <v>TP</v>
@@ -15193,24 +15242,24 @@
       </c>
     </row>
     <row r="217" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B217" s="12" t="s">
+      <c r="B217" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="C217" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D217" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E217" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F217" s="12"/>
-      <c r="G217" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H217" s="12"/>
-      <c r="I217" s="13"/>
+      <c r="C217" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D217" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E217" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F217" s="14"/>
+      <c r="G217" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H217" s="14"/>
+      <c r="I217" s="15"/>
       <c r="K217" t="str">
         <f t="shared" si="32"/>
         <v>TP</v>
@@ -18328,24 +18377,24 @@
       </c>
     </row>
     <row r="268" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B268" s="12" t="s">
+      <c r="B268" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C268" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D268" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E268" s="12"/>
-      <c r="F268" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G268" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H268" s="12"/>
-      <c r="I268" s="13"/>
+      <c r="C268" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D268" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E268" s="14"/>
+      <c r="F268" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G268" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H268" s="14"/>
+      <c r="I268" s="15"/>
       <c r="K268" t="str">
         <f t="shared" si="42"/>
         <v>TP</v>
@@ -20922,20 +20971,20 @@
       </c>
     </row>
     <row r="313" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B313" s="12" t="s">
+      <c r="B313" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="C313" s="12"/>
-      <c r="D313" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E313" s="12"/>
-      <c r="F313" s="12"/>
-      <c r="G313" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H313" s="12"/>
-      <c r="I313" s="13"/>
+      <c r="C313" s="14"/>
+      <c r="D313" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E313" s="14"/>
+      <c r="F313" s="14"/>
+      <c r="G313" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H313" s="14"/>
+      <c r="I313" s="15"/>
       <c r="K313" t="str">
         <f t="shared" si="42"/>
         <v>TP</v>
@@ -21790,20 +21839,20 @@
       </c>
     </row>
     <row r="331" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B331" s="12" t="s">
+      <c r="B331" s="14" t="s">
         <v>310</v>
       </c>
-      <c r="C331" s="12"/>
-      <c r="D331" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E331" s="12"/>
-      <c r="F331" s="12"/>
-      <c r="G331" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H331" s="12"/>
-      <c r="I331" s="13"/>
+      <c r="C331" s="14"/>
+      <c r="D331" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E331" s="14"/>
+      <c r="F331" s="14"/>
+      <c r="G331" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H331" s="14"/>
+      <c r="I331" s="15"/>
       <c r="K331" t="str">
         <f t="shared" si="52"/>
         <v>TP</v>
@@ -22719,24 +22768,24 @@
       </c>
     </row>
     <row r="348" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B348" s="12" t="s">
+      <c r="B348" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C348" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D348" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E348" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F348" s="12"/>
-      <c r="G348" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H348" s="12"/>
-      <c r="I348" s="13"/>
+      <c r="C348" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D348" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E348" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F348" s="14"/>
+      <c r="G348" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H348" s="14"/>
+      <c r="I348" s="15"/>
       <c r="K348" t="str">
         <f t="shared" si="52"/>
         <v>TP</v>
@@ -24785,20 +24834,20 @@
       </c>
     </row>
     <row r="385" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B385" s="12" t="s">
+      <c r="B385" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C385" s="12"/>
-      <c r="D385" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E385" s="12"/>
-      <c r="F385" s="12"/>
-      <c r="G385" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H385" s="12"/>
-      <c r="I385" s="13"/>
+      <c r="C385" s="14"/>
+      <c r="D385" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E385" s="14"/>
+      <c r="F385" s="14"/>
+      <c r="G385" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H385" s="14"/>
+      <c r="I385" s="15"/>
       <c r="K385" t="str">
         <f t="shared" si="52"/>
         <v>TP</v>
@@ -26244,24 +26293,24 @@
       </c>
     </row>
     <row r="413" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B413" s="12" t="s">
+      <c r="B413" s="14" t="s">
         <v>352</v>
       </c>
-      <c r="C413" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D413" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E413" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F413" s="12"/>
-      <c r="G413" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H413" s="12"/>
-      <c r="I413" s="13"/>
+      <c r="C413" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D413" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E413" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F413" s="14"/>
+      <c r="G413" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H413" s="14"/>
+      <c r="I413" s="15"/>
       <c r="K413" t="str">
         <f t="shared" si="62"/>
         <v>TP</v>
@@ -28630,24 +28679,24 @@
       </c>
     </row>
     <row r="453" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B453" s="12" t="s">
+      <c r="B453" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C453" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D453" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E453" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F453" s="12"/>
-      <c r="G453" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H453" s="12"/>
-      <c r="I453" s="13"/>
+      <c r="C453" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D453" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E453" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F453" s="14"/>
+      <c r="G453" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H453" s="14"/>
+      <c r="I453" s="15"/>
       <c r="K453" t="str">
         <f t="shared" si="72"/>
         <v>TP</v>
@@ -30878,26 +30927,26 @@
       </c>
     </row>
     <row r="489" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B489" s="12" t="s">
+      <c r="B489" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C489" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D489" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E489" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F489" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G489" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H489" s="12"/>
-      <c r="I489" s="13"/>
+      <c r="C489" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D489" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E489" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F489" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G489" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H489" s="14"/>
+      <c r="I489" s="15"/>
       <c r="K489" t="str">
         <f t="shared" si="72"/>
         <v>TP</v>
@@ -33085,22 +33134,22 @@
       </c>
     </row>
     <row r="526" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B526" s="12" t="s">
+      <c r="B526" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C526" s="12"/>
-      <c r="D526" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E526" s="12"/>
-      <c r="F526" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G526" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H526" s="12"/>
-      <c r="I526" s="13"/>
+      <c r="C526" s="14"/>
+      <c r="D526" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E526" s="14"/>
+      <c r="F526" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G526" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H526" s="14"/>
+      <c r="I526" s="15"/>
       <c r="K526" t="str">
         <f t="shared" si="82"/>
         <v>TP</v>
@@ -34496,24 +34545,24 @@
       </c>
     </row>
     <row r="553" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B553" s="12" t="s">
+      <c r="B553" s="14" t="s">
         <v>452</v>
       </c>
-      <c r="C553" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D553" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E553" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F553" s="12"/>
-      <c r="G553" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H553" s="12"/>
-      <c r="I553" s="13"/>
+      <c r="C553" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D553" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E553" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F553" s="14"/>
+      <c r="G553" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H553" s="14"/>
+      <c r="I553" s="15"/>
       <c r="K553" t="str">
         <f t="shared" si="82"/>
         <v>TP</v>
@@ -34996,7 +35045,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="561" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B561" t="s">
         <v>459</v>
       </c>
@@ -35059,7 +35108,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="562" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B562" t="s">
         <v>460</v>
       </c>
@@ -35122,7 +35171,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="563" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B563" t="s">
         <v>461</v>
       </c>
@@ -35185,7 +35234,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="564" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B564" t="s">
         <v>462</v>
       </c>
@@ -35248,7 +35297,7 @@
         <v>TP</v>
       </c>
     </row>
-    <row r="565" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B565" t="s">
         <v>463</v>
       </c>
@@ -35311,7 +35360,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="566" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="566" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B566" t="s">
         <v>464</v>
       </c>
@@ -35374,7 +35423,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="567" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="567" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B567" t="s">
         <v>465</v>
       </c>
@@ -35437,7 +35486,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="568" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="568" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B568" t="s">
         <v>466</v>
       </c>
@@ -35500,7 +35549,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="569" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A569" s="4"/>
       <c r="B569" s="3" t="s">
         <v>467</v>
@@ -35565,44 +35614,44 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="572" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B572" s="18" t="s">
+    <row r="572" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B572" s="20" t="s">
         <v>476</v>
       </c>
-      <c r="C572" s="10">
-        <f>COUNTIF(C3:C569, " TP") + C593</f>
+      <c r="C572" s="12">
+        <f>COUNTIF(C3:C569, " TP") + C596</f>
         <v>402</v>
       </c>
-      <c r="D572" s="10">
-        <f t="shared" ref="D572:I572" si="92">COUNTIF(D3:D569, " TP") + D593</f>
-        <v>576</v>
-      </c>
-      <c r="E572" s="10">
+      <c r="D572" s="12">
+        <f t="shared" ref="D572:I572" si="92">COUNTIF(D3:D569, " TP") + D596</f>
+        <v>575</v>
+      </c>
+      <c r="E572" s="12">
         <f t="shared" si="92"/>
         <v>208</v>
       </c>
-      <c r="F572" s="10">
+      <c r="F572" s="12">
         <f t="shared" si="92"/>
         <v>32</v>
       </c>
-      <c r="G572" s="10">
+      <c r="G572" s="12">
         <f t="shared" si="92"/>
         <v>31</v>
       </c>
-      <c r="H572" s="10">
+      <c r="H572" s="12">
         <f t="shared" si="92"/>
         <v>90</v>
       </c>
-      <c r="I572" s="24">
+      <c r="I572" s="26">
         <f t="shared" si="92"/>
-        <v>92</v>
-      </c>
-      <c r="K572" s="11">
-        <f>COUNTIF(K3:K569, "TP") + K593</f>
+        <v>93</v>
+      </c>
+      <c r="K572" s="47">
+        <f>COUNTIF(K3:K569, "TP") + K596</f>
         <v>684</v>
       </c>
       <c r="L572" s="11">
-        <f>COUNTIF(L3:L569, "TP") + L593</f>
+        <f>COUNTIF(L3:L569, "TP") + L596</f>
         <v>76</v>
       </c>
       <c r="M572" s="11">
@@ -35633,393 +35682,390 @@
         <f t="shared" si="93"/>
         <v>509</v>
       </c>
-      <c r="T572" s="11">
+      <c r="T572" s="48">
         <f>COUNTIF(T3:T569, "TP")</f>
         <v>372</v>
       </c>
     </row>
-    <row r="573" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B573" s="19" t="s">
+    <row r="573" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B573" s="21" t="s">
         <v>477</v>
       </c>
-      <c r="C573" s="14">
-        <f>COUNTIF(C3:C569, " FN") + C594</f>
+      <c r="C573" s="16">
+        <f>COUNTIF(C3:C569, " FN") + C597</f>
         <v>66</v>
       </c>
-      <c r="D573" s="14">
-        <f t="shared" ref="D573:I573" si="94">COUNTIF(D3:D569, " FN") + D594</f>
+      <c r="D573" s="16">
+        <f t="shared" ref="D573:I573" si="94">COUNTIF(D3:D569, " FN") + D597</f>
         <v>141</v>
       </c>
-      <c r="E573" s="14">
+      <c r="E573" s="16">
         <f t="shared" si="94"/>
         <v>147</v>
       </c>
-      <c r="F573" s="14">
+      <c r="F573" s="16">
         <f t="shared" si="94"/>
         <v>25</v>
       </c>
-      <c r="G573" s="14">
+      <c r="G573" s="16">
         <f t="shared" si="94"/>
         <v>536</v>
       </c>
-      <c r="H573" s="14">
+      <c r="H573" s="16">
         <f t="shared" si="94"/>
-        <v>291</v>
-      </c>
-      <c r="I573" s="25">
+        <v>290</v>
+      </c>
+      <c r="I573" s="27">
         <f t="shared" si="94"/>
-        <v>443</v>
-      </c>
-      <c r="K573" s="14">
-        <f>COUNTIF(K3:K569, "FN") + K594</f>
+        <v>441</v>
+      </c>
+      <c r="K573" s="21">
+        <f>COUNTIF(K3:K569, "FN") + K597</f>
         <v>32</v>
       </c>
-      <c r="L573" s="14">
-        <f>COUNTIF(L3:L569, "FN") + L594</f>
+      <c r="L573" s="16">
+        <f>COUNTIF(L3:L569, "FN") + L597</f>
         <v>640</v>
       </c>
-      <c r="M573" s="14">
+      <c r="M573" s="16">
         <f t="shared" ref="L573:T573" si="95">COUNTIF(M3:M569, "FN")</f>
         <v>15</v>
       </c>
-      <c r="N573" s="14">
+      <c r="N573" s="16">
         <f t="shared" si="95"/>
         <v>214</v>
       </c>
-      <c r="O573" s="14">
+      <c r="O573" s="16">
         <f t="shared" si="95"/>
         <v>15</v>
       </c>
-      <c r="P573" s="14">
+      <c r="P573" s="16">
         <f t="shared" si="95"/>
         <v>130</v>
       </c>
-      <c r="Q573" s="14">
+      <c r="Q573" s="16">
         <f t="shared" si="95"/>
         <v>62</v>
       </c>
-      <c r="R573" s="14">
+      <c r="R573" s="16">
         <f t="shared" si="95"/>
         <v>266</v>
       </c>
-      <c r="S573" s="14">
+      <c r="S573" s="16">
         <f>COUNTIF(S3:S569, "FN")</f>
         <v>58</v>
       </c>
-      <c r="T573" s="14">
+      <c r="T573" s="27">
         <f t="shared" si="95"/>
         <v>195</v>
       </c>
     </row>
-    <row r="574" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B574" s="20" t="s">
+    <row r="574" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B574" s="22" t="s">
         <v>480</v>
       </c>
-      <c r="C574" s="15">
+      <c r="C574" s="17">
         <v>436</v>
       </c>
-      <c r="D574" s="15">
+      <c r="D574" s="17">
         <v>54</v>
       </c>
-      <c r="E574" s="15">
-        <v>2</v>
-      </c>
-      <c r="F574" s="15">
+      <c r="E574" s="17">
+        <v>2</v>
+      </c>
+      <c r="F574" s="17">
         <v>1</v>
       </c>
-      <c r="G574" s="15">
+      <c r="G574" s="17">
         <v>22</v>
       </c>
-      <c r="H574" s="15">
-        <v>2</v>
-      </c>
-      <c r="I574" s="26">
+      <c r="H574" s="17">
+        <v>2</v>
+      </c>
+      <c r="I574" s="28">
         <v>16</v>
       </c>
-      <c r="J574" s="11"/>
-      <c r="K574" s="7">
-        <f>K581+K588+K595</f>
+      <c r="J574" s="13"/>
+      <c r="K574" s="55">
+        <f>K581+K588+K598</f>
         <v>517</v>
       </c>
-      <c r="L574" s="7">
-        <v>2</v>
-      </c>
-      <c r="M574" s="7">
+      <c r="L574" s="54">
+        <v>2</v>
+      </c>
+      <c r="M574" s="54">
         <f>M581+M588</f>
         <v>458</v>
       </c>
-      <c r="N574" s="7">
+      <c r="N574" s="54">
         <v>0</v>
       </c>
-      <c r="O574" s="7">
+      <c r="O574" s="54">
         <f>O581+O588</f>
         <v>458</v>
       </c>
-      <c r="P574" s="7">
+      <c r="P574" s="54">
         <v>0</v>
       </c>
-      <c r="Q574" s="7">
+      <c r="Q574" s="54">
         <f>Q581+Q588</f>
         <v>437</v>
       </c>
-      <c r="R574" s="7">
+      <c r="R574" s="54">
         <v>0</v>
       </c>
-      <c r="S574" s="7">
+      <c r="S574" s="54">
         <f>S581+S588</f>
         <v>34</v>
       </c>
-      <c r="T574" s="11">
+      <c r="T574" s="15">
         <v>0</v>
       </c>
-      <c r="V574" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="575" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B575" s="21" t="s">
+    </row>
+    <row r="575" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B575" s="23" t="s">
         <v>478</v>
       </c>
-      <c r="C575" s="29">
+      <c r="C575" s="31">
         <f>C572/(C572+C574)</f>
         <v>0.47971360381861577</v>
       </c>
-      <c r="D575" s="29">
+      <c r="D575" s="31">
         <f t="shared" ref="D575:I575" si="96">D572/(D572+D574)</f>
-        <v>0.91428571428571426</v>
-      </c>
-      <c r="E575" s="29">
+        <v>0.91414944356120831</v>
+      </c>
+      <c r="E575" s="31">
         <f t="shared" si="96"/>
         <v>0.99047619047619051</v>
       </c>
-      <c r="F575" s="29">
+      <c r="F575" s="31">
         <f t="shared" si="96"/>
         <v>0.96969696969696972</v>
       </c>
-      <c r="G575" s="29">
+      <c r="G575" s="31">
         <f t="shared" si="96"/>
         <v>0.58490566037735847</v>
       </c>
-      <c r="H575" s="29">
+      <c r="H575" s="31">
         <f t="shared" si="96"/>
         <v>0.97826086956521741</v>
       </c>
-      <c r="I575" s="30">
+      <c r="I575" s="32">
         <f t="shared" si="96"/>
-        <v>0.85185185185185186</v>
-      </c>
-      <c r="J575" s="37"/>
-      <c r="K575" s="37">
+        <v>0.85321100917431192</v>
+      </c>
+      <c r="J575" s="39"/>
+      <c r="K575" s="50">
         <f>K572/(K572+K574)</f>
         <v>0.56952539550374692</v>
       </c>
-      <c r="L575" s="37">
+      <c r="L575" s="39">
         <f t="shared" ref="L575" si="97">L572/(L572+L574)</f>
         <v>0.97435897435897434</v>
       </c>
-      <c r="M575" s="37">
+      <c r="M575" s="39">
         <f t="shared" ref="M575" si="98">M572/(M572+M574)</f>
         <v>0.54653465346534658</v>
       </c>
-      <c r="N575" s="37">
+      <c r="N575" s="39">
         <f t="shared" ref="N575" si="99">N572/(N572+N574)</f>
         <v>1</v>
       </c>
-      <c r="O575" s="37">
+      <c r="O575" s="39">
         <f t="shared" ref="O575" si="100">O572/(O572+O574)</f>
         <v>0.54653465346534658</v>
       </c>
-      <c r="P575" s="37">
+      <c r="P575" s="39">
         <f t="shared" ref="P575" si="101">P572/(P572+P574)</f>
         <v>1</v>
       </c>
-      <c r="Q575" s="37">
+      <c r="Q575" s="39">
         <f t="shared" ref="Q575" si="102">Q572/(Q572+Q574)</f>
         <v>0.48222748815165878</v>
       </c>
-      <c r="R575" s="37">
+      <c r="R575" s="39">
         <f t="shared" ref="R575" si="103">R572/(R572+R574)</f>
         <v>1</v>
       </c>
-      <c r="S575" s="37">
+      <c r="S575" s="39">
         <f>S572/(S572+S574)</f>
         <v>0.93738489871086561</v>
       </c>
-      <c r="T575" s="37">
+      <c r="T575" s="33">
         <f t="shared" ref="T575" si="104">T572/(T572+T574)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="576" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B576" s="21" t="s">
+    <row r="576" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B576" s="23" t="s">
         <v>479</v>
       </c>
-      <c r="C576" s="29">
+      <c r="C576" s="31">
         <f>C572/(C572+C573)</f>
         <v>0.85897435897435892</v>
       </c>
-      <c r="D576" s="29">
+      <c r="D576" s="31">
         <f>D572/(D572+D573)</f>
-        <v>0.80334728033472802</v>
-      </c>
-      <c r="E576" s="29">
+        <v>0.80307262569832405</v>
+      </c>
+      <c r="E576" s="31">
         <f>E572/(E572+E573)</f>
         <v>0.58591549295774648</v>
       </c>
-      <c r="F576" s="29">
+      <c r="F576" s="31">
         <f>F572/(F572+F573)</f>
         <v>0.56140350877192979</v>
       </c>
-      <c r="G576" s="29">
+      <c r="G576" s="31">
         <f>G572/(G572+G573)</f>
         <v>5.4673721340388004E-2</v>
       </c>
-      <c r="H576" s="29">
+      <c r="H576" s="31">
         <f>H572/(H572+H573)</f>
-        <v>0.23622047244094488</v>
-      </c>
-      <c r="I576" s="31">
+        <v>0.23684210526315788</v>
+      </c>
+      <c r="I576" s="33">
         <f>I572/(I572+I573)</f>
-        <v>0.17196261682242991</v>
-      </c>
-      <c r="J576" s="37"/>
-      <c r="K576" s="37">
+        <v>0.17415730337078653</v>
+      </c>
+      <c r="J576" s="39"/>
+      <c r="K576" s="50">
         <f t="shared" ref="J576:T576" si="105">K572/(K572+K573)</f>
         <v>0.95530726256983245</v>
       </c>
-      <c r="L576" s="37">
+      <c r="L576" s="39">
         <f t="shared" si="105"/>
         <v>0.10614525139664804</v>
       </c>
-      <c r="M576" s="37">
+      <c r="M576" s="39">
         <f t="shared" si="105"/>
         <v>0.97354497354497349</v>
       </c>
-      <c r="N576" s="37">
+      <c r="N576" s="39">
         <f t="shared" si="105"/>
         <v>0.62257495590828926</v>
       </c>
-      <c r="O576" s="37">
+      <c r="O576" s="39">
         <f t="shared" si="105"/>
         <v>0.97354497354497349</v>
       </c>
-      <c r="P576" s="37">
+      <c r="P576" s="39">
         <f t="shared" si="105"/>
         <v>0.7707231040564374</v>
       </c>
-      <c r="Q576" s="37">
+      <c r="Q576" s="39">
         <f t="shared" si="105"/>
         <v>0.86780383795309168</v>
       </c>
-      <c r="R576" s="37">
+      <c r="R576" s="39">
         <f t="shared" si="105"/>
         <v>0.43283582089552236</v>
       </c>
-      <c r="S576" s="37">
+      <c r="S576" s="39">
         <f t="shared" si="105"/>
         <v>0.89770723104056438</v>
       </c>
-      <c r="T576" s="37">
+      <c r="T576" s="33">
         <f t="shared" si="105"/>
         <v>0.65608465608465605</v>
       </c>
     </row>
-    <row r="577" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B577" s="22" t="s">
+    <row r="577" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B577" s="24" t="s">
         <v>491</v>
       </c>
-      <c r="C577" s="32">
+      <c r="C577" s="34">
         <f>(2*C572)/((2*C572)+C574+C573)</f>
         <v>0.61562021439509951</v>
       </c>
-      <c r="D577" s="32">
+      <c r="D577" s="34">
         <f>(2*D572)/((2*D572)+D574+D573)</f>
-        <v>0.85523385300668153</v>
-      </c>
-      <c r="E577" s="32">
+        <v>0.85501858736059477</v>
+      </c>
+      <c r="E577" s="34">
         <f t="shared" ref="D577:I577" si="106">(2*E572)/((2*E572)+E574+E573)</f>
         <v>0.73628318584070795</v>
       </c>
-      <c r="F577" s="32">
+      <c r="F577" s="34">
         <f t="shared" si="106"/>
         <v>0.71111111111111114</v>
       </c>
-      <c r="G577" s="32">
+      <c r="G577" s="34">
         <f t="shared" si="106"/>
         <v>0.1</v>
       </c>
-      <c r="H577" s="32">
+      <c r="H577" s="34">
         <f t="shared" si="106"/>
-        <v>0.38054968287526425</v>
-      </c>
-      <c r="I577" s="33">
+        <v>0.38135593220338981</v>
+      </c>
+      <c r="I577" s="35">
         <f t="shared" si="106"/>
-        <v>0.28615863141524106</v>
-      </c>
-      <c r="J577" s="37"/>
-      <c r="K577" s="37">
+        <v>0.28926905132192848</v>
+      </c>
+      <c r="J577" s="39"/>
+      <c r="K577" s="51">
         <f t="shared" ref="J577:T577" si="107">(2*K572)/((2*K572)+K574+K573)</f>
         <v>0.71361502347417838</v>
       </c>
-      <c r="L577" s="37">
+      <c r="L577" s="34">
         <f t="shared" si="107"/>
         <v>0.19143576826196473</v>
       </c>
-      <c r="M577" s="37">
+      <c r="M577" s="34">
         <f t="shared" si="107"/>
         <v>0.70006341154090046</v>
       </c>
-      <c r="N577" s="37">
+      <c r="N577" s="34">
         <f t="shared" si="107"/>
         <v>0.7673913043478261</v>
       </c>
-      <c r="O577" s="37">
+      <c r="O577" s="34">
         <f t="shared" si="107"/>
         <v>0.70006341154090046</v>
       </c>
-      <c r="P577" s="37">
+      <c r="P577" s="34">
         <f t="shared" si="107"/>
         <v>0.87051792828685259</v>
       </c>
-      <c r="Q577" s="37">
+      <c r="Q577" s="34">
         <f t="shared" si="107"/>
         <v>0.61995430312262001</v>
       </c>
-      <c r="R577" s="37">
+      <c r="R577" s="34">
         <f t="shared" si="107"/>
         <v>0.60416666666666663</v>
       </c>
-      <c r="S577" s="37">
+      <c r="S577" s="34">
         <f t="shared" si="107"/>
         <v>0.91711711711711708</v>
       </c>
-      <c r="T577" s="37">
+      <c r="T577" s="35">
         <f t="shared" si="107"/>
         <v>0.792332268370607</v>
       </c>
     </row>
-    <row r="578" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B578" s="17"/>
-      <c r="C578" s="17"/>
-      <c r="D578" s="17"/>
-      <c r="E578" s="17"/>
-      <c r="F578" s="17"/>
-      <c r="G578" s="17"/>
-      <c r="H578" s="17"/>
-      <c r="I578" s="17"/>
-      <c r="K578" s="11"/>
-      <c r="L578" s="11"/>
-      <c r="M578" s="11"/>
-      <c r="N578" s="11"/>
-      <c r="O578" s="11"/>
-      <c r="P578" s="11"/>
-      <c r="Q578" s="11"/>
-      <c r="R578" s="11"/>
-      <c r="S578" s="11"/>
-      <c r="T578" s="11"/>
-    </row>
-    <row r="579" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B579" s="18" t="s">
+    <row r="578" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B578" s="19"/>
+      <c r="C578" s="19"/>
+      <c r="D578" s="19"/>
+      <c r="E578" s="19"/>
+      <c r="F578" s="19"/>
+      <c r="G578" s="19"/>
+      <c r="H578" s="19"/>
+      <c r="I578" s="19"/>
+      <c r="K578" s="19"/>
+      <c r="L578" s="19"/>
+      <c r="M578" s="19"/>
+      <c r="N578" s="19"/>
+      <c r="O578" s="19"/>
+      <c r="P578" s="19"/>
+      <c r="Q578" s="19"/>
+      <c r="R578" s="19"/>
+      <c r="S578" s="19"/>
+      <c r="T578" s="19"/>
+    </row>
+    <row r="579" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B579" s="20" t="s">
         <v>487</v>
       </c>
       <c r="C579" s="1">
@@ -36043,50 +36089,50 @@
         <v>27</v>
       </c>
       <c r="H579" s="1"/>
-      <c r="I579" s="24"/>
-      <c r="K579" s="14">
+      <c r="I579" s="26"/>
+      <c r="K579" s="21">
         <f>COUNTIF(K3:K7, "TP") + COUNTIF(K14:K30, "TP") + COUNTIF(K73:K87, "TP") + COUNTIF(K122:K129, "TP") + COUNTIF(K142:K148, "TP") + COUNTIF(K162:K173, "TP") + COUNTIF(K203:K217, "TP") + COUNTIF(K252:K268, "TP") + COUNTIF(K306:K313, "TP") + COUNTIF(K327:K331, "TP") + COUNTIF(K338:K348, "TP") + COUNTIF(K375:K385, "TP") + COUNTIF(K404:K413, "TP") + COUNTIF(K443:K453, "TP") + COUNTIF(K478:K489, "TP") + COUNTIF(K518:K526, "TP") + COUNTIF(K545:K553, "TP")</f>
         <v>179</v>
       </c>
-      <c r="L579" s="14">
+      <c r="L579" s="16">
         <f t="shared" ref="L579:T579" si="108">COUNTIF(L3:L7, "TP") + COUNTIF(L14:L30, "TP") + COUNTIF(L73:L87, "TP") + COUNTIF(L122:L129, "TP") + COUNTIF(L142:L148, "TP") + COUNTIF(L162:L173, "TP") + COUNTIF(L203:L217, "TP") + COUNTIF(L252:L268, "TP") + COUNTIF(L306:L313, "TP") + COUNTIF(L327:L331, "TP") + COUNTIF(L338:L348, "TP") + COUNTIF(L375:L385, "TP") + COUNTIF(L404:L413, "TP") + COUNTIF(L443:L453, "TP") + COUNTIF(L478:L489, "TP") + COUNTIF(L518:L526, "TP") + COUNTIF(L545:L553, "TP")</f>
         <v>24</v>
       </c>
-      <c r="M579" s="14">
+      <c r="M579" s="16">
         <f t="shared" si="108"/>
         <v>179</v>
       </c>
-      <c r="N579" s="14">
+      <c r="N579" s="16">
         <f t="shared" si="108"/>
         <v>145</v>
       </c>
-      <c r="O579" s="14">
+      <c r="O579" s="16">
         <f t="shared" si="108"/>
         <v>179</v>
       </c>
-      <c r="P579" s="14">
+      <c r="P579" s="16">
         <f t="shared" si="108"/>
         <v>158</v>
       </c>
-      <c r="Q579" s="14">
+      <c r="Q579" s="16">
         <f t="shared" si="108"/>
         <v>125</v>
       </c>
-      <c r="R579" s="14">
+      <c r="R579" s="16">
         <f t="shared" si="108"/>
         <v>82</v>
       </c>
-      <c r="S579" s="14">
+      <c r="S579" s="16">
         <f t="shared" si="108"/>
         <v>178</v>
       </c>
-      <c r="T579" s="14">
+      <c r="T579" s="27">
         <f t="shared" si="108"/>
         <v>153</v>
       </c>
     </row>
-    <row r="580" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B580" s="19" t="s">
+    <row r="580" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B580" s="21" t="s">
         <v>484</v>
       </c>
       <c r="C580" s="1">
@@ -36110,325 +36156,322 @@
         <v>155</v>
       </c>
       <c r="H580" s="1"/>
-      <c r="I580" s="25"/>
-      <c r="K580" s="14">
+      <c r="I580" s="27"/>
+      <c r="K580" s="21">
         <f>COUNTIF(K3:K7, "FN") + COUNTIF(K14:K30, "FN") + COUNTIF(K73:K87, "FN") + COUNTIF(K122:K129, "FN") + COUNTIF(K142:K148, "FN") + COUNTIF(K162:K173, "FN") + COUNTIF(K203:K217, "FN") + COUNTIF(K252:K268, "FN") + COUNTIF(K306:K313, "FN") + COUNTIF(K327:K331, "FN") + COUNTIF(K338:K348, "FN") + COUNTIF(K375:K385, "FN") + COUNTIF(K404:K413, "FN") + COUNTIF(K443:K453, "FN") + COUNTIF(K478:K489, "FN") + COUNTIF(K518:K526, "FN") + COUNTIF(K545:K553, "FN")</f>
         <v>3</v>
       </c>
-      <c r="L580" s="14">
+      <c r="L580" s="16">
         <f t="shared" ref="L580:T580" si="109">COUNTIF(L3:L7, "FN") + COUNTIF(L14:L30, "FN") + COUNTIF(L73:L87, "FN") + COUNTIF(L122:L129, "FN") + COUNTIF(L142:L148, "FN") + COUNTIF(L162:L173, "FN") + COUNTIF(L203:L217, "FN") + COUNTIF(L252:L268, "FN") + COUNTIF(L306:L313, "FN") + COUNTIF(L327:L331, "FN") + COUNTIF(L338:L348, "FN") + COUNTIF(L375:L385, "FN") + COUNTIF(L404:L413, "FN") + COUNTIF(L443:L453, "FN") + COUNTIF(L478:L489, "FN") + COUNTIF(L518:L526, "FN") + COUNTIF(L545:L553, "FN")</f>
         <v>158</v>
       </c>
-      <c r="M580" s="14">
+      <c r="M580" s="16">
         <f t="shared" si="109"/>
         <v>3</v>
       </c>
-      <c r="N580" s="14">
+      <c r="N580" s="16">
         <f t="shared" si="109"/>
         <v>37</v>
       </c>
-      <c r="O580" s="14">
+      <c r="O580" s="16">
         <f t="shared" si="109"/>
         <v>3</v>
       </c>
-      <c r="P580" s="14">
+      <c r="P580" s="16">
         <f t="shared" si="109"/>
         <v>24</v>
       </c>
-      <c r="Q580" s="14">
+      <c r="Q580" s="16">
         <f t="shared" si="109"/>
         <v>19</v>
       </c>
-      <c r="R580" s="14">
+      <c r="R580" s="16">
         <f t="shared" si="109"/>
         <v>62</v>
       </c>
-      <c r="S580" s="14">
+      <c r="S580" s="16">
         <f t="shared" si="109"/>
         <v>4</v>
       </c>
-      <c r="T580" s="14">
+      <c r="T580" s="27">
         <f t="shared" si="109"/>
         <v>29</v>
       </c>
     </row>
-    <row r="581" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B581" s="20" t="s">
+    <row r="581" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B581" s="22" t="s">
         <v>481</v>
       </c>
-      <c r="C581" s="15">
+      <c r="C581" s="17">
         <v>41</v>
       </c>
-      <c r="D581" s="15">
+      <c r="D581" s="17">
         <v>5</v>
       </c>
-      <c r="E581" s="15">
+      <c r="E581" s="17">
         <v>0</v>
       </c>
-      <c r="F581" s="15">
+      <c r="F581" s="17">
         <v>1</v>
       </c>
-      <c r="G581" s="15">
+      <c r="G581" s="17">
         <v>21</v>
       </c>
-      <c r="H581" s="15"/>
-      <c r="I581" s="26"/>
-      <c r="K581" s="11">
+      <c r="H581" s="17"/>
+      <c r="I581" s="28"/>
+      <c r="K581" s="53">
         <v>68</v>
       </c>
-      <c r="L581" s="11">
+      <c r="L581" s="14">
         <v>0</v>
       </c>
-      <c r="M581" s="11">
+      <c r="M581" s="14">
         <v>46</v>
       </c>
-      <c r="N581" s="11">
+      <c r="N581" s="14">
         <v>0</v>
       </c>
-      <c r="O581" s="7">
+      <c r="O581" s="54">
         <v>46</v>
       </c>
-      <c r="P581" s="7">
+      <c r="P581" s="54">
         <v>0</v>
       </c>
-      <c r="Q581" s="7">
+      <c r="Q581" s="54">
         <v>41</v>
       </c>
-      <c r="R581" s="11">
+      <c r="R581" s="14">
         <v>0</v>
       </c>
-      <c r="S581" s="7">
+      <c r="S581" s="54">
         <v>5</v>
       </c>
-      <c r="T581" s="11">
+      <c r="T581" s="15">
         <v>0</v>
       </c>
-      <c r="V581" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="582" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B582" s="19" t="s">
+    </row>
+    <row r="582" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B582" s="21" t="s">
         <v>493</v>
       </c>
-      <c r="C582" s="29">
+      <c r="C582" s="31">
         <f>C579/(C579+C581)</f>
         <v>0.75</v>
       </c>
-      <c r="D582" s="29">
+      <c r="D582" s="31">
         <f t="shared" ref="D582:G582" si="110">D579/(D579+D581)</f>
         <v>0.97267759562841527</v>
       </c>
-      <c r="E582" s="29">
+      <c r="E582" s="31">
         <f t="shared" si="110"/>
         <v>1</v>
       </c>
-      <c r="F582" s="29">
+      <c r="F582" s="31">
         <f t="shared" si="110"/>
         <v>0.96969696969696972</v>
       </c>
-      <c r="G582" s="29">
+      <c r="G582" s="31">
         <f t="shared" si="110"/>
         <v>0.5625</v>
       </c>
-      <c r="H582" s="14"/>
-      <c r="I582" s="25"/>
-      <c r="K582" s="37">
+      <c r="H582" s="16"/>
+      <c r="I582" s="27"/>
+      <c r="K582" s="50">
         <f t="shared" ref="K582" si="111">K579/(K579+K581)</f>
         <v>0.7246963562753036</v>
       </c>
-      <c r="L582" s="37">
+      <c r="L582" s="39">
         <f t="shared" ref="L582" si="112">L579/(L579+L581)</f>
         <v>1</v>
       </c>
-      <c r="M582" s="37">
+      <c r="M582" s="39">
         <f t="shared" ref="M582" si="113">M579/(M579+M581)</f>
         <v>0.79555555555555557</v>
       </c>
-      <c r="N582" s="37">
+      <c r="N582" s="39">
         <f t="shared" ref="N582" si="114">N579/(N579+N581)</f>
         <v>1</v>
       </c>
-      <c r="O582" s="37">
+      <c r="O582" s="39">
         <f t="shared" ref="O582" si="115">O579/(O579+O581)</f>
         <v>0.79555555555555557</v>
       </c>
-      <c r="P582" s="37">
+      <c r="P582" s="39">
         <f t="shared" ref="P582" si="116">P579/(P579+P581)</f>
         <v>1</v>
       </c>
-      <c r="Q582" s="37">
+      <c r="Q582" s="39">
         <f t="shared" ref="Q582" si="117">Q579/(Q579+Q581)</f>
         <v>0.75301204819277112</v>
       </c>
-      <c r="R582" s="37">
+      <c r="R582" s="39">
         <f t="shared" ref="R582" si="118">R579/(R579+R581)</f>
         <v>1</v>
       </c>
-      <c r="S582" s="37">
+      <c r="S582" s="39">
         <f t="shared" ref="S582" si="119">S579/(S579+S581)</f>
         <v>0.97267759562841527</v>
       </c>
-      <c r="T582" s="37">
+      <c r="T582" s="33">
         <f t="shared" ref="T582" si="120">T579/(T579+T581)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="583" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B583" s="19" t="s">
+    <row r="583" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B583" s="21" t="s">
         <v>492</v>
       </c>
-      <c r="C583" s="29">
+      <c r="C583" s="31">
         <f>C579/(C579+C580)</f>
         <v>0.85416666666666663</v>
       </c>
-      <c r="D583" s="29">
+      <c r="D583" s="31">
         <f t="shared" ref="D583:I583" si="121">D579/(D579+D580)</f>
         <v>0.97802197802197799</v>
       </c>
-      <c r="E583" s="29">
+      <c r="E583" s="31">
         <f t="shared" si="121"/>
         <v>0.76363636363636367</v>
       </c>
-      <c r="F583" s="29">
+      <c r="F583" s="31">
         <f t="shared" si="121"/>
         <v>0.56140350877192979</v>
       </c>
-      <c r="G583" s="29">
+      <c r="G583" s="31">
         <f>G579/(G579+G580)</f>
         <v>0.14835164835164835</v>
       </c>
       <c r="I583" s="5"/>
-      <c r="K583" s="37">
+      <c r="K583" s="50">
         <f>K579/(K579+K580)</f>
         <v>0.98351648351648346</v>
       </c>
-      <c r="L583" s="37">
+      <c r="L583" s="39">
         <f>L579/(L579+L580)</f>
         <v>0.13186813186813187</v>
       </c>
-      <c r="M583" s="37">
+      <c r="M583" s="39">
         <f t="shared" ref="L583:T583" si="122">M579/(M579+M580)</f>
         <v>0.98351648351648346</v>
       </c>
-      <c r="N583" s="37">
+      <c r="N583" s="39">
         <f t="shared" si="122"/>
         <v>0.79670329670329665</v>
       </c>
-      <c r="O583" s="37">
+      <c r="O583" s="39">
         <f t="shared" si="122"/>
         <v>0.98351648351648346</v>
       </c>
-      <c r="P583" s="37">
+      <c r="P583" s="39">
         <f t="shared" si="122"/>
         <v>0.86813186813186816</v>
       </c>
-      <c r="Q583" s="37">
+      <c r="Q583" s="39">
         <f t="shared" si="122"/>
         <v>0.86805555555555558</v>
       </c>
-      <c r="R583" s="37">
+      <c r="R583" s="39">
         <f t="shared" si="122"/>
         <v>0.56944444444444442</v>
       </c>
-      <c r="S583" s="37">
+      <c r="S583" s="39">
         <f t="shared" si="122"/>
         <v>0.97802197802197799</v>
       </c>
-      <c r="T583" s="37">
+      <c r="T583" s="33">
         <f t="shared" si="122"/>
         <v>0.84065934065934067</v>
       </c>
     </row>
-    <row r="584" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B584" s="23" t="s">
+    <row r="584" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B584" s="25" t="s">
         <v>494</v>
       </c>
-      <c r="C584" s="32">
+      <c r="C584" s="34">
         <f>(2*C579)/((2*C579)+C581+C580)</f>
         <v>0.79870129870129869</v>
       </c>
-      <c r="D584" s="32">
+      <c r="D584" s="34">
         <f t="shared" ref="D584:G584" si="123">(2*D579)/((2*D579)+D581+D580)</f>
         <v>0.97534246575342465</v>
       </c>
-      <c r="E584" s="32">
+      <c r="E584" s="34">
         <f t="shared" si="123"/>
         <v>0.865979381443299</v>
       </c>
-      <c r="F584" s="32">
+      <c r="F584" s="34">
         <f t="shared" si="123"/>
         <v>0.71111111111111114</v>
       </c>
-      <c r="G584" s="32">
+      <c r="G584" s="34">
         <f t="shared" si="123"/>
         <v>0.23478260869565218</v>
       </c>
-      <c r="H584" s="16"/>
-      <c r="I584" s="27"/>
-      <c r="K584" s="37">
+      <c r="H584" s="18"/>
+      <c r="I584" s="29"/>
+      <c r="K584" s="51">
         <f t="shared" ref="K584:T584" si="124">(2*K579)/((2*K579)+K581+K580)</f>
         <v>0.83449883449883455</v>
       </c>
-      <c r="L584" s="37">
+      <c r="L584" s="34">
         <f t="shared" si="124"/>
         <v>0.23300970873786409</v>
       </c>
-      <c r="M584" s="37">
+      <c r="M584" s="34">
         <f>(2*M579)/((2*M579)+M581+M580)</f>
         <v>0.87960687960687955</v>
       </c>
-      <c r="N584" s="37">
+      <c r="N584" s="34">
         <f t="shared" si="124"/>
         <v>0.88685015290519875</v>
       </c>
-      <c r="O584" s="37">
+      <c r="O584" s="34">
         <f t="shared" si="124"/>
         <v>0.87960687960687955</v>
       </c>
-      <c r="P584" s="37">
+      <c r="P584" s="34">
         <f t="shared" si="124"/>
         <v>0.92941176470588238</v>
       </c>
-      <c r="Q584" s="37">
+      <c r="Q584" s="34">
         <f t="shared" si="124"/>
         <v>0.80645161290322576</v>
       </c>
-      <c r="R584" s="37">
+      <c r="R584" s="34">
         <f t="shared" si="124"/>
         <v>0.72566371681415931</v>
       </c>
-      <c r="S584" s="37">
+      <c r="S584" s="34">
         <f t="shared" si="124"/>
         <v>0.97534246575342465</v>
       </c>
-      <c r="T584" s="37">
+      <c r="T584" s="35">
         <f t="shared" si="124"/>
         <v>0.91343283582089552</v>
       </c>
     </row>
-    <row r="585" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B585" s="17"/>
-      <c r="C585" s="17"/>
-      <c r="D585" s="17"/>
-      <c r="E585" s="17"/>
-      <c r="F585" s="17"/>
-      <c r="G585" s="17"/>
-      <c r="H585" s="17"/>
-      <c r="I585" s="17"/>
-      <c r="K585" s="11"/>
-      <c r="L585" s="11"/>
-      <c r="M585" s="11"/>
-      <c r="N585" s="11"/>
-      <c r="O585" s="11"/>
-      <c r="P585" s="11"/>
-      <c r="Q585" s="11"/>
-      <c r="R585" s="11"/>
-      <c r="S585" s="11"/>
-      <c r="T585" s="11"/>
-    </row>
-    <row r="586" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B586" s="18" t="s">
+    <row r="585" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B585" s="19"/>
+      <c r="C585" s="19"/>
+      <c r="D585" s="19"/>
+      <c r="E585" s="19"/>
+      <c r="F585" s="19"/>
+      <c r="G585" s="19"/>
+      <c r="H585" s="19"/>
+      <c r="I585" s="19"/>
+      <c r="K585" s="19"/>
+      <c r="L585" s="19"/>
+      <c r="M585" s="19"/>
+      <c r="N585" s="19"/>
+      <c r="O585" s="19"/>
+      <c r="P585" s="19"/>
+      <c r="Q585" s="19"/>
+      <c r="R585" s="19"/>
+      <c r="S585" s="19"/>
+      <c r="T585" s="19"/>
+    </row>
+    <row r="586" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B586" s="20" t="s">
         <v>488</v>
       </c>
       <c r="C586" s="1">
@@ -36449,53 +36492,53 @@
         <v>4</v>
       </c>
       <c r="H586" s="1"/>
-      <c r="I586" s="24">
+      <c r="I586" s="26">
         <f>COUNTIF(I554:I569, " TP") + COUNTIF(I527:I544, " TP") + COUNTIF(I490:I517, " TP") + COUNTIF(I454:I477, " TP") + COUNTIF(I414:I442, " TP") + COUNTIF(I386:I403, " TP") + COUNTIF(I349:I374, " TP") + COUNTIF(I332:I337, " TP") + COUNTIF(I314:I326, " TP") + COUNTIF(I269:I305, " TP") + COUNTIF(I218:I251, " TP") + COUNTIF(I174:I202, " TP") + COUNTIF(I149:I161, " TP") + COUNTIF(I130:I141, " TP") + COUNTIF(I88:I121, " TP") + COUNTIF(I31:I72, " TP") + COUNTIF(I8:I13, " TP")</f>
         <v>7</v>
       </c>
-      <c r="K586" s="1">
+      <c r="K586" s="21">
         <f>COUNTIF(K554:K569, "TP") + COUNTIF(K527:K544, "TP") + COUNTIF(K490:K517, "TP") + COUNTIF(K454:K477, "TP") + COUNTIF(K414:K442, "TP") + COUNTIF(K386:K403, "TP") + COUNTIF(K349:K374, "TP") + COUNTIF(K332:K337, "TP") + COUNTIF(K314:K326, "TP") + COUNTIF(K269:K305, "TP") + COUNTIF(K218:K251, "TP") + COUNTIF(K174:K202, "TP") + COUNTIF(K149:K161, "TP") + COUNTIF(K130:K141, "TP") + COUNTIF(K88:K121, "TP") + COUNTIF(K31:K72, "TP") + COUNTIF(K8:K13, "TP")</f>
         <v>374</v>
       </c>
-      <c r="L586" s="1">
+      <c r="L586" s="16">
         <f t="shared" ref="L586:T586" si="125">COUNTIF(L554:L569, "TP") + COUNTIF(L527:L544, "TP") + COUNTIF(L490:L517, "TP") + COUNTIF(L454:L477, "TP") + COUNTIF(L414:L442, "TP") + COUNTIF(L386:L403, "TP") + COUNTIF(L349:L374, "TP") + COUNTIF(L332:L337, "TP") + COUNTIF(L314:L326, "TP") + COUNTIF(L269:L305, "TP") + COUNTIF(L218:L251, "TP") + COUNTIF(L174:L202, "TP") + COUNTIF(L149:L161, "TP") + COUNTIF(L130:L141, "TP") + COUNTIF(L88:L121, "TP") + COUNTIF(L31:L72, "TP") + COUNTIF(L8:L13, "TP")</f>
         <v>0</v>
       </c>
-      <c r="M586" s="1">
+      <c r="M586" s="16">
         <f t="shared" si="125"/>
         <v>373</v>
       </c>
-      <c r="N586" s="1">
+      <c r="N586" s="16">
         <f t="shared" si="125"/>
         <v>208</v>
       </c>
-      <c r="O586" s="1">
+      <c r="O586" s="16">
         <f t="shared" si="125"/>
         <v>373</v>
       </c>
-      <c r="P586" s="1">
+      <c r="P586" s="16">
         <f t="shared" si="125"/>
         <v>279</v>
       </c>
-      <c r="Q586" s="1">
+      <c r="Q586" s="16">
         <f t="shared" si="125"/>
         <v>282</v>
       </c>
-      <c r="R586" s="1">
+      <c r="R586" s="16">
         <f t="shared" si="125"/>
         <v>121</v>
       </c>
-      <c r="S586" s="1">
+      <c r="S586" s="16">
         <f t="shared" si="125"/>
         <v>331</v>
       </c>
-      <c r="T586" s="1">
+      <c r="T586" s="27">
         <f t="shared" si="125"/>
         <v>219</v>
       </c>
     </row>
-    <row r="587" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B587" s="19" t="s">
+    <row r="587" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B587" s="21" t="s">
         <v>485</v>
       </c>
       <c r="C587" s="1">
@@ -36519,555 +36562,741 @@
         <f>COUNTIF(H554:H569, " FN") + COUNTIF(H527:H544, " FN") + COUNTIF(H490:H517, " FN") + COUNTIF(H454:H477, " FN") + COUNTIF(H414:H442, " FN") + COUNTIF(H386:H403, " FN") + COUNTIF(H349:H374, " FN") + COUNTIF(H332:H337, " FN") + COUNTIF(H314:H326, " FN") + COUNTIF(H269:H305, " FN") + COUNTIF(H218:H251, " FN") + COUNTIF(H174:H202, " FN") + COUNTIF(H149:H161, " FN") + COUNTIF(H130:H141, " FN") + COUNTIF(H88:H121, " FN") + COUNTIF(H31:H72, " FN") + COUNTIF(H8:H13, " FN")</f>
         <v>259</v>
       </c>
-      <c r="I587" s="25">
+      <c r="I587" s="27">
         <f>COUNTIF(I554:I569, " FN") + COUNTIF(I527:I544, " FN") + COUNTIF(I490:I517, " FN") + COUNTIF(I454:I477, " FN") + COUNTIF(I414:I442, " FN") + COUNTIF(I386:I403, " FN") + COUNTIF(I349:I374, " FN") + COUNTIF(I332:I337, " FN") + COUNTIF(I314:I326, " FN") + COUNTIF(I269:I305, " FN") + COUNTIF(I218:I251, " FN") + COUNTIF(I174:I202, " FN") + COUNTIF(I149:I161, " FN") + COUNTIF(I130:I141, " FN") + COUNTIF(I88:I121, " FN") + COUNTIF(I31:I72, " FN") + COUNTIF(I8:I13, " FN")</f>
         <v>378</v>
       </c>
-      <c r="K587" s="1">
+      <c r="K587" s="21">
         <f>COUNTIF(K554:K569, "FN") + COUNTIF(K527:K544, "FN") + COUNTIF(K490:K517, "FN") + COUNTIF(K454:K477, "FN") + COUNTIF(K414:K442, "FN") + COUNTIF(K386:K403, "FN") + COUNTIF(K349:K374, "FN") + COUNTIF(K332:K337, "FN") + COUNTIF(K314:K326, "FN") + COUNTIF(K269:K305, "FN") + COUNTIF(K218:K251, "FN") + COUNTIF(K174:K202, "FN") + COUNTIF(K149:K161, "FN") + COUNTIF(K130:K141, "FN") + COUNTIF(K88:K121, "FN") + COUNTIF(K31:K72, "FN") + COUNTIF(K8:K13, "FN")</f>
         <v>11</v>
       </c>
-      <c r="L587" s="1">
+      <c r="L587" s="16">
         <f t="shared" ref="L587:T587" si="126">COUNTIF(L554:L569, "FN") + COUNTIF(L527:L544, "FN") + COUNTIF(L490:L517, "FN") + COUNTIF(L454:L477, "FN") + COUNTIF(L414:L442, "FN") + COUNTIF(L386:L403, "FN") + COUNTIF(L349:L374, "FN") + COUNTIF(L332:L337, "FN") + COUNTIF(L314:L326, "FN") + COUNTIF(L269:L305, "FN") + COUNTIF(L218:L251, "FN") + COUNTIF(L174:L202, "FN") + COUNTIF(L149:L161, "FN") + COUNTIF(L130:L141, "FN") + COUNTIF(L88:L121, "FN") + COUNTIF(L31:L72, "FN") + COUNTIF(L8:L13, "FN")</f>
         <v>385</v>
       </c>
-      <c r="M587" s="1">
+      <c r="M587" s="16">
         <f t="shared" si="126"/>
         <v>12</v>
       </c>
-      <c r="N587" s="1">
+      <c r="N587" s="16">
         <f t="shared" si="126"/>
         <v>177</v>
       </c>
-      <c r="O587" s="1">
+      <c r="O587" s="16">
         <f t="shared" si="126"/>
         <v>12</v>
       </c>
-      <c r="P587" s="1">
+      <c r="P587" s="16">
         <f t="shared" si="126"/>
         <v>106</v>
       </c>
-      <c r="Q587" s="1">
+      <c r="Q587" s="16">
         <f t="shared" si="126"/>
         <v>43</v>
       </c>
-      <c r="R587" s="1">
+      <c r="R587" s="16">
         <f t="shared" si="126"/>
         <v>204</v>
       </c>
-      <c r="S587" s="1">
+      <c r="S587" s="16">
         <f t="shared" si="126"/>
         <v>54</v>
       </c>
-      <c r="T587" s="1">
+      <c r="T587" s="27">
         <f t="shared" si="126"/>
         <v>166</v>
       </c>
     </row>
-    <row r="588" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B588" s="20" t="s">
+    <row r="588" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B588" s="22" t="s">
         <v>483</v>
       </c>
-      <c r="C588" s="15">
+      <c r="C588" s="17">
         <v>395</v>
       </c>
-      <c r="D588" s="15">
+      <c r="D588" s="17">
         <v>27</v>
       </c>
-      <c r="E588" s="15">
-        <v>2</v>
-      </c>
-      <c r="F588" s="15"/>
-      <c r="G588" s="15">
+      <c r="E588" s="17">
+        <v>2</v>
+      </c>
+      <c r="F588" s="17"/>
+      <c r="G588" s="17">
         <v>1</v>
       </c>
-      <c r="H588" s="15"/>
-      <c r="I588" s="26">
-        <v>2</v>
-      </c>
-      <c r="K588" s="11">
+      <c r="H588" s="17"/>
+      <c r="I588" s="28">
+        <v>2</v>
+      </c>
+      <c r="K588" s="53">
         <v>415</v>
       </c>
-      <c r="L588" s="11">
+      <c r="L588" s="14">
         <v>0</v>
       </c>
-      <c r="M588" s="7">
+      <c r="M588" s="54">
         <v>412</v>
       </c>
-      <c r="N588" s="11">
+      <c r="N588" s="14">
         <v>0</v>
       </c>
-      <c r="O588" s="7">
+      <c r="O588" s="54">
         <v>412</v>
       </c>
-      <c r="P588" s="11">
+      <c r="P588" s="14">
         <v>0</v>
       </c>
-      <c r="Q588" s="7">
+      <c r="Q588" s="54">
         <v>396</v>
       </c>
-      <c r="R588" s="11">
+      <c r="R588" s="14">
         <v>0</v>
       </c>
-      <c r="S588" s="7">
+      <c r="S588" s="54">
         <v>29</v>
       </c>
-      <c r="T588" s="11">
+      <c r="T588" s="15">
         <v>0</v>
       </c>
-      <c r="V588" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="589" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B589" s="21" t="s">
+    </row>
+    <row r="589" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B589" s="23" t="s">
         <v>495</v>
       </c>
-      <c r="C589" s="29">
+      <c r="C589" s="31">
         <f>C586/(C586+C588)</f>
         <v>0.41394658753709201</v>
       </c>
-      <c r="D589" s="29">
+      <c r="D589" s="31">
         <f t="shared" ref="D589:K589" si="127">D586/(D586+D588)</f>
         <v>0.9221902017291066</v>
       </c>
-      <c r="E589" s="29">
+      <c r="E589" s="31">
         <f t="shared" si="127"/>
         <v>0.98412698412698407</v>
       </c>
-      <c r="F589" s="29">
+      <c r="F589" s="31">
         <v>0</v>
       </c>
-      <c r="G589" s="29">
+      <c r="G589" s="31">
         <f t="shared" si="127"/>
         <v>0.8</v>
       </c>
-      <c r="I589" s="28"/>
-      <c r="K589" s="37">
+      <c r="I589" s="30"/>
+      <c r="K589" s="50">
         <f t="shared" si="127"/>
         <v>0.47401774397972118</v>
       </c>
-      <c r="L589" s="37" t="e">
+      <c r="L589" s="39" t="e">
         <f t="shared" ref="L589" si="128">L586/(L586+L588)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M589" s="37">
+      <c r="M589" s="39">
         <f t="shared" ref="M589" si="129">M586/(M586+M588)</f>
         <v>0.47515923566878981</v>
       </c>
-      <c r="N589" s="37">
+      <c r="N589" s="39">
         <f t="shared" ref="N589" si="130">N586/(N586+N588)</f>
         <v>1</v>
       </c>
-      <c r="O589" s="37">
+      <c r="O589" s="39">
         <f t="shared" ref="O589" si="131">O586/(O586+O588)</f>
         <v>0.47515923566878981</v>
       </c>
-      <c r="P589" s="37">
+      <c r="P589" s="39">
         <f t="shared" ref="P589" si="132">P586/(P586+P588)</f>
         <v>1</v>
       </c>
-      <c r="Q589" s="37">
+      <c r="Q589" s="39">
         <f t="shared" ref="Q589" si="133">Q586/(Q586+Q588)</f>
         <v>0.41592920353982299</v>
       </c>
-      <c r="R589" s="37">
+      <c r="R589" s="39">
         <f t="shared" ref="R589" si="134">R586/(R586+R588)</f>
         <v>1</v>
       </c>
-      <c r="S589" s="37">
+      <c r="S589" s="39">
         <f t="shared" ref="S589" si="135">S586/(S586+S588)</f>
         <v>0.9194444444444444</v>
       </c>
-      <c r="T589" s="37">
+      <c r="T589" s="33">
         <f t="shared" ref="T589" si="136">T586/(T586+T588)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="590" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B590" s="21" t="s">
+    <row r="590" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B590" s="23" t="s">
         <v>496</v>
       </c>
-      <c r="C590" s="29">
+      <c r="C590" s="31">
         <f>C586/(C586+C587)</f>
         <v>0.86111111111111116</v>
       </c>
-      <c r="D590" s="29">
+      <c r="D590" s="31">
         <f t="shared" ref="D590:K590" si="137">D586/(D586+D587)</f>
         <v>0.83116883116883122</v>
       </c>
-      <c r="E590" s="29">
+      <c r="E590" s="31">
         <f t="shared" si="137"/>
         <v>0.5061224489795918</v>
       </c>
-      <c r="F590" s="29">
+      <c r="F590" s="31">
         <v>0</v>
       </c>
-      <c r="G590" s="29">
+      <c r="G590" s="31">
         <f t="shared" si="137"/>
         <v>1.038961038961039E-2</v>
       </c>
       <c r="I590" s="5"/>
-      <c r="K590" s="37">
+      <c r="K590" s="50">
         <f t="shared" si="137"/>
         <v>0.97142857142857142</v>
       </c>
-      <c r="L590" s="37">
+      <c r="L590" s="39">
         <f t="shared" ref="L590:T590" si="138">L586/(L586+L587)</f>
         <v>0</v>
       </c>
-      <c r="M590" s="37">
+      <c r="M590" s="39">
         <f t="shared" si="138"/>
         <v>0.96883116883116882</v>
       </c>
-      <c r="N590" s="37">
+      <c r="N590" s="39">
         <f t="shared" si="138"/>
         <v>0.54025974025974022</v>
       </c>
-      <c r="O590" s="37">
+      <c r="O590" s="39">
         <f t="shared" si="138"/>
         <v>0.96883116883116882</v>
       </c>
-      <c r="P590" s="37">
+      <c r="P590" s="39">
         <f t="shared" si="138"/>
         <v>0.72467532467532469</v>
       </c>
-      <c r="Q590" s="37">
+      <c r="Q590" s="39">
         <f t="shared" si="138"/>
         <v>0.86769230769230765</v>
       </c>
-      <c r="R590" s="37">
+      <c r="R590" s="39">
         <f t="shared" si="138"/>
         <v>0.37230769230769228</v>
       </c>
-      <c r="S590" s="37">
+      <c r="S590" s="39">
         <f t="shared" si="138"/>
         <v>0.85974025974025969</v>
       </c>
-      <c r="T590" s="37">
+      <c r="T590" s="33">
         <f t="shared" si="138"/>
         <v>0.5688311688311688</v>
       </c>
     </row>
-    <row r="591" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B591" s="22" t="s">
+    <row r="591" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B591" s="24" t="s">
         <v>497</v>
       </c>
-      <c r="C591" s="32">
+      <c r="C591" s="34">
         <f>(2*C586)/((2*C586)+C588+C587)</f>
         <v>0.5591182364729459</v>
       </c>
-      <c r="D591" s="32">
+      <c r="D591" s="34">
         <f t="shared" ref="D591:K591" si="139">(2*D586)/((2*D586)+D588+D587)</f>
         <v>0.87431693989071035</v>
       </c>
-      <c r="E591" s="32">
+      <c r="E591" s="34">
         <f t="shared" si="139"/>
         <v>0.66846361185983827</v>
       </c>
-      <c r="F591" s="32">
+      <c r="F591" s="34">
         <v>0</v>
       </c>
-      <c r="G591" s="32">
+      <c r="G591" s="34">
         <f t="shared" si="139"/>
         <v>2.0512820512820513E-2</v>
       </c>
       <c r="H591" s="3"/>
       <c r="I591" s="6"/>
-      <c r="K591" s="37">
+      <c r="K591" s="51">
         <f t="shared" si="139"/>
         <v>0.63713798977853497</v>
       </c>
-      <c r="L591" s="37">
+      <c r="L591" s="34">
         <f t="shared" ref="L591:T591" si="140">(2*L586)/((2*L586)+L588+L587)</f>
         <v>0</v>
       </c>
-      <c r="M591" s="37">
+      <c r="M591" s="34">
         <f t="shared" si="140"/>
         <v>0.63760683760683756</v>
       </c>
-      <c r="N591" s="37">
+      <c r="N591" s="34">
         <f t="shared" si="140"/>
         <v>0.70151770657672852</v>
       </c>
-      <c r="O591" s="37">
+      <c r="O591" s="34">
         <f t="shared" si="140"/>
         <v>0.63760683760683756</v>
       </c>
-      <c r="P591" s="37">
+      <c r="P591" s="34">
         <f t="shared" si="140"/>
         <v>0.84036144578313254</v>
       </c>
-      <c r="Q591" s="37">
+      <c r="Q591" s="34">
         <f t="shared" si="140"/>
         <v>0.56231306081754739</v>
       </c>
-      <c r="R591" s="37">
+      <c r="R591" s="34">
         <f t="shared" si="140"/>
         <v>0.54260089686098656</v>
       </c>
-      <c r="S591" s="37">
+      <c r="S591" s="34">
         <f t="shared" si="140"/>
         <v>0.88859060402684564</v>
       </c>
-      <c r="T591" s="37">
+      <c r="T591" s="35">
         <f t="shared" si="140"/>
         <v>0.72516556291390732</v>
       </c>
     </row>
-    <row r="592" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B592" s="17"/>
-      <c r="C592" s="17"/>
-      <c r="D592" s="17"/>
-      <c r="E592" s="17"/>
-      <c r="F592" s="17"/>
-      <c r="G592" s="17"/>
-      <c r="H592" s="17"/>
-      <c r="I592" s="17"/>
-      <c r="K592" s="11"/>
-      <c r="L592" s="11"/>
-      <c r="M592" s="11"/>
-      <c r="N592" s="11"/>
-      <c r="O592" s="11"/>
-      <c r="P592" s="11"/>
-      <c r="Q592" s="11"/>
-      <c r="R592" s="11"/>
-      <c r="S592" s="11"/>
-      <c r="T592" s="11"/>
-    </row>
-    <row r="593" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B593" s="18" t="s">
+    <row r="592" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B592" s="11"/>
+      <c r="C592" s="11"/>
+      <c r="D592" s="11"/>
+      <c r="E592" s="11"/>
+      <c r="F592" s="11"/>
+      <c r="G592" s="11"/>
+      <c r="H592" s="11"/>
+      <c r="I592" s="11"/>
+      <c r="K592" s="13"/>
+      <c r="L592" s="13"/>
+      <c r="M592" s="13"/>
+      <c r="N592" s="13"/>
+      <c r="O592" s="13"/>
+      <c r="P592" s="13"/>
+      <c r="Q592" s="13"/>
+      <c r="R592" s="13"/>
+      <c r="S592" s="13"/>
+      <c r="T592" s="13"/>
+    </row>
+    <row r="593" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A593" s="41"/>
+      <c r="B593" s="42"/>
+      <c r="C593" s="42"/>
+      <c r="D593" s="42"/>
+      <c r="E593" s="42"/>
+      <c r="F593" s="42"/>
+      <c r="G593" s="42"/>
+      <c r="H593" s="42"/>
+      <c r="I593" s="42"/>
+      <c r="J593" s="42"/>
+      <c r="K593" s="42"/>
+      <c r="L593" s="42"/>
+      <c r="M593" s="42"/>
+      <c r="N593" s="42"/>
+      <c r="O593" s="42"/>
+      <c r="P593" s="42"/>
+      <c r="Q593" s="42"/>
+      <c r="R593" s="42"/>
+      <c r="S593" s="42"/>
+      <c r="T593" s="42"/>
+    </row>
+    <row r="594" spans="1:20" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B594" s="13"/>
+      <c r="C594" s="13"/>
+      <c r="D594" s="43"/>
+      <c r="E594" s="43"/>
+      <c r="F594" s="43"/>
+      <c r="G594" s="43"/>
+      <c r="H594" s="43"/>
+      <c r="I594" s="43"/>
+      <c r="J594" s="2"/>
+      <c r="K594" s="44" t="s">
+        <v>508</v>
+      </c>
+      <c r="L594" s="44"/>
+      <c r="M594" s="44" t="s">
+        <v>509</v>
+      </c>
+      <c r="N594" s="44"/>
+      <c r="O594" s="44" t="s">
+        <v>510</v>
+      </c>
+      <c r="P594" s="44"/>
+      <c r="Q594" s="44" t="s">
+        <v>511</v>
+      </c>
+      <c r="R594" s="44"/>
+      <c r="S594" s="13"/>
+      <c r="T594" s="13"/>
+    </row>
+    <row r="595" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A595" s="8"/>
+      <c r="B595" s="40"/>
+      <c r="C595" s="45"/>
+      <c r="D595" s="37" t="s">
+        <v>502</v>
+      </c>
+      <c r="E595" s="37"/>
+      <c r="F595" s="37"/>
+      <c r="G595" s="37"/>
+      <c r="H595" s="37" t="s">
+        <v>507</v>
+      </c>
+      <c r="I595" s="46" t="s">
+        <v>506</v>
+      </c>
+      <c r="J595" s="8"/>
+      <c r="K595" s="37" t="s">
+        <v>470</v>
+      </c>
+      <c r="L595" s="37" t="s">
+        <v>471</v>
+      </c>
+      <c r="M595" s="37" t="s">
+        <v>470</v>
+      </c>
+      <c r="N595" s="37" t="s">
+        <v>471</v>
+      </c>
+      <c r="O595" s="37" t="s">
+        <v>470</v>
+      </c>
+      <c r="P595" s="37" t="s">
+        <v>471</v>
+      </c>
+      <c r="Q595" s="37" t="s">
+        <v>470</v>
+      </c>
+      <c r="R595" s="37" t="s">
+        <v>471</v>
+      </c>
+      <c r="S595" s="13"/>
+      <c r="T595" s="13"/>
+    </row>
+    <row r="596" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B596" s="20" t="s">
         <v>489</v>
       </c>
-      <c r="C593" s="1"/>
-      <c r="D593" s="1">
-        <v>78</v>
-      </c>
-      <c r="E593" s="1"/>
-      <c r="F593" s="1"/>
-      <c r="G593" s="1"/>
-      <c r="H593" s="1">
+      <c r="C596" s="1"/>
+      <c r="D596" s="1">
+        <v>77</v>
+      </c>
+      <c r="E596" s="1"/>
+      <c r="F596" s="1"/>
+      <c r="G596" s="1"/>
+      <c r="H596" s="1">
         <v>90</v>
       </c>
-      <c r="I593" s="24">
-        <v>85</v>
-      </c>
-      <c r="K593" s="7">
+      <c r="I596" s="26">
+        <v>86</v>
+      </c>
+      <c r="K596" s="52">
         <v>131</v>
       </c>
-      <c r="L593" s="7">
+      <c r="L596" s="7">
         <v>52</v>
       </c>
-      <c r="M593" s="11"/>
-      <c r="N593" s="11"/>
-      <c r="O593" s="11"/>
-      <c r="P593" s="11"/>
-      <c r="Q593" s="11"/>
-      <c r="R593" s="11"/>
-      <c r="S593" s="11"/>
-      <c r="T593" s="11"/>
-    </row>
-    <row r="594" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B594" s="19" t="s">
+      <c r="M596" s="7">
+        <v>123</v>
+      </c>
+      <c r="N596" s="7">
+        <v>71</v>
+      </c>
+      <c r="O596" s="7">
+        <v>111</v>
+      </c>
+      <c r="P596" s="7">
+        <v>52</v>
+      </c>
+      <c r="Q596" s="7">
+        <v>123</v>
+      </c>
+      <c r="R596" s="7">
+        <v>79</v>
+      </c>
+      <c r="S596" s="23"/>
+      <c r="T596" s="13"/>
+    </row>
+    <row r="597" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B597" s="21" t="s">
         <v>486</v>
       </c>
-      <c r="C594" s="1"/>
-      <c r="D594" s="1">
+      <c r="C597" s="1"/>
+      <c r="D597" s="1">
         <v>72</v>
       </c>
-      <c r="E594" s="1"/>
-      <c r="F594" s="1"/>
-      <c r="G594" s="1"/>
-      <c r="H594" s="1">
-        <v>32</v>
-      </c>
-      <c r="I594" s="25">
-        <v>65</v>
-      </c>
-      <c r="K594" s="7">
+      <c r="E597" s="1"/>
+      <c r="F597" s="1"/>
+      <c r="G597" s="1"/>
+      <c r="H597" s="1">
+        <v>31</v>
+      </c>
+      <c r="I597" s="27">
+        <v>63</v>
+      </c>
+      <c r="K597" s="49">
         <v>18</v>
       </c>
-      <c r="L594" s="7">
+      <c r="L597" s="7">
         <v>97</v>
       </c>
-      <c r="M594" s="11"/>
-      <c r="N594" s="11"/>
-      <c r="O594" s="11"/>
-      <c r="P594" s="11"/>
-      <c r="Q594" s="11"/>
-      <c r="R594" s="11"/>
-      <c r="S594" s="11"/>
-      <c r="T594" s="11"/>
-    </row>
-    <row r="595" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B595" s="20" t="s">
+      <c r="M597" s="7">
+        <v>27</v>
+      </c>
+      <c r="N597" s="7">
+        <v>79</v>
+      </c>
+      <c r="O597" s="7">
+        <v>38</v>
+      </c>
+      <c r="P597" s="7">
+        <v>97</v>
+      </c>
+      <c r="Q597" s="7">
+        <v>26</v>
+      </c>
+      <c r="R597" s="7">
+        <v>70</v>
+      </c>
+      <c r="S597" s="23"/>
+      <c r="T597" s="13"/>
+    </row>
+    <row r="598" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B598" s="22" t="s">
         <v>482</v>
       </c>
-      <c r="C595" s="15"/>
-      <c r="D595" s="15">
+      <c r="C598" s="17"/>
+      <c r="D598" s="17">
         <v>22</v>
       </c>
-      <c r="E595" s="15"/>
-      <c r="F595" s="15"/>
-      <c r="G595" s="15"/>
-      <c r="H595" s="15">
-        <v>2</v>
-      </c>
-      <c r="I595" s="26">
+      <c r="E598" s="17"/>
+      <c r="F598" s="17"/>
+      <c r="G598" s="17"/>
+      <c r="H598" s="17">
+        <v>6</v>
+      </c>
+      <c r="I598" s="28">
+        <v>11</v>
+      </c>
+      <c r="K598" s="53">
+        <v>34</v>
+      </c>
+      <c r="L598" s="54">
+        <v>2</v>
+      </c>
+      <c r="M598" s="54">
+        <v>26</v>
+      </c>
+      <c r="N598" s="54">
+        <v>3</v>
+      </c>
+      <c r="O598" s="14">
+        <v>31</v>
+      </c>
+      <c r="P598" s="54">
+        <v>2</v>
+      </c>
+      <c r="Q598" s="14">
         <v>14</v>
       </c>
-      <c r="K595" s="11">
-        <v>34</v>
-      </c>
-      <c r="L595" s="7">
-        <v>2</v>
-      </c>
-      <c r="M595" s="7"/>
-      <c r="N595" s="7"/>
-      <c r="O595" s="11"/>
-      <c r="P595" s="7"/>
-      <c r="Q595" s="11"/>
-      <c r="R595" s="11"/>
-      <c r="S595" s="11"/>
-      <c r="T595" s="11"/>
-    </row>
-    <row r="596" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B596" s="19" t="s">
+      <c r="R598" s="15">
+        <v>3</v>
+      </c>
+      <c r="S598" s="23"/>
+      <c r="T598" s="13"/>
+    </row>
+    <row r="599" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B599" s="21" t="s">
         <v>498</v>
       </c>
-      <c r="C596" s="14"/>
-      <c r="D596" s="29">
-        <f>D593/(D593+D595)</f>
-        <v>0.78</v>
-      </c>
-      <c r="E596" s="29"/>
-      <c r="F596" s="29"/>
-      <c r="G596" s="29"/>
-      <c r="H596" s="29">
-        <f t="shared" ref="E596:K596" si="141">H593/(H593+H595)</f>
-        <v>0.97826086956521741</v>
-      </c>
-      <c r="I596" s="30">
+      <c r="C599" s="16"/>
+      <c r="D599" s="31">
+        <f>D596/(D596+D598)</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E599" s="31"/>
+      <c r="F599" s="31"/>
+      <c r="G599" s="31"/>
+      <c r="H599" s="31">
+        <f t="shared" ref="E599:K599" si="141">H596/(H596+H598)</f>
+        <v>0.9375</v>
+      </c>
+      <c r="I599" s="32">
         <f t="shared" si="141"/>
-        <v>0.85858585858585856</v>
-      </c>
-      <c r="K596" s="37">
+        <v>0.88659793814432986</v>
+      </c>
+      <c r="K599" s="50">
         <f t="shared" si="141"/>
         <v>0.79393939393939394</v>
       </c>
-      <c r="L596" s="37">
-        <f t="shared" ref="L596" si="142">L593/(L593+L595)</f>
+      <c r="L599" s="39">
+        <f t="shared" ref="L599" si="142">L596/(L596+L598)</f>
         <v>0.96296296296296291</v>
       </c>
-      <c r="M596" s="37"/>
-      <c r="N596" s="37"/>
-      <c r="O596" s="37"/>
-      <c r="P596" s="37"/>
-      <c r="Q596" s="37"/>
-      <c r="R596" s="37"/>
-      <c r="S596" s="37"/>
-      <c r="T596" s="37"/>
-    </row>
-    <row r="597" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B597" s="19" t="s">
+      <c r="M599" s="39">
+        <f t="shared" ref="M599" si="143">M596/(M596+M598)</f>
+        <v>0.82550335570469802</v>
+      </c>
+      <c r="N599" s="39">
+        <f t="shared" ref="N599" si="144">N596/(N596+N598)</f>
+        <v>0.95945945945945943</v>
+      </c>
+      <c r="O599" s="39">
+        <f t="shared" ref="O599" si="145">O596/(O596+O598)</f>
+        <v>0.78169014084507038</v>
+      </c>
+      <c r="P599" s="39">
+        <f t="shared" ref="P599" si="146">P596/(P596+P598)</f>
+        <v>0.96296296296296291</v>
+      </c>
+      <c r="Q599" s="39">
+        <f t="shared" ref="Q599" si="147">Q596/(Q596+Q598)</f>
+        <v>0.8978102189781022</v>
+      </c>
+      <c r="R599" s="39">
+        <f t="shared" ref="R599" si="148">R596/(R596+R598)</f>
+        <v>0.96341463414634143</v>
+      </c>
+      <c r="S599" s="50"/>
+      <c r="T599" s="39"/>
+    </row>
+    <row r="600" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B600" s="21" t="s">
         <v>499</v>
       </c>
-      <c r="C597" s="14"/>
-      <c r="D597" s="29">
-        <f>D593/(D593+D594)</f>
-        <v>0.52</v>
-      </c>
-      <c r="E597" s="29"/>
-      <c r="F597" s="29"/>
-      <c r="G597" s="29"/>
-      <c r="H597" s="29">
-        <f t="shared" ref="E597:K597" si="143">H593/(H593+H594)</f>
-        <v>0.73770491803278693</v>
-      </c>
-      <c r="I597" s="31">
-        <f t="shared" si="143"/>
-        <v>0.56666666666666665</v>
-      </c>
-      <c r="K597" s="37">
-        <f t="shared" si="143"/>
+      <c r="C600" s="16"/>
+      <c r="D600" s="31">
+        <f>D596/(D596+D597)</f>
+        <v>0.51677852348993292</v>
+      </c>
+      <c r="E600" s="31"/>
+      <c r="F600" s="31"/>
+      <c r="G600" s="31"/>
+      <c r="H600" s="31">
+        <f t="shared" ref="E600:K600" si="149">H596/(H596+H597)</f>
+        <v>0.74380165289256195</v>
+      </c>
+      <c r="I600" s="33">
+        <f t="shared" si="149"/>
+        <v>0.57718120805369133</v>
+      </c>
+      <c r="K600" s="50">
+        <f t="shared" si="149"/>
         <v>0.87919463087248317</v>
       </c>
-      <c r="L597" s="37">
-        <f t="shared" ref="L597:T597" si="144">L593/(L593+L594)</f>
+      <c r="L600" s="39">
+        <f t="shared" ref="L600:T600" si="150">L596/(L596+L597)</f>
         <v>0.34899328859060402</v>
       </c>
-      <c r="M597" s="37"/>
-      <c r="N597" s="37"/>
-      <c r="O597" s="37"/>
-      <c r="P597" s="37"/>
-      <c r="Q597" s="37"/>
-      <c r="R597" s="37"/>
-      <c r="S597" s="37"/>
-      <c r="T597" s="37"/>
-    </row>
-    <row r="598" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B598" s="23" t="s">
+      <c r="M600" s="39">
+        <f t="shared" ref="M600:R600" si="151">M596/(M596+M597)</f>
+        <v>0.82</v>
+      </c>
+      <c r="N600" s="39">
+        <f t="shared" si="151"/>
+        <v>0.47333333333333333</v>
+      </c>
+      <c r="O600" s="39">
+        <f t="shared" si="151"/>
+        <v>0.74496644295302017</v>
+      </c>
+      <c r="P600" s="39">
+        <f t="shared" si="151"/>
+        <v>0.34899328859060402</v>
+      </c>
+      <c r="Q600" s="39">
+        <f t="shared" si="151"/>
+        <v>0.82550335570469802</v>
+      </c>
+      <c r="R600" s="39">
+        <f t="shared" si="151"/>
+        <v>0.53020134228187921</v>
+      </c>
+      <c r="S600" s="50"/>
+      <c r="T600" s="39"/>
+    </row>
+    <row r="601" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B601" s="25" t="s">
         <v>500</v>
       </c>
-      <c r="C598" s="16"/>
-      <c r="D598" s="32">
-        <f>(2*D593)/((2*D593)+D595+D594)</f>
-        <v>0.624</v>
-      </c>
-      <c r="E598" s="32"/>
-      <c r="F598" s="32"/>
-      <c r="G598" s="32"/>
-      <c r="H598" s="32">
-        <f t="shared" ref="E598:K598" si="145">(2*H593)/((2*H593)+H595+H594)</f>
-        <v>0.84112149532710279</v>
-      </c>
-      <c r="I598" s="33">
-        <f t="shared" si="145"/>
-        <v>0.68273092369477917</v>
-      </c>
-      <c r="K598" s="37">
-        <f t="shared" si="145"/>
+      <c r="C601" s="18"/>
+      <c r="D601" s="34">
+        <f>(2*D596)/((2*D596)+D598+D597)</f>
+        <v>0.62096774193548387</v>
+      </c>
+      <c r="E601" s="34"/>
+      <c r="F601" s="34"/>
+      <c r="G601" s="34"/>
+      <c r="H601" s="34">
+        <f t="shared" ref="E601:K601" si="152">(2*H596)/((2*H596)+H598+H597)</f>
+        <v>0.82949308755760365</v>
+      </c>
+      <c r="I601" s="35">
+        <f t="shared" si="152"/>
+        <v>0.69918699186991873</v>
+      </c>
+      <c r="K601" s="51">
+        <f t="shared" si="152"/>
         <v>0.83439490445859876</v>
       </c>
-      <c r="L598" s="37">
-        <f t="shared" ref="L598:T598" si="146">(2*L593)/((2*L593)+L595+L594)</f>
+      <c r="L601" s="34">
+        <f t="shared" ref="L601:T601" si="153">(2*L596)/((2*L596)+L598+L597)</f>
         <v>0.51231527093596063</v>
       </c>
-      <c r="M598" s="37"/>
-      <c r="N598" s="37"/>
-      <c r="O598" s="37"/>
-      <c r="P598" s="37"/>
-      <c r="Q598" s="37"/>
-      <c r="R598" s="37"/>
-      <c r="S598" s="37"/>
-      <c r="T598" s="37"/>
-    </row>
-    <row r="599" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B599" s="11"/>
-      <c r="C599" s="11"/>
-      <c r="D599" s="11"/>
-      <c r="E599" s="11"/>
-      <c r="F599" s="11"/>
-      <c r="G599" s="11"/>
-      <c r="H599" s="11"/>
-      <c r="I599" s="11"/>
-    </row>
-    <row r="600" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B600" s="11"/>
-      <c r="C600" s="11"/>
-      <c r="D600" s="11"/>
-      <c r="E600" s="11"/>
-      <c r="F600" s="11"/>
-      <c r="G600" s="11"/>
-      <c r="H600" s="11"/>
-      <c r="I600" s="11"/>
+      <c r="M601" s="34">
+        <f t="shared" ref="M601:R601" si="154">(2*M596)/((2*M596)+M598+M597)</f>
+        <v>0.82274247491638797</v>
+      </c>
+      <c r="N601" s="34">
+        <f t="shared" si="154"/>
+        <v>0.6339285714285714</v>
+      </c>
+      <c r="O601" s="34">
+        <f t="shared" si="154"/>
+        <v>0.76288659793814428</v>
+      </c>
+      <c r="P601" s="34">
+        <f t="shared" si="154"/>
+        <v>0.51231527093596063</v>
+      </c>
+      <c r="Q601" s="34">
+        <f t="shared" si="154"/>
+        <v>0.8601398601398601</v>
+      </c>
+      <c r="R601" s="34">
+        <f t="shared" si="154"/>
+        <v>0.68398268398268403</v>
+      </c>
+      <c r="S601" s="50"/>
+      <c r="T601" s="39"/>
+    </row>
+    <row r="602" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B602" s="13"/>
+      <c r="C602" s="13"/>
+      <c r="D602" s="13"/>
+      <c r="E602" s="13"/>
+      <c r="F602" s="13"/>
+      <c r="G602" s="13"/>
+      <c r="H602" s="13"/>
+      <c r="I602" s="13"/>
+    </row>
+    <row r="603" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B603" s="13"/>
+      <c r="C603" s="13"/>
+      <c r="D603" s="13"/>
+      <c r="E603" s="13"/>
+      <c r="F603" s="13"/>
+      <c r="G603" s="13"/>
+      <c r="H603" s="13"/>
+      <c r="I603" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:T1"/>
+    <mergeCell ref="K594:L594"/>
+    <mergeCell ref="M594:N594"/>
+    <mergeCell ref="O594:P594"/>
+    <mergeCell ref="Q594:R594"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:I569">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="FP">

</xml_diff>

<commit_message>
data: add calculation of best possible combination of tools overall
</commit_message>
<xml_diff>
--- a/merged_results/complete_results.xlsx
+++ b/merged_results/complete_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/Documents/Own/Papers_and_Projects/comparison_ArchRec_tools/GitHub_SARbenchmarks/merged_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C205A821-5FE2-094D-BC68-5835C8899DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAAF6E2-2B25-7D46-BBA2-C4D1CA873FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" xr2:uid="{21E6DDBE-06EB-864D-8BE4-57F9A90E46C0}"/>
   </bookViews>
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3304" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3315" uniqueCount="517">
   <si>
     <t xml:space="preserve"> RAD</t>
   </si>
@@ -1818,6 +1818,21 @@
   </si>
   <si>
     <t>RAD + RAS</t>
+  </si>
+  <si>
+    <t>Best</t>
+  </si>
+  <si>
+    <t>Components: C2D</t>
+  </si>
+  <si>
+    <t>Connections: C2D + MDG OR</t>
+  </si>
+  <si>
+    <t>Endpoints: RAD + RAS OR</t>
+  </si>
+  <si>
+    <t>Sum</t>
   </si>
 </sst>
 </file>
@@ -1841,12 +1856,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -2009,7 +2030,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2017,6 +2038,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2052,7 +2074,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2086,6 +2108,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2486,11 +2515,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E181CEDB-9761-A944-9A62-062C9F034F3F}">
-  <dimension ref="A1:Y603"/>
+  <dimension ref="A1:Y617"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A580" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J601" sqref="J601"/>
+      <pane ySplit="2" topLeftCell="A590" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G610" sqref="G610"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2504,26 +2533,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="10" t="s">
         <v>469</v>
       </c>
-      <c r="L1" s="9"/>
+      <c r="L1" s="10"/>
       <c r="M1" s="2" t="s">
         <v>474</v>
       </c>
       <c r="N1" s="2"/>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9" t="s">
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10" t="s">
         <v>473</v>
       </c>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9" t="s">
+      <c r="R1" s="10"/>
+      <c r="S1" s="10" t="s">
         <v>475</v>
       </c>
-      <c r="T1" s="9"/>
+      <c r="T1" s="10"/>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
@@ -2533,55 +2562,55 @@
       <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="37" t="s">
         <v>501</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="37" t="s">
         <v>502</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="37" t="s">
         <v>503</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="37" t="s">
         <v>504</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="38" t="s">
         <v>505</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="39" t="s">
         <v>506</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="11" t="s">
         <v>470</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="11" t="s">
         <v>471</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="11" t="s">
         <v>470</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="11" t="s">
         <v>471</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="11" t="s">
         <v>470</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="P2" s="11" t="s">
         <v>471</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="Q2" s="11" t="s">
         <v>470</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="R2" s="11" t="s">
         <v>471</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="S2" s="11" t="s">
         <v>470</v>
       </c>
-      <c r="T2" s="10" t="s">
+      <c r="T2" s="11" t="s">
         <v>471</v>
       </c>
     </row>
@@ -2765,20 +2794,20 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="16"/>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
         <v>TP</v>
@@ -3994,22 +4023,22 @@
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H30" s="14"/>
-      <c r="I30" s="15"/>
+      <c r="C30" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="15"/>
+      <c r="I30" s="16"/>
       <c r="K30" t="str">
         <f t="shared" si="0"/>
         <v>TP</v>
@@ -4061,7 +4090,7 @@
       <c r="D31" t="s">
         <v>2</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="G31" s="14" t="s">
         <v>4</v>
       </c>
       <c r="I31" s="5" t="s">
@@ -4118,7 +4147,7 @@
       <c r="D32" t="s">
         <v>2</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="G32" s="14" t="s">
         <v>4</v>
       </c>
       <c r="I32" s="5" t="s">
@@ -7265,24 +7294,24 @@
       </c>
     </row>
     <row r="87" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B87" s="14" t="s">
+      <c r="B87" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C87" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D87" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E87" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F87" s="14"/>
-      <c r="G87" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H87" s="14"/>
-      <c r="I87" s="15"/>
+      <c r="C87" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E87" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F87" s="15"/>
+      <c r="G87" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H87" s="15"/>
+      <c r="I87" s="16"/>
       <c r="K87" t="str">
         <f t="shared" si="12"/>
         <v>TP</v>
@@ -7337,7 +7366,7 @@
       <c r="E88" t="s">
         <v>4</v>
       </c>
-      <c r="G88" s="13" t="s">
+      <c r="G88" s="14" t="s">
         <v>4</v>
       </c>
       <c r="H88" t="s">
@@ -7400,7 +7429,7 @@
       <c r="E89" t="s">
         <v>2</v>
       </c>
-      <c r="G89" s="13" t="s">
+      <c r="G89" s="14" t="s">
         <v>4</v>
       </c>
       <c r="H89" t="s">
@@ -9878,24 +9907,24 @@
       </c>
     </row>
     <row r="129" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B129" s="14" t="s">
+      <c r="B129" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C129" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D129" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E129" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F129" s="14"/>
-      <c r="G129" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H129" s="14"/>
-      <c r="I129" s="15"/>
+      <c r="C129" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D129" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E129" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F129" s="15"/>
+      <c r="G129" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H129" s="15"/>
+      <c r="I129" s="16"/>
       <c r="K129" t="str">
         <f t="shared" si="12"/>
         <v>TP</v>
@@ -9950,7 +9979,7 @@
       <c r="E130" t="s">
         <v>2</v>
       </c>
-      <c r="G130" s="13" t="s">
+      <c r="G130" s="14" t="s">
         <v>4</v>
       </c>
       <c r="H130" t="s">
@@ -10013,7 +10042,7 @@
       <c r="E131" t="s">
         <v>2</v>
       </c>
-      <c r="G131" s="13" t="s">
+      <c r="G131" s="14" t="s">
         <v>4</v>
       </c>
       <c r="H131" t="s">
@@ -11065,26 +11094,26 @@
       </c>
     </row>
     <row r="148" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B148" s="14" t="s">
+      <c r="B148" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="C148" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D148" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E148" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F148" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G148" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H148" s="14"/>
-      <c r="I148" s="15"/>
+      <c r="C148" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D148" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E148" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F148" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G148" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H148" s="15"/>
+      <c r="I148" s="16"/>
       <c r="K148" t="str">
         <f t="shared" si="22"/>
         <v>TP</v>
@@ -11139,7 +11168,7 @@
       <c r="E149" t="s">
         <v>2</v>
       </c>
-      <c r="G149" s="13" t="s">
+      <c r="G149" s="14" t="s">
         <v>4</v>
       </c>
       <c r="H149" t="s">
@@ -11202,7 +11231,7 @@
       <c r="E150" t="s">
         <v>4</v>
       </c>
-      <c r="G150" s="13" t="s">
+      <c r="G150" s="14" t="s">
         <v>4</v>
       </c>
       <c r="H150" t="s">
@@ -11265,7 +11294,7 @@
       <c r="E151" t="s">
         <v>4</v>
       </c>
-      <c r="G151" s="13" t="s">
+      <c r="G151" s="14" t="s">
         <v>4</v>
       </c>
       <c r="H151" t="s">
@@ -11328,7 +11357,7 @@
       <c r="E152" t="s">
         <v>2</v>
       </c>
-      <c r="G152" s="13" t="s">
+      <c r="G152" s="14" t="s">
         <v>4</v>
       </c>
       <c r="H152" t="s">
@@ -12622,26 +12651,26 @@
       </c>
     </row>
     <row r="173" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B173" s="14" t="s">
+      <c r="B173" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C173" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D173" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E173" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F173" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G173" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H173" s="14"/>
-      <c r="I173" s="15"/>
+      <c r="C173" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D173" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E173" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F173" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G173" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H173" s="15"/>
+      <c r="I173" s="16"/>
       <c r="K173" t="str">
         <f t="shared" si="22"/>
         <v>TP</v>
@@ -15242,24 +15271,24 @@
       </c>
     </row>
     <row r="217" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B217" s="14" t="s">
+      <c r="B217" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="C217" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D217" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E217" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F217" s="14"/>
-      <c r="G217" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H217" s="14"/>
-      <c r="I217" s="15"/>
+      <c r="C217" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D217" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E217" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F217" s="15"/>
+      <c r="G217" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H217" s="15"/>
+      <c r="I217" s="16"/>
       <c r="K217" t="str">
         <f t="shared" si="32"/>
         <v>TP</v>
@@ -18377,24 +18406,24 @@
       </c>
     </row>
     <row r="268" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B268" s="14" t="s">
+      <c r="B268" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C268" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D268" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E268" s="14"/>
-      <c r="F268" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G268" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H268" s="14"/>
-      <c r="I268" s="15"/>
+      <c r="C268" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D268" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E268" s="15"/>
+      <c r="F268" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G268" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H268" s="15"/>
+      <c r="I268" s="16"/>
       <c r="K268" t="str">
         <f t="shared" si="42"/>
         <v>TP</v>
@@ -20971,20 +21000,20 @@
       </c>
     </row>
     <row r="313" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B313" s="14" t="s">
+      <c r="B313" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="C313" s="14"/>
-      <c r="D313" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E313" s="14"/>
-      <c r="F313" s="14"/>
-      <c r="G313" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H313" s="14"/>
-      <c r="I313" s="15"/>
+      <c r="C313" s="15"/>
+      <c r="D313" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E313" s="15"/>
+      <c r="F313" s="15"/>
+      <c r="G313" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H313" s="15"/>
+      <c r="I313" s="16"/>
       <c r="K313" t="str">
         <f t="shared" si="42"/>
         <v>TP</v>
@@ -21839,20 +21868,20 @@
       </c>
     </row>
     <row r="331" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B331" s="14" t="s">
+      <c r="B331" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="C331" s="14"/>
-      <c r="D331" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E331" s="14"/>
-      <c r="F331" s="14"/>
-      <c r="G331" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="H331" s="14"/>
-      <c r="I331" s="15"/>
+      <c r="C331" s="15"/>
+      <c r="D331" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E331" s="15"/>
+      <c r="F331" s="15"/>
+      <c r="G331" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H331" s="15"/>
+      <c r="I331" s="16"/>
       <c r="K331" t="str">
         <f t="shared" si="52"/>
         <v>TP</v>
@@ -22768,24 +22797,24 @@
       </c>
     </row>
     <row r="348" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B348" s="14" t="s">
+      <c r="B348" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C348" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D348" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E348" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F348" s="14"/>
-      <c r="G348" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H348" s="14"/>
-      <c r="I348" s="15"/>
+      <c r="C348" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D348" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E348" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F348" s="15"/>
+      <c r="G348" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H348" s="15"/>
+      <c r="I348" s="16"/>
       <c r="K348" t="str">
         <f t="shared" si="52"/>
         <v>TP</v>
@@ -24834,20 +24863,20 @@
       </c>
     </row>
     <row r="385" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B385" s="14" t="s">
+      <c r="B385" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C385" s="14"/>
-      <c r="D385" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E385" s="14"/>
-      <c r="F385" s="14"/>
-      <c r="G385" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H385" s="14"/>
-      <c r="I385" s="15"/>
+      <c r="C385" s="15"/>
+      <c r="D385" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E385" s="15"/>
+      <c r="F385" s="15"/>
+      <c r="G385" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H385" s="15"/>
+      <c r="I385" s="16"/>
       <c r="K385" t="str">
         <f t="shared" si="52"/>
         <v>TP</v>
@@ -26293,24 +26322,24 @@
       </c>
     </row>
     <row r="413" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B413" s="14" t="s">
+      <c r="B413" s="15" t="s">
         <v>352</v>
       </c>
-      <c r="C413" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D413" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E413" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F413" s="14"/>
-      <c r="G413" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H413" s="14"/>
-      <c r="I413" s="15"/>
+      <c r="C413" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D413" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E413" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F413" s="15"/>
+      <c r="G413" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H413" s="15"/>
+      <c r="I413" s="16"/>
       <c r="K413" t="str">
         <f t="shared" si="62"/>
         <v>TP</v>
@@ -28679,24 +28708,24 @@
       </c>
     </row>
     <row r="453" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B453" s="14" t="s">
+      <c r="B453" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C453" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D453" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E453" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F453" s="14"/>
-      <c r="G453" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H453" s="14"/>
-      <c r="I453" s="15"/>
+      <c r="C453" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D453" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E453" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F453" s="15"/>
+      <c r="G453" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H453" s="15"/>
+      <c r="I453" s="16"/>
       <c r="K453" t="str">
         <f t="shared" si="72"/>
         <v>TP</v>
@@ -30927,26 +30956,26 @@
       </c>
     </row>
     <row r="489" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B489" s="14" t="s">
+      <c r="B489" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C489" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D489" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E489" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F489" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G489" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H489" s="14"/>
-      <c r="I489" s="15"/>
+      <c r="C489" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D489" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E489" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F489" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G489" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H489" s="15"/>
+      <c r="I489" s="16"/>
       <c r="K489" t="str">
         <f t="shared" si="72"/>
         <v>TP</v>
@@ -33134,22 +33163,22 @@
       </c>
     </row>
     <row r="526" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B526" s="14" t="s">
+      <c r="B526" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C526" s="14"/>
-      <c r="D526" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E526" s="14"/>
-      <c r="F526" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G526" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H526" s="14"/>
-      <c r="I526" s="15"/>
+      <c r="C526" s="15"/>
+      <c r="D526" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E526" s="15"/>
+      <c r="F526" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G526" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H526" s="15"/>
+      <c r="I526" s="16"/>
       <c r="K526" t="str">
         <f t="shared" si="82"/>
         <v>TP</v>
@@ -34545,24 +34574,24 @@
       </c>
     </row>
     <row r="553" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B553" s="14" t="s">
+      <c r="B553" s="15" t="s">
         <v>452</v>
       </c>
-      <c r="C553" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D553" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E553" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F553" s="14"/>
-      <c r="G553" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H553" s="14"/>
-      <c r="I553" s="15"/>
+      <c r="C553" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D553" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E553" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F553" s="15"/>
+      <c r="G553" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H553" s="15"/>
+      <c r="I553" s="16"/>
       <c r="K553" t="str">
         <f t="shared" si="82"/>
         <v>TP</v>
@@ -35615,457 +35644,457 @@
       </c>
     </row>
     <row r="572" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B572" s="20" t="s">
+      <c r="B572" s="21" t="s">
         <v>476</v>
       </c>
-      <c r="C572" s="12">
+      <c r="C572" s="13">
         <f>COUNTIF(C3:C569, " TP") + C596</f>
         <v>402</v>
       </c>
-      <c r="D572" s="12">
+      <c r="D572" s="13">
         <f t="shared" ref="D572:I572" si="92">COUNTIF(D3:D569, " TP") + D596</f>
         <v>575</v>
       </c>
-      <c r="E572" s="12">
+      <c r="E572" s="13">
         <f t="shared" si="92"/>
         <v>208</v>
       </c>
-      <c r="F572" s="12">
+      <c r="F572" s="13">
         <f t="shared" si="92"/>
         <v>32</v>
       </c>
-      <c r="G572" s="12">
+      <c r="G572" s="13">
         <f t="shared" si="92"/>
         <v>31</v>
       </c>
-      <c r="H572" s="12">
+      <c r="H572" s="13">
         <f t="shared" si="92"/>
         <v>90</v>
       </c>
-      <c r="I572" s="26">
+      <c r="I572" s="27">
         <f t="shared" si="92"/>
         <v>93</v>
       </c>
-      <c r="K572" s="47">
+      <c r="K572" s="48">
         <f>COUNTIF(K3:K569, "TP") + K596</f>
         <v>684</v>
       </c>
-      <c r="L572" s="11">
+      <c r="L572" s="12">
         <f>COUNTIF(L3:L569, "TP") + L596</f>
         <v>76</v>
       </c>
-      <c r="M572" s="11">
+      <c r="M572" s="12">
         <f t="shared" ref="L572:S572" si="93">COUNTIF(M3:M569, "TP")</f>
         <v>552</v>
       </c>
-      <c r="N572" s="11">
+      <c r="N572" s="12">
         <f t="shared" si="93"/>
         <v>353</v>
       </c>
-      <c r="O572" s="11">
+      <c r="O572" s="12">
         <f t="shared" si="93"/>
         <v>552</v>
       </c>
-      <c r="P572" s="11">
+      <c r="P572" s="12">
         <f t="shared" si="93"/>
         <v>437</v>
       </c>
-      <c r="Q572" s="11">
+      <c r="Q572" s="12">
         <f t="shared" si="93"/>
         <v>407</v>
       </c>
-      <c r="R572" s="11">
+      <c r="R572" s="12">
         <f t="shared" si="93"/>
         <v>203</v>
       </c>
-      <c r="S572" s="11">
+      <c r="S572" s="12">
         <f t="shared" si="93"/>
         <v>509</v>
       </c>
-      <c r="T572" s="48">
+      <c r="T572" s="49">
         <f>COUNTIF(T3:T569, "TP")</f>
         <v>372</v>
       </c>
     </row>
     <row r="573" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B573" s="21" t="s">
+      <c r="B573" s="22" t="s">
         <v>477</v>
       </c>
-      <c r="C573" s="16">
+      <c r="C573" s="17">
         <f>COUNTIF(C3:C569, " FN") + C597</f>
         <v>66</v>
       </c>
-      <c r="D573" s="16">
+      <c r="D573" s="17">
         <f t="shared" ref="D573:I573" si="94">COUNTIF(D3:D569, " FN") + D597</f>
         <v>141</v>
       </c>
-      <c r="E573" s="16">
+      <c r="E573" s="17">
         <f t="shared" si="94"/>
         <v>147</v>
       </c>
-      <c r="F573" s="16">
+      <c r="F573" s="17">
         <f t="shared" si="94"/>
         <v>25</v>
       </c>
-      <c r="G573" s="16">
+      <c r="G573" s="17">
         <f t="shared" si="94"/>
         <v>536</v>
       </c>
-      <c r="H573" s="16">
+      <c r="H573" s="17">
         <f t="shared" si="94"/>
         <v>290</v>
       </c>
-      <c r="I573" s="27">
+      <c r="I573" s="28">
         <f t="shared" si="94"/>
         <v>441</v>
       </c>
-      <c r="K573" s="21">
+      <c r="K573" s="22">
         <f>COUNTIF(K3:K569, "FN") + K597</f>
         <v>32</v>
       </c>
-      <c r="L573" s="16">
+      <c r="L573" s="17">
         <f>COUNTIF(L3:L569, "FN") + L597</f>
         <v>640</v>
       </c>
-      <c r="M573" s="16">
+      <c r="M573" s="17">
         <f t="shared" ref="L573:T573" si="95">COUNTIF(M3:M569, "FN")</f>
         <v>15</v>
       </c>
-      <c r="N573" s="16">
+      <c r="N573" s="17">
         <f t="shared" si="95"/>
         <v>214</v>
       </c>
-      <c r="O573" s="16">
+      <c r="O573" s="17">
         <f t="shared" si="95"/>
         <v>15</v>
       </c>
-      <c r="P573" s="16">
+      <c r="P573" s="17">
         <f t="shared" si="95"/>
         <v>130</v>
       </c>
-      <c r="Q573" s="16">
+      <c r="Q573" s="17">
         <f t="shared" si="95"/>
         <v>62</v>
       </c>
-      <c r="R573" s="16">
+      <c r="R573" s="17">
         <f t="shared" si="95"/>
         <v>266</v>
       </c>
-      <c r="S573" s="16">
+      <c r="S573" s="17">
         <f>COUNTIF(S3:S569, "FN")</f>
         <v>58</v>
       </c>
-      <c r="T573" s="27">
+      <c r="T573" s="28">
         <f t="shared" si="95"/>
         <v>195</v>
       </c>
     </row>
     <row r="574" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B574" s="22" t="s">
+      <c r="B574" s="23" t="s">
         <v>480</v>
       </c>
-      <c r="C574" s="17">
+      <c r="C574" s="18">
         <v>436</v>
       </c>
-      <c r="D574" s="17">
+      <c r="D574" s="18">
         <v>54</v>
       </c>
-      <c r="E574" s="17">
-        <v>2</v>
-      </c>
-      <c r="F574" s="17">
+      <c r="E574" s="18">
+        <v>2</v>
+      </c>
+      <c r="F574" s="18">
         <v>1</v>
       </c>
-      <c r="G574" s="17">
+      <c r="G574" s="18">
         <v>22</v>
       </c>
-      <c r="H574" s="17">
-        <v>2</v>
-      </c>
-      <c r="I574" s="28">
+      <c r="H574" s="18">
+        <v>2</v>
+      </c>
+      <c r="I574" s="29">
         <v>16</v>
       </c>
-      <c r="J574" s="13"/>
-      <c r="K574" s="55">
+      <c r="J574" s="14"/>
+      <c r="K574" s="56">
         <f>K581+K588+K598</f>
         <v>517</v>
       </c>
-      <c r="L574" s="54">
-        <v>2</v>
-      </c>
-      <c r="M574" s="54">
+      <c r="L574" s="55">
+        <v>2</v>
+      </c>
+      <c r="M574" s="55">
         <f>M581+M588</f>
         <v>458</v>
       </c>
-      <c r="N574" s="54">
+      <c r="N574" s="55">
         <v>0</v>
       </c>
-      <c r="O574" s="54">
+      <c r="O574" s="55">
         <f>O581+O588</f>
         <v>458</v>
       </c>
-      <c r="P574" s="54">
+      <c r="P574" s="55">
         <v>0</v>
       </c>
-      <c r="Q574" s="54">
+      <c r="Q574" s="55">
         <f>Q581+Q588</f>
         <v>437</v>
       </c>
-      <c r="R574" s="54">
+      <c r="R574" s="55">
         <v>0</v>
       </c>
-      <c r="S574" s="54">
+      <c r="S574" s="55">
         <f>S581+S588</f>
         <v>34</v>
       </c>
-      <c r="T574" s="15">
+      <c r="T574" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="575" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B575" s="23" t="s">
+      <c r="B575" s="24" t="s">
         <v>478</v>
       </c>
-      <c r="C575" s="31">
+      <c r="C575" s="32">
         <f>C572/(C572+C574)</f>
         <v>0.47971360381861577</v>
       </c>
-      <c r="D575" s="31">
+      <c r="D575" s="32">
         <f t="shared" ref="D575:I575" si="96">D572/(D572+D574)</f>
         <v>0.91414944356120831</v>
       </c>
-      <c r="E575" s="31">
+      <c r="E575" s="32">
         <f t="shared" si="96"/>
         <v>0.99047619047619051</v>
       </c>
-      <c r="F575" s="31">
+      <c r="F575" s="32">
         <f t="shared" si="96"/>
         <v>0.96969696969696972</v>
       </c>
-      <c r="G575" s="31">
+      <c r="G575" s="32">
         <f t="shared" si="96"/>
         <v>0.58490566037735847</v>
       </c>
-      <c r="H575" s="31">
+      <c r="H575" s="32">
         <f t="shared" si="96"/>
         <v>0.97826086956521741</v>
       </c>
-      <c r="I575" s="32">
+      <c r="I575" s="33">
         <f t="shared" si="96"/>
         <v>0.85321100917431192</v>
       </c>
-      <c r="J575" s="39"/>
-      <c r="K575" s="50">
+      <c r="J575" s="40"/>
+      <c r="K575" s="51">
         <f>K572/(K572+K574)</f>
         <v>0.56952539550374692</v>
       </c>
-      <c r="L575" s="39">
+      <c r="L575" s="40">
         <f t="shared" ref="L575" si="97">L572/(L572+L574)</f>
         <v>0.97435897435897434</v>
       </c>
-      <c r="M575" s="39">
+      <c r="M575" s="40">
         <f t="shared" ref="M575" si="98">M572/(M572+M574)</f>
         <v>0.54653465346534658</v>
       </c>
-      <c r="N575" s="39">
+      <c r="N575" s="40">
         <f t="shared" ref="N575" si="99">N572/(N572+N574)</f>
         <v>1</v>
       </c>
-      <c r="O575" s="39">
+      <c r="O575" s="40">
         <f t="shared" ref="O575" si="100">O572/(O572+O574)</f>
         <v>0.54653465346534658</v>
       </c>
-      <c r="P575" s="39">
+      <c r="P575" s="40">
         <f t="shared" ref="P575" si="101">P572/(P572+P574)</f>
         <v>1</v>
       </c>
-      <c r="Q575" s="39">
+      <c r="Q575" s="40">
         <f t="shared" ref="Q575" si="102">Q572/(Q572+Q574)</f>
         <v>0.48222748815165878</v>
       </c>
-      <c r="R575" s="39">
+      <c r="R575" s="40">
         <f t="shared" ref="R575" si="103">R572/(R572+R574)</f>
         <v>1</v>
       </c>
-      <c r="S575" s="39">
+      <c r="S575" s="40">
         <f>S572/(S572+S574)</f>
         <v>0.93738489871086561</v>
       </c>
-      <c r="T575" s="33">
+      <c r="T575" s="34">
         <f t="shared" ref="T575" si="104">T572/(T572+T574)</f>
         <v>1</v>
       </c>
     </row>
     <row r="576" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B576" s="23" t="s">
+      <c r="B576" s="24" t="s">
         <v>479</v>
       </c>
-      <c r="C576" s="31">
+      <c r="C576" s="32">
         <f>C572/(C572+C573)</f>
         <v>0.85897435897435892</v>
       </c>
-      <c r="D576" s="31">
+      <c r="D576" s="32">
         <f>D572/(D572+D573)</f>
         <v>0.80307262569832405</v>
       </c>
-      <c r="E576" s="31">
+      <c r="E576" s="32">
         <f>E572/(E572+E573)</f>
         <v>0.58591549295774648</v>
       </c>
-      <c r="F576" s="31">
+      <c r="F576" s="32">
         <f>F572/(F572+F573)</f>
         <v>0.56140350877192979</v>
       </c>
-      <c r="G576" s="31">
+      <c r="G576" s="32">
         <f>G572/(G572+G573)</f>
         <v>5.4673721340388004E-2</v>
       </c>
-      <c r="H576" s="31">
+      <c r="H576" s="32">
         <f>H572/(H572+H573)</f>
         <v>0.23684210526315788</v>
       </c>
-      <c r="I576" s="33">
+      <c r="I576" s="34">
         <f>I572/(I572+I573)</f>
         <v>0.17415730337078653</v>
       </c>
-      <c r="J576" s="39"/>
-      <c r="K576" s="50">
+      <c r="J576" s="40"/>
+      <c r="K576" s="51">
         <f t="shared" ref="J576:T576" si="105">K572/(K572+K573)</f>
         <v>0.95530726256983245</v>
       </c>
-      <c r="L576" s="39">
+      <c r="L576" s="40">
         <f t="shared" si="105"/>
         <v>0.10614525139664804</v>
       </c>
-      <c r="M576" s="39">
+      <c r="M576" s="40">
         <f t="shared" si="105"/>
         <v>0.97354497354497349</v>
       </c>
-      <c r="N576" s="39">
+      <c r="N576" s="40">
         <f t="shared" si="105"/>
         <v>0.62257495590828926</v>
       </c>
-      <c r="O576" s="39">
+      <c r="O576" s="40">
         <f t="shared" si="105"/>
         <v>0.97354497354497349</v>
       </c>
-      <c r="P576" s="39">
+      <c r="P576" s="40">
         <f t="shared" si="105"/>
         <v>0.7707231040564374</v>
       </c>
-      <c r="Q576" s="39">
+      <c r="Q576" s="40">
         <f t="shared" si="105"/>
         <v>0.86780383795309168</v>
       </c>
-      <c r="R576" s="39">
+      <c r="R576" s="40">
         <f t="shared" si="105"/>
         <v>0.43283582089552236</v>
       </c>
-      <c r="S576" s="39">
+      <c r="S576" s="40">
         <f t="shared" si="105"/>
         <v>0.89770723104056438</v>
       </c>
-      <c r="T576" s="33">
+      <c r="T576" s="34">
         <f t="shared" si="105"/>
         <v>0.65608465608465605</v>
       </c>
     </row>
     <row r="577" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B577" s="24" t="s">
+      <c r="B577" s="25" t="s">
         <v>491</v>
       </c>
-      <c r="C577" s="34">
+      <c r="C577" s="35">
         <f>(2*C572)/((2*C572)+C574+C573)</f>
         <v>0.61562021439509951</v>
       </c>
-      <c r="D577" s="34">
+      <c r="D577" s="35">
         <f>(2*D572)/((2*D572)+D574+D573)</f>
         <v>0.85501858736059477</v>
       </c>
-      <c r="E577" s="34">
+      <c r="E577" s="35">
         <f t="shared" ref="D577:I577" si="106">(2*E572)/((2*E572)+E574+E573)</f>
         <v>0.73628318584070795</v>
       </c>
-      <c r="F577" s="34">
+      <c r="F577" s="35">
         <f t="shared" si="106"/>
         <v>0.71111111111111114</v>
       </c>
-      <c r="G577" s="34">
+      <c r="G577" s="35">
         <f t="shared" si="106"/>
         <v>0.1</v>
       </c>
-      <c r="H577" s="34">
+      <c r="H577" s="35">
         <f t="shared" si="106"/>
         <v>0.38135593220338981</v>
       </c>
-      <c r="I577" s="35">
+      <c r="I577" s="36">
         <f t="shared" si="106"/>
         <v>0.28926905132192848</v>
       </c>
-      <c r="J577" s="39"/>
-      <c r="K577" s="51">
+      <c r="J577" s="40"/>
+      <c r="K577" s="52">
         <f t="shared" ref="J577:T577" si="107">(2*K572)/((2*K572)+K574+K573)</f>
         <v>0.71361502347417838</v>
       </c>
-      <c r="L577" s="34">
+      <c r="L577" s="35">
         <f t="shared" si="107"/>
         <v>0.19143576826196473</v>
       </c>
-      <c r="M577" s="34">
+      <c r="M577" s="35">
         <f t="shared" si="107"/>
         <v>0.70006341154090046</v>
       </c>
-      <c r="N577" s="34">
+      <c r="N577" s="35">
         <f t="shared" si="107"/>
         <v>0.7673913043478261</v>
       </c>
-      <c r="O577" s="34">
+      <c r="O577" s="35">
         <f t="shared" si="107"/>
         <v>0.70006341154090046</v>
       </c>
-      <c r="P577" s="34">
+      <c r="P577" s="35">
         <f t="shared" si="107"/>
         <v>0.87051792828685259</v>
       </c>
-      <c r="Q577" s="34">
+      <c r="Q577" s="35">
         <f t="shared" si="107"/>
         <v>0.61995430312262001</v>
       </c>
-      <c r="R577" s="34">
+      <c r="R577" s="35">
         <f t="shared" si="107"/>
         <v>0.60416666666666663</v>
       </c>
-      <c r="S577" s="34">
+      <c r="S577" s="35">
         <f t="shared" si="107"/>
         <v>0.91711711711711708</v>
       </c>
-      <c r="T577" s="35">
+      <c r="T577" s="36">
         <f t="shared" si="107"/>
         <v>0.792332268370607</v>
       </c>
     </row>
     <row r="578" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B578" s="19"/>
-      <c r="C578" s="19"/>
-      <c r="D578" s="19"/>
-      <c r="E578" s="19"/>
-      <c r="F578" s="19"/>
-      <c r="G578" s="19"/>
-      <c r="H578" s="19"/>
-      <c r="I578" s="19"/>
-      <c r="K578" s="19"/>
-      <c r="L578" s="19"/>
-      <c r="M578" s="19"/>
-      <c r="N578" s="19"/>
-      <c r="O578" s="19"/>
-      <c r="P578" s="19"/>
-      <c r="Q578" s="19"/>
-      <c r="R578" s="19"/>
-      <c r="S578" s="19"/>
-      <c r="T578" s="19"/>
+      <c r="B578" s="20"/>
+      <c r="C578" s="20"/>
+      <c r="D578" s="20"/>
+      <c r="E578" s="20"/>
+      <c r="F578" s="20"/>
+      <c r="G578" s="20"/>
+      <c r="H578" s="20"/>
+      <c r="I578" s="20"/>
+      <c r="K578" s="20"/>
+      <c r="L578" s="20"/>
+      <c r="M578" s="20"/>
+      <c r="N578" s="20"/>
+      <c r="O578" s="20"/>
+      <c r="P578" s="20"/>
+      <c r="Q578" s="20"/>
+      <c r="R578" s="20"/>
+      <c r="S578" s="20"/>
+      <c r="T578" s="20"/>
     </row>
     <row r="579" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B579" s="20" t="s">
+      <c r="B579" s="21" t="s">
         <v>487</v>
       </c>
       <c r="C579" s="1">
@@ -36089,50 +36118,50 @@
         <v>27</v>
       </c>
       <c r="H579" s="1"/>
-      <c r="I579" s="26"/>
-      <c r="K579" s="21">
+      <c r="I579" s="27"/>
+      <c r="K579" s="22">
         <f>COUNTIF(K3:K7, "TP") + COUNTIF(K14:K30, "TP") + COUNTIF(K73:K87, "TP") + COUNTIF(K122:K129, "TP") + COUNTIF(K142:K148, "TP") + COUNTIF(K162:K173, "TP") + COUNTIF(K203:K217, "TP") + COUNTIF(K252:K268, "TP") + COUNTIF(K306:K313, "TP") + COUNTIF(K327:K331, "TP") + COUNTIF(K338:K348, "TP") + COUNTIF(K375:K385, "TP") + COUNTIF(K404:K413, "TP") + COUNTIF(K443:K453, "TP") + COUNTIF(K478:K489, "TP") + COUNTIF(K518:K526, "TP") + COUNTIF(K545:K553, "TP")</f>
         <v>179</v>
       </c>
-      <c r="L579" s="16">
+      <c r="L579" s="17">
         <f t="shared" ref="L579:T579" si="108">COUNTIF(L3:L7, "TP") + COUNTIF(L14:L30, "TP") + COUNTIF(L73:L87, "TP") + COUNTIF(L122:L129, "TP") + COUNTIF(L142:L148, "TP") + COUNTIF(L162:L173, "TP") + COUNTIF(L203:L217, "TP") + COUNTIF(L252:L268, "TP") + COUNTIF(L306:L313, "TP") + COUNTIF(L327:L331, "TP") + COUNTIF(L338:L348, "TP") + COUNTIF(L375:L385, "TP") + COUNTIF(L404:L413, "TP") + COUNTIF(L443:L453, "TP") + COUNTIF(L478:L489, "TP") + COUNTIF(L518:L526, "TP") + COUNTIF(L545:L553, "TP")</f>
         <v>24</v>
       </c>
-      <c r="M579" s="16">
+      <c r="M579" s="17">
         <f t="shared" si="108"/>
         <v>179</v>
       </c>
-      <c r="N579" s="16">
+      <c r="N579" s="17">
         <f t="shared" si="108"/>
         <v>145</v>
       </c>
-      <c r="O579" s="16">
+      <c r="O579" s="17">
         <f t="shared" si="108"/>
         <v>179</v>
       </c>
-      <c r="P579" s="16">
+      <c r="P579" s="17">
         <f t="shared" si="108"/>
         <v>158</v>
       </c>
-      <c r="Q579" s="16">
+      <c r="Q579" s="17">
         <f t="shared" si="108"/>
         <v>125</v>
       </c>
-      <c r="R579" s="16">
+      <c r="R579" s="17">
         <f t="shared" si="108"/>
         <v>82</v>
       </c>
-      <c r="S579" s="16">
+      <c r="S579" s="17">
         <f t="shared" si="108"/>
         <v>178</v>
       </c>
-      <c r="T579" s="27">
+      <c r="T579" s="28">
         <f t="shared" si="108"/>
         <v>153</v>
       </c>
     </row>
     <row r="580" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B580" s="21" t="s">
+      <c r="B580" s="22" t="s">
         <v>484</v>
       </c>
       <c r="C580" s="1">
@@ -36156,322 +36185,322 @@
         <v>155</v>
       </c>
       <c r="H580" s="1"/>
-      <c r="I580" s="27"/>
-      <c r="K580" s="21">
+      <c r="I580" s="28"/>
+      <c r="K580" s="22">
         <f>COUNTIF(K3:K7, "FN") + COUNTIF(K14:K30, "FN") + COUNTIF(K73:K87, "FN") + COUNTIF(K122:K129, "FN") + COUNTIF(K142:K148, "FN") + COUNTIF(K162:K173, "FN") + COUNTIF(K203:K217, "FN") + COUNTIF(K252:K268, "FN") + COUNTIF(K306:K313, "FN") + COUNTIF(K327:K331, "FN") + COUNTIF(K338:K348, "FN") + COUNTIF(K375:K385, "FN") + COUNTIF(K404:K413, "FN") + COUNTIF(K443:K453, "FN") + COUNTIF(K478:K489, "FN") + COUNTIF(K518:K526, "FN") + COUNTIF(K545:K553, "FN")</f>
         <v>3</v>
       </c>
-      <c r="L580" s="16">
+      <c r="L580" s="17">
         <f t="shared" ref="L580:T580" si="109">COUNTIF(L3:L7, "FN") + COUNTIF(L14:L30, "FN") + COUNTIF(L73:L87, "FN") + COUNTIF(L122:L129, "FN") + COUNTIF(L142:L148, "FN") + COUNTIF(L162:L173, "FN") + COUNTIF(L203:L217, "FN") + COUNTIF(L252:L268, "FN") + COUNTIF(L306:L313, "FN") + COUNTIF(L327:L331, "FN") + COUNTIF(L338:L348, "FN") + COUNTIF(L375:L385, "FN") + COUNTIF(L404:L413, "FN") + COUNTIF(L443:L453, "FN") + COUNTIF(L478:L489, "FN") + COUNTIF(L518:L526, "FN") + COUNTIF(L545:L553, "FN")</f>
         <v>158</v>
       </c>
-      <c r="M580" s="16">
+      <c r="M580" s="17">
         <f t="shared" si="109"/>
         <v>3</v>
       </c>
-      <c r="N580" s="16">
+      <c r="N580" s="17">
         <f t="shared" si="109"/>
         <v>37</v>
       </c>
-      <c r="O580" s="16">
+      <c r="O580" s="17">
         <f t="shared" si="109"/>
         <v>3</v>
       </c>
-      <c r="P580" s="16">
+      <c r="P580" s="17">
         <f t="shared" si="109"/>
         <v>24</v>
       </c>
-      <c r="Q580" s="16">
+      <c r="Q580" s="17">
         <f t="shared" si="109"/>
         <v>19</v>
       </c>
-      <c r="R580" s="16">
+      <c r="R580" s="17">
         <f t="shared" si="109"/>
         <v>62</v>
       </c>
-      <c r="S580" s="16">
+      <c r="S580" s="17">
         <f t="shared" si="109"/>
         <v>4</v>
       </c>
-      <c r="T580" s="27">
+      <c r="T580" s="28">
         <f t="shared" si="109"/>
         <v>29</v>
       </c>
     </row>
     <row r="581" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B581" s="22" t="s">
+      <c r="B581" s="23" t="s">
         <v>481</v>
       </c>
-      <c r="C581" s="17">
+      <c r="C581" s="18">
         <v>41</v>
       </c>
-      <c r="D581" s="17">
+      <c r="D581" s="18">
         <v>5</v>
       </c>
-      <c r="E581" s="17">
+      <c r="E581" s="18">
         <v>0</v>
       </c>
-      <c r="F581" s="17">
+      <c r="F581" s="18">
         <v>1</v>
       </c>
-      <c r="G581" s="17">
+      <c r="G581" s="18">
         <v>21</v>
       </c>
-      <c r="H581" s="17"/>
-      <c r="I581" s="28"/>
-      <c r="K581" s="53">
+      <c r="H581" s="18"/>
+      <c r="I581" s="29"/>
+      <c r="K581" s="54">
         <v>68</v>
       </c>
-      <c r="L581" s="14">
+      <c r="L581" s="15">
         <v>0</v>
       </c>
-      <c r="M581" s="14">
+      <c r="M581" s="15">
         <v>46</v>
       </c>
-      <c r="N581" s="14">
+      <c r="N581" s="15">
         <v>0</v>
       </c>
-      <c r="O581" s="54">
+      <c r="O581" s="55">
         <v>46</v>
       </c>
-      <c r="P581" s="54">
+      <c r="P581" s="55">
         <v>0</v>
       </c>
-      <c r="Q581" s="54">
+      <c r="Q581" s="55">
         <v>41</v>
       </c>
-      <c r="R581" s="14">
+      <c r="R581" s="15">
         <v>0</v>
       </c>
-      <c r="S581" s="54">
+      <c r="S581" s="55">
         <v>5</v>
       </c>
-      <c r="T581" s="15">
+      <c r="T581" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="582" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B582" s="21" t="s">
+      <c r="B582" s="22" t="s">
         <v>493</v>
       </c>
-      <c r="C582" s="31">
+      <c r="C582" s="32">
         <f>C579/(C579+C581)</f>
         <v>0.75</v>
       </c>
-      <c r="D582" s="31">
+      <c r="D582" s="32">
         <f t="shared" ref="D582:G582" si="110">D579/(D579+D581)</f>
         <v>0.97267759562841527</v>
       </c>
-      <c r="E582" s="31">
+      <c r="E582" s="32">
         <f t="shared" si="110"/>
         <v>1</v>
       </c>
-      <c r="F582" s="31">
+      <c r="F582" s="32">
         <f t="shared" si="110"/>
         <v>0.96969696969696972</v>
       </c>
-      <c r="G582" s="31">
+      <c r="G582" s="32">
         <f t="shared" si="110"/>
         <v>0.5625</v>
       </c>
-      <c r="H582" s="16"/>
-      <c r="I582" s="27"/>
-      <c r="K582" s="50">
+      <c r="H582" s="17"/>
+      <c r="I582" s="28"/>
+      <c r="K582" s="51">
         <f t="shared" ref="K582" si="111">K579/(K579+K581)</f>
         <v>0.7246963562753036</v>
       </c>
-      <c r="L582" s="39">
+      <c r="L582" s="40">
         <f t="shared" ref="L582" si="112">L579/(L579+L581)</f>
         <v>1</v>
       </c>
-      <c r="M582" s="39">
+      <c r="M582" s="40">
         <f t="shared" ref="M582" si="113">M579/(M579+M581)</f>
         <v>0.79555555555555557</v>
       </c>
-      <c r="N582" s="39">
+      <c r="N582" s="40">
         <f t="shared" ref="N582" si="114">N579/(N579+N581)</f>
         <v>1</v>
       </c>
-      <c r="O582" s="39">
+      <c r="O582" s="40">
         <f t="shared" ref="O582" si="115">O579/(O579+O581)</f>
         <v>0.79555555555555557</v>
       </c>
-      <c r="P582" s="39">
+      <c r="P582" s="40">
         <f t="shared" ref="P582" si="116">P579/(P579+P581)</f>
         <v>1</v>
       </c>
-      <c r="Q582" s="39">
+      <c r="Q582" s="40">
         <f t="shared" ref="Q582" si="117">Q579/(Q579+Q581)</f>
         <v>0.75301204819277112</v>
       </c>
-      <c r="R582" s="39">
+      <c r="R582" s="40">
         <f t="shared" ref="R582" si="118">R579/(R579+R581)</f>
         <v>1</v>
       </c>
-      <c r="S582" s="39">
+      <c r="S582" s="40">
         <f t="shared" ref="S582" si="119">S579/(S579+S581)</f>
         <v>0.97267759562841527</v>
       </c>
-      <c r="T582" s="33">
+      <c r="T582" s="34">
         <f t="shared" ref="T582" si="120">T579/(T579+T581)</f>
         <v>1</v>
       </c>
     </row>
     <row r="583" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B583" s="21" t="s">
+      <c r="B583" s="22" t="s">
         <v>492</v>
       </c>
-      <c r="C583" s="31">
+      <c r="C583" s="32">
         <f>C579/(C579+C580)</f>
         <v>0.85416666666666663</v>
       </c>
-      <c r="D583" s="31">
+      <c r="D583" s="32">
         <f t="shared" ref="D583:I583" si="121">D579/(D579+D580)</f>
         <v>0.97802197802197799</v>
       </c>
-      <c r="E583" s="31">
+      <c r="E583" s="32">
         <f t="shared" si="121"/>
         <v>0.76363636363636367</v>
       </c>
-      <c r="F583" s="31">
+      <c r="F583" s="32">
         <f t="shared" si="121"/>
         <v>0.56140350877192979</v>
       </c>
-      <c r="G583" s="31">
+      <c r="G583" s="32">
         <f>G579/(G579+G580)</f>
         <v>0.14835164835164835</v>
       </c>
       <c r="I583" s="5"/>
-      <c r="K583" s="50">
+      <c r="K583" s="51">
         <f>K579/(K579+K580)</f>
         <v>0.98351648351648346</v>
       </c>
-      <c r="L583" s="39">
+      <c r="L583" s="40">
         <f>L579/(L579+L580)</f>
         <v>0.13186813186813187</v>
       </c>
-      <c r="M583" s="39">
+      <c r="M583" s="40">
         <f t="shared" ref="L583:T583" si="122">M579/(M579+M580)</f>
         <v>0.98351648351648346</v>
       </c>
-      <c r="N583" s="39">
+      <c r="N583" s="40">
         <f t="shared" si="122"/>
         <v>0.79670329670329665</v>
       </c>
-      <c r="O583" s="39">
+      <c r="O583" s="40">
         <f t="shared" si="122"/>
         <v>0.98351648351648346</v>
       </c>
-      <c r="P583" s="39">
+      <c r="P583" s="40">
         <f t="shared" si="122"/>
         <v>0.86813186813186816</v>
       </c>
-      <c r="Q583" s="39">
+      <c r="Q583" s="40">
         <f t="shared" si="122"/>
         <v>0.86805555555555558</v>
       </c>
-      <c r="R583" s="39">
+      <c r="R583" s="40">
         <f t="shared" si="122"/>
         <v>0.56944444444444442</v>
       </c>
-      <c r="S583" s="39">
+      <c r="S583" s="40">
         <f t="shared" si="122"/>
         <v>0.97802197802197799</v>
       </c>
-      <c r="T583" s="33">
+      <c r="T583" s="34">
         <f t="shared" si="122"/>
         <v>0.84065934065934067</v>
       </c>
     </row>
     <row r="584" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B584" s="25" t="s">
+      <c r="B584" s="26" t="s">
         <v>494</v>
       </c>
-      <c r="C584" s="34">
+      <c r="C584" s="35">
         <f>(2*C579)/((2*C579)+C581+C580)</f>
         <v>0.79870129870129869</v>
       </c>
-      <c r="D584" s="34">
+      <c r="D584" s="35">
         <f t="shared" ref="D584:G584" si="123">(2*D579)/((2*D579)+D581+D580)</f>
         <v>0.97534246575342465</v>
       </c>
-      <c r="E584" s="34">
+      <c r="E584" s="35">
         <f t="shared" si="123"/>
         <v>0.865979381443299</v>
       </c>
-      <c r="F584" s="34">
+      <c r="F584" s="35">
         <f t="shared" si="123"/>
         <v>0.71111111111111114</v>
       </c>
-      <c r="G584" s="34">
+      <c r="G584" s="35">
         <f t="shared" si="123"/>
         <v>0.23478260869565218</v>
       </c>
-      <c r="H584" s="18"/>
-      <c r="I584" s="29"/>
-      <c r="K584" s="51">
+      <c r="H584" s="19"/>
+      <c r="I584" s="30"/>
+      <c r="K584" s="52">
         <f t="shared" ref="K584:T584" si="124">(2*K579)/((2*K579)+K581+K580)</f>
         <v>0.83449883449883455</v>
       </c>
-      <c r="L584" s="34">
+      <c r="L584" s="35">
         <f t="shared" si="124"/>
         <v>0.23300970873786409</v>
       </c>
-      <c r="M584" s="34">
+      <c r="M584" s="35">
         <f>(2*M579)/((2*M579)+M581+M580)</f>
         <v>0.87960687960687955</v>
       </c>
-      <c r="N584" s="34">
+      <c r="N584" s="35">
         <f t="shared" si="124"/>
         <v>0.88685015290519875</v>
       </c>
-      <c r="O584" s="34">
+      <c r="O584" s="35">
         <f t="shared" si="124"/>
         <v>0.87960687960687955</v>
       </c>
-      <c r="P584" s="34">
+      <c r="P584" s="35">
         <f t="shared" si="124"/>
         <v>0.92941176470588238</v>
       </c>
-      <c r="Q584" s="34">
+      <c r="Q584" s="35">
         <f t="shared" si="124"/>
         <v>0.80645161290322576</v>
       </c>
-      <c r="R584" s="34">
+      <c r="R584" s="35">
         <f t="shared" si="124"/>
         <v>0.72566371681415931</v>
       </c>
-      <c r="S584" s="34">
+      <c r="S584" s="35">
         <f t="shared" si="124"/>
         <v>0.97534246575342465</v>
       </c>
-      <c r="T584" s="35">
+      <c r="T584" s="36">
         <f t="shared" si="124"/>
         <v>0.91343283582089552</v>
       </c>
     </row>
     <row r="585" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B585" s="19"/>
-      <c r="C585" s="19"/>
-      <c r="D585" s="19"/>
-      <c r="E585" s="19"/>
-      <c r="F585" s="19"/>
-      <c r="G585" s="19"/>
-      <c r="H585" s="19"/>
-      <c r="I585" s="19"/>
-      <c r="K585" s="19"/>
-      <c r="L585" s="19"/>
-      <c r="M585" s="19"/>
-      <c r="N585" s="19"/>
-      <c r="O585" s="19"/>
-      <c r="P585" s="19"/>
-      <c r="Q585" s="19"/>
-      <c r="R585" s="19"/>
-      <c r="S585" s="19"/>
-      <c r="T585" s="19"/>
+      <c r="B585" s="20"/>
+      <c r="C585" s="20"/>
+      <c r="D585" s="20"/>
+      <c r="E585" s="20"/>
+      <c r="F585" s="20"/>
+      <c r="G585" s="20"/>
+      <c r="H585" s="20"/>
+      <c r="I585" s="20"/>
+      <c r="K585" s="20"/>
+      <c r="L585" s="20"/>
+      <c r="M585" s="20"/>
+      <c r="N585" s="20"/>
+      <c r="O585" s="20"/>
+      <c r="P585" s="20"/>
+      <c r="Q585" s="20"/>
+      <c r="R585" s="20"/>
+      <c r="S585" s="20"/>
+      <c r="T585" s="20"/>
     </row>
     <row r="586" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B586" s="20" t="s">
+      <c r="B586" s="21" t="s">
         <v>488</v>
       </c>
       <c r="C586" s="1">
@@ -36492,53 +36521,53 @@
         <v>4</v>
       </c>
       <c r="H586" s="1"/>
-      <c r="I586" s="26">
+      <c r="I586" s="27">
         <f>COUNTIF(I554:I569, " TP") + COUNTIF(I527:I544, " TP") + COUNTIF(I490:I517, " TP") + COUNTIF(I454:I477, " TP") + COUNTIF(I414:I442, " TP") + COUNTIF(I386:I403, " TP") + COUNTIF(I349:I374, " TP") + COUNTIF(I332:I337, " TP") + COUNTIF(I314:I326, " TP") + COUNTIF(I269:I305, " TP") + COUNTIF(I218:I251, " TP") + COUNTIF(I174:I202, " TP") + COUNTIF(I149:I161, " TP") + COUNTIF(I130:I141, " TP") + COUNTIF(I88:I121, " TP") + COUNTIF(I31:I72, " TP") + COUNTIF(I8:I13, " TP")</f>
         <v>7</v>
       </c>
-      <c r="K586" s="21">
+      <c r="K586" s="22">
         <f>COUNTIF(K554:K569, "TP") + COUNTIF(K527:K544, "TP") + COUNTIF(K490:K517, "TP") + COUNTIF(K454:K477, "TP") + COUNTIF(K414:K442, "TP") + COUNTIF(K386:K403, "TP") + COUNTIF(K349:K374, "TP") + COUNTIF(K332:K337, "TP") + COUNTIF(K314:K326, "TP") + COUNTIF(K269:K305, "TP") + COUNTIF(K218:K251, "TP") + COUNTIF(K174:K202, "TP") + COUNTIF(K149:K161, "TP") + COUNTIF(K130:K141, "TP") + COUNTIF(K88:K121, "TP") + COUNTIF(K31:K72, "TP") + COUNTIF(K8:K13, "TP")</f>
         <v>374</v>
       </c>
-      <c r="L586" s="16">
+      <c r="L586" s="17">
         <f t="shared" ref="L586:T586" si="125">COUNTIF(L554:L569, "TP") + COUNTIF(L527:L544, "TP") + COUNTIF(L490:L517, "TP") + COUNTIF(L454:L477, "TP") + COUNTIF(L414:L442, "TP") + COUNTIF(L386:L403, "TP") + COUNTIF(L349:L374, "TP") + COUNTIF(L332:L337, "TP") + COUNTIF(L314:L326, "TP") + COUNTIF(L269:L305, "TP") + COUNTIF(L218:L251, "TP") + COUNTIF(L174:L202, "TP") + COUNTIF(L149:L161, "TP") + COUNTIF(L130:L141, "TP") + COUNTIF(L88:L121, "TP") + COUNTIF(L31:L72, "TP") + COUNTIF(L8:L13, "TP")</f>
         <v>0</v>
       </c>
-      <c r="M586" s="16">
+      <c r="M586" s="17">
         <f t="shared" si="125"/>
         <v>373</v>
       </c>
-      <c r="N586" s="16">
+      <c r="N586" s="17">
         <f t="shared" si="125"/>
         <v>208</v>
       </c>
-      <c r="O586" s="16">
+      <c r="O586" s="17">
         <f t="shared" si="125"/>
         <v>373</v>
       </c>
-      <c r="P586" s="16">
+      <c r="P586" s="17">
         <f t="shared" si="125"/>
         <v>279</v>
       </c>
-      <c r="Q586" s="16">
+      <c r="Q586" s="17">
         <f t="shared" si="125"/>
         <v>282</v>
       </c>
-      <c r="R586" s="16">
+      <c r="R586" s="17">
         <f t="shared" si="125"/>
         <v>121</v>
       </c>
-      <c r="S586" s="16">
+      <c r="S586" s="17">
         <f t="shared" si="125"/>
         <v>331</v>
       </c>
-      <c r="T586" s="27">
+      <c r="T586" s="28">
         <f t="shared" si="125"/>
         <v>219</v>
       </c>
     </row>
     <row r="587" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B587" s="21" t="s">
+      <c r="B587" s="22" t="s">
         <v>485</v>
       </c>
       <c r="C587" s="1">
@@ -36562,416 +36591,416 @@
         <f>COUNTIF(H554:H569, " FN") + COUNTIF(H527:H544, " FN") + COUNTIF(H490:H517, " FN") + COUNTIF(H454:H477, " FN") + COUNTIF(H414:H442, " FN") + COUNTIF(H386:H403, " FN") + COUNTIF(H349:H374, " FN") + COUNTIF(H332:H337, " FN") + COUNTIF(H314:H326, " FN") + COUNTIF(H269:H305, " FN") + COUNTIF(H218:H251, " FN") + COUNTIF(H174:H202, " FN") + COUNTIF(H149:H161, " FN") + COUNTIF(H130:H141, " FN") + COUNTIF(H88:H121, " FN") + COUNTIF(H31:H72, " FN") + COUNTIF(H8:H13, " FN")</f>
         <v>259</v>
       </c>
-      <c r="I587" s="27">
+      <c r="I587" s="28">
         <f>COUNTIF(I554:I569, " FN") + COUNTIF(I527:I544, " FN") + COUNTIF(I490:I517, " FN") + COUNTIF(I454:I477, " FN") + COUNTIF(I414:I442, " FN") + COUNTIF(I386:I403, " FN") + COUNTIF(I349:I374, " FN") + COUNTIF(I332:I337, " FN") + COUNTIF(I314:I326, " FN") + COUNTIF(I269:I305, " FN") + COUNTIF(I218:I251, " FN") + COUNTIF(I174:I202, " FN") + COUNTIF(I149:I161, " FN") + COUNTIF(I130:I141, " FN") + COUNTIF(I88:I121, " FN") + COUNTIF(I31:I72, " FN") + COUNTIF(I8:I13, " FN")</f>
         <v>378</v>
       </c>
-      <c r="K587" s="21">
+      <c r="K587" s="22">
         <f>COUNTIF(K554:K569, "FN") + COUNTIF(K527:K544, "FN") + COUNTIF(K490:K517, "FN") + COUNTIF(K454:K477, "FN") + COUNTIF(K414:K442, "FN") + COUNTIF(K386:K403, "FN") + COUNTIF(K349:K374, "FN") + COUNTIF(K332:K337, "FN") + COUNTIF(K314:K326, "FN") + COUNTIF(K269:K305, "FN") + COUNTIF(K218:K251, "FN") + COUNTIF(K174:K202, "FN") + COUNTIF(K149:K161, "FN") + COUNTIF(K130:K141, "FN") + COUNTIF(K88:K121, "FN") + COUNTIF(K31:K72, "FN") + COUNTIF(K8:K13, "FN")</f>
         <v>11</v>
       </c>
-      <c r="L587" s="16">
+      <c r="L587" s="17">
         <f t="shared" ref="L587:T587" si="126">COUNTIF(L554:L569, "FN") + COUNTIF(L527:L544, "FN") + COUNTIF(L490:L517, "FN") + COUNTIF(L454:L477, "FN") + COUNTIF(L414:L442, "FN") + COUNTIF(L386:L403, "FN") + COUNTIF(L349:L374, "FN") + COUNTIF(L332:L337, "FN") + COUNTIF(L314:L326, "FN") + COUNTIF(L269:L305, "FN") + COUNTIF(L218:L251, "FN") + COUNTIF(L174:L202, "FN") + COUNTIF(L149:L161, "FN") + COUNTIF(L130:L141, "FN") + COUNTIF(L88:L121, "FN") + COUNTIF(L31:L72, "FN") + COUNTIF(L8:L13, "FN")</f>
         <v>385</v>
       </c>
-      <c r="M587" s="16">
+      <c r="M587" s="17">
         <f t="shared" si="126"/>
         <v>12</v>
       </c>
-      <c r="N587" s="16">
+      <c r="N587" s="17">
         <f t="shared" si="126"/>
         <v>177</v>
       </c>
-      <c r="O587" s="16">
+      <c r="O587" s="17">
         <f t="shared" si="126"/>
         <v>12</v>
       </c>
-      <c r="P587" s="16">
+      <c r="P587" s="17">
         <f t="shared" si="126"/>
         <v>106</v>
       </c>
-      <c r="Q587" s="16">
+      <c r="Q587" s="17">
         <f t="shared" si="126"/>
         <v>43</v>
       </c>
-      <c r="R587" s="16">
+      <c r="R587" s="17">
         <f t="shared" si="126"/>
         <v>204</v>
       </c>
-      <c r="S587" s="16">
+      <c r="S587" s="17">
         <f t="shared" si="126"/>
         <v>54</v>
       </c>
-      <c r="T587" s="27">
+      <c r="T587" s="28">
         <f t="shared" si="126"/>
         <v>166</v>
       </c>
     </row>
     <row r="588" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B588" s="22" t="s">
+      <c r="B588" s="23" t="s">
         <v>483</v>
       </c>
-      <c r="C588" s="17">
+      <c r="C588" s="18">
         <v>395</v>
       </c>
-      <c r="D588" s="17">
+      <c r="D588" s="18">
         <v>27</v>
       </c>
-      <c r="E588" s="17">
-        <v>2</v>
-      </c>
-      <c r="F588" s="17"/>
-      <c r="G588" s="17">
+      <c r="E588" s="18">
+        <v>2</v>
+      </c>
+      <c r="F588" s="18"/>
+      <c r="G588" s="18">
         <v>1</v>
       </c>
-      <c r="H588" s="17"/>
-      <c r="I588" s="28">
-        <v>2</v>
-      </c>
-      <c r="K588" s="53">
+      <c r="H588" s="18"/>
+      <c r="I588" s="29">
+        <v>2</v>
+      </c>
+      <c r="K588" s="54">
         <v>415</v>
       </c>
-      <c r="L588" s="14">
+      <c r="L588" s="15">
         <v>0</v>
       </c>
-      <c r="M588" s="54">
+      <c r="M588" s="55">
         <v>412</v>
       </c>
-      <c r="N588" s="14">
+      <c r="N588" s="15">
         <v>0</v>
       </c>
-      <c r="O588" s="54">
+      <c r="O588" s="55">
         <v>412</v>
       </c>
-      <c r="P588" s="14">
+      <c r="P588" s="15">
         <v>0</v>
       </c>
-      <c r="Q588" s="54">
+      <c r="Q588" s="55">
         <v>396</v>
       </c>
-      <c r="R588" s="14">
+      <c r="R588" s="15">
         <v>0</v>
       </c>
-      <c r="S588" s="54">
+      <c r="S588" s="55">
         <v>29</v>
       </c>
-      <c r="T588" s="15">
+      <c r="T588" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="589" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B589" s="23" t="s">
+      <c r="B589" s="24" t="s">
         <v>495</v>
       </c>
-      <c r="C589" s="31">
+      <c r="C589" s="32">
         <f>C586/(C586+C588)</f>
         <v>0.41394658753709201</v>
       </c>
-      <c r="D589" s="31">
+      <c r="D589" s="32">
         <f t="shared" ref="D589:K589" si="127">D586/(D586+D588)</f>
         <v>0.9221902017291066</v>
       </c>
-      <c r="E589" s="31">
+      <c r="E589" s="32">
         <f t="shared" si="127"/>
         <v>0.98412698412698407</v>
       </c>
-      <c r="F589" s="31">
+      <c r="F589" s="32">
         <v>0</v>
       </c>
-      <c r="G589" s="31">
+      <c r="G589" s="32">
         <f t="shared" si="127"/>
         <v>0.8</v>
       </c>
-      <c r="I589" s="30"/>
-      <c r="K589" s="50">
+      <c r="I589" s="31"/>
+      <c r="K589" s="51">
         <f t="shared" si="127"/>
         <v>0.47401774397972118</v>
       </c>
-      <c r="L589" s="39" t="e">
+      <c r="L589" s="40" t="e">
         <f t="shared" ref="L589" si="128">L586/(L586+L588)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M589" s="39">
+      <c r="M589" s="40">
         <f t="shared" ref="M589" si="129">M586/(M586+M588)</f>
         <v>0.47515923566878981</v>
       </c>
-      <c r="N589" s="39">
+      <c r="N589" s="40">
         <f t="shared" ref="N589" si="130">N586/(N586+N588)</f>
         <v>1</v>
       </c>
-      <c r="O589" s="39">
+      <c r="O589" s="40">
         <f t="shared" ref="O589" si="131">O586/(O586+O588)</f>
         <v>0.47515923566878981</v>
       </c>
-      <c r="P589" s="39">
+      <c r="P589" s="40">
         <f t="shared" ref="P589" si="132">P586/(P586+P588)</f>
         <v>1</v>
       </c>
-      <c r="Q589" s="39">
+      <c r="Q589" s="40">
         <f t="shared" ref="Q589" si="133">Q586/(Q586+Q588)</f>
         <v>0.41592920353982299</v>
       </c>
-      <c r="R589" s="39">
+      <c r="R589" s="40">
         <f t="shared" ref="R589" si="134">R586/(R586+R588)</f>
         <v>1</v>
       </c>
-      <c r="S589" s="39">
+      <c r="S589" s="40">
         <f t="shared" ref="S589" si="135">S586/(S586+S588)</f>
         <v>0.9194444444444444</v>
       </c>
-      <c r="T589" s="33">
+      <c r="T589" s="34">
         <f t="shared" ref="T589" si="136">T586/(T586+T588)</f>
         <v>1</v>
       </c>
     </row>
     <row r="590" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B590" s="23" t="s">
+      <c r="B590" s="24" t="s">
         <v>496</v>
       </c>
-      <c r="C590" s="31">
+      <c r="C590" s="32">
         <f>C586/(C586+C587)</f>
         <v>0.86111111111111116</v>
       </c>
-      <c r="D590" s="31">
+      <c r="D590" s="32">
         <f t="shared" ref="D590:K590" si="137">D586/(D586+D587)</f>
         <v>0.83116883116883122</v>
       </c>
-      <c r="E590" s="31">
+      <c r="E590" s="32">
         <f t="shared" si="137"/>
         <v>0.5061224489795918</v>
       </c>
-      <c r="F590" s="31">
+      <c r="F590" s="32">
         <v>0</v>
       </c>
-      <c r="G590" s="31">
+      <c r="G590" s="32">
         <f t="shared" si="137"/>
         <v>1.038961038961039E-2</v>
       </c>
       <c r="I590" s="5"/>
-      <c r="K590" s="50">
+      <c r="K590" s="51">
         <f t="shared" si="137"/>
         <v>0.97142857142857142</v>
       </c>
-      <c r="L590" s="39">
+      <c r="L590" s="40">
         <f t="shared" ref="L590:T590" si="138">L586/(L586+L587)</f>
         <v>0</v>
       </c>
-      <c r="M590" s="39">
+      <c r="M590" s="40">
         <f t="shared" si="138"/>
         <v>0.96883116883116882</v>
       </c>
-      <c r="N590" s="39">
+      <c r="N590" s="40">
         <f t="shared" si="138"/>
         <v>0.54025974025974022</v>
       </c>
-      <c r="O590" s="39">
+      <c r="O590" s="40">
         <f t="shared" si="138"/>
         <v>0.96883116883116882</v>
       </c>
-      <c r="P590" s="39">
+      <c r="P590" s="40">
         <f t="shared" si="138"/>
         <v>0.72467532467532469</v>
       </c>
-      <c r="Q590" s="39">
+      <c r="Q590" s="40">
         <f t="shared" si="138"/>
         <v>0.86769230769230765</v>
       </c>
-      <c r="R590" s="39">
+      <c r="R590" s="40">
         <f t="shared" si="138"/>
         <v>0.37230769230769228</v>
       </c>
-      <c r="S590" s="39">
+      <c r="S590" s="40">
         <f t="shared" si="138"/>
         <v>0.85974025974025969</v>
       </c>
-      <c r="T590" s="33">
+      <c r="T590" s="34">
         <f t="shared" si="138"/>
         <v>0.5688311688311688</v>
       </c>
     </row>
     <row r="591" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B591" s="24" t="s">
+      <c r="B591" s="25" t="s">
         <v>497</v>
       </c>
-      <c r="C591" s="34">
+      <c r="C591" s="35">
         <f>(2*C586)/((2*C586)+C588+C587)</f>
         <v>0.5591182364729459</v>
       </c>
-      <c r="D591" s="34">
+      <c r="D591" s="35">
         <f t="shared" ref="D591:K591" si="139">(2*D586)/((2*D586)+D588+D587)</f>
         <v>0.87431693989071035</v>
       </c>
-      <c r="E591" s="34">
+      <c r="E591" s="35">
         <f t="shared" si="139"/>
         <v>0.66846361185983827</v>
       </c>
-      <c r="F591" s="34">
+      <c r="F591" s="35">
         <v>0</v>
       </c>
-      <c r="G591" s="34">
+      <c r="G591" s="35">
         <f t="shared" si="139"/>
         <v>2.0512820512820513E-2</v>
       </c>
       <c r="H591" s="3"/>
       <c r="I591" s="6"/>
-      <c r="K591" s="51">
+      <c r="K591" s="52">
         <f t="shared" si="139"/>
         <v>0.63713798977853497</v>
       </c>
-      <c r="L591" s="34">
+      <c r="L591" s="35">
         <f t="shared" ref="L591:T591" si="140">(2*L586)/((2*L586)+L588+L587)</f>
         <v>0</v>
       </c>
-      <c r="M591" s="34">
+      <c r="M591" s="35">
         <f t="shared" si="140"/>
         <v>0.63760683760683756</v>
       </c>
-      <c r="N591" s="34">
+      <c r="N591" s="35">
         <f t="shared" si="140"/>
         <v>0.70151770657672852</v>
       </c>
-      <c r="O591" s="34">
+      <c r="O591" s="35">
         <f t="shared" si="140"/>
         <v>0.63760683760683756</v>
       </c>
-      <c r="P591" s="34">
+      <c r="P591" s="35">
         <f t="shared" si="140"/>
         <v>0.84036144578313254</v>
       </c>
-      <c r="Q591" s="34">
+      <c r="Q591" s="35">
         <f t="shared" si="140"/>
         <v>0.56231306081754739</v>
       </c>
-      <c r="R591" s="34">
+      <c r="R591" s="35">
         <f t="shared" si="140"/>
         <v>0.54260089686098656</v>
       </c>
-      <c r="S591" s="34">
+      <c r="S591" s="35">
         <f t="shared" si="140"/>
         <v>0.88859060402684564</v>
       </c>
-      <c r="T591" s="35">
+      <c r="T591" s="36">
         <f t="shared" si="140"/>
         <v>0.72516556291390732</v>
       </c>
     </row>
     <row r="592" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B592" s="11"/>
-      <c r="C592" s="11"/>
-      <c r="D592" s="11"/>
-      <c r="E592" s="11"/>
-      <c r="F592" s="11"/>
-      <c r="G592" s="11"/>
-      <c r="H592" s="11"/>
-      <c r="I592" s="11"/>
-      <c r="K592" s="13"/>
-      <c r="L592" s="13"/>
-      <c r="M592" s="13"/>
-      <c r="N592" s="13"/>
-      <c r="O592" s="13"/>
-      <c r="P592" s="13"/>
-      <c r="Q592" s="13"/>
-      <c r="R592" s="13"/>
-      <c r="S592" s="13"/>
-      <c r="T592" s="13"/>
+      <c r="B592" s="12"/>
+      <c r="C592" s="12"/>
+      <c r="D592" s="12"/>
+      <c r="E592" s="12"/>
+      <c r="F592" s="12"/>
+      <c r="G592" s="12"/>
+      <c r="H592" s="12"/>
+      <c r="I592" s="12"/>
+      <c r="K592" s="14"/>
+      <c r="L592" s="14"/>
+      <c r="M592" s="14"/>
+      <c r="N592" s="14"/>
+      <c r="O592" s="14"/>
+      <c r="P592" s="14"/>
+      <c r="Q592" s="14"/>
+      <c r="R592" s="14"/>
+      <c r="S592" s="14"/>
+      <c r="T592" s="14"/>
     </row>
     <row r="593" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A593" s="41"/>
-      <c r="B593" s="42"/>
-      <c r="C593" s="42"/>
-      <c r="D593" s="42"/>
-      <c r="E593" s="42"/>
-      <c r="F593" s="42"/>
-      <c r="G593" s="42"/>
-      <c r="H593" s="42"/>
-      <c r="I593" s="42"/>
-      <c r="J593" s="42"/>
-      <c r="K593" s="42"/>
-      <c r="L593" s="42"/>
-      <c r="M593" s="42"/>
-      <c r="N593" s="42"/>
-      <c r="O593" s="42"/>
-      <c r="P593" s="42"/>
-      <c r="Q593" s="42"/>
-      <c r="R593" s="42"/>
-      <c r="S593" s="42"/>
-      <c r="T593" s="42"/>
+      <c r="A593" s="42"/>
+      <c r="B593" s="43"/>
+      <c r="C593" s="43"/>
+      <c r="D593" s="43"/>
+      <c r="E593" s="43"/>
+      <c r="F593" s="43"/>
+      <c r="G593" s="43"/>
+      <c r="H593" s="43"/>
+      <c r="I593" s="43"/>
+      <c r="J593" s="43"/>
+      <c r="K593" s="43"/>
+      <c r="L593" s="43"/>
+      <c r="M593" s="43"/>
+      <c r="N593" s="43"/>
+      <c r="O593" s="43"/>
+      <c r="P593" s="43"/>
+      <c r="Q593" s="43"/>
+      <c r="R593" s="43"/>
+      <c r="S593" s="43"/>
+      <c r="T593" s="43"/>
     </row>
     <row r="594" spans="1:20" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B594" s="13"/>
-      <c r="C594" s="13"/>
-      <c r="D594" s="43"/>
-      <c r="E594" s="43"/>
-      <c r="F594" s="43"/>
-      <c r="G594" s="43"/>
-      <c r="H594" s="43"/>
-      <c r="I594" s="43"/>
+      <c r="B594" s="14"/>
+      <c r="C594" s="14"/>
+      <c r="D594" s="44"/>
+      <c r="E594" s="44"/>
+      <c r="F594" s="44"/>
+      <c r="G594" s="44"/>
+      <c r="H594" s="44"/>
+      <c r="I594" s="44"/>
       <c r="J594" s="2"/>
-      <c r="K594" s="44" t="s">
+      <c r="K594" s="45" t="s">
         <v>508</v>
       </c>
-      <c r="L594" s="44"/>
-      <c r="M594" s="44" t="s">
+      <c r="L594" s="45"/>
+      <c r="M594" s="45" t="s">
         <v>509</v>
       </c>
-      <c r="N594" s="44"/>
-      <c r="O594" s="44" t="s">
+      <c r="N594" s="45"/>
+      <c r="O594" s="45" t="s">
         <v>510</v>
       </c>
-      <c r="P594" s="44"/>
-      <c r="Q594" s="44" t="s">
+      <c r="P594" s="45"/>
+      <c r="Q594" s="45" t="s">
         <v>511</v>
       </c>
-      <c r="R594" s="44"/>
-      <c r="S594" s="13"/>
-      <c r="T594" s="13"/>
+      <c r="R594" s="45"/>
+      <c r="S594" s="14"/>
+      <c r="T594" s="14"/>
     </row>
     <row r="595" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A595" s="8"/>
-      <c r="B595" s="40"/>
-      <c r="C595" s="45"/>
-      <c r="D595" s="37" t="s">
+      <c r="A595" s="9"/>
+      <c r="B595" s="41"/>
+      <c r="C595" s="46"/>
+      <c r="D595" s="38" t="s">
         <v>502</v>
       </c>
-      <c r="E595" s="37"/>
-      <c r="F595" s="37"/>
-      <c r="G595" s="37"/>
-      <c r="H595" s="37" t="s">
+      <c r="E595" s="38"/>
+      <c r="F595" s="38"/>
+      <c r="G595" s="38"/>
+      <c r="H595" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="I595" s="46" t="s">
+      <c r="I595" s="47" t="s">
         <v>506</v>
       </c>
-      <c r="J595" s="8"/>
-      <c r="K595" s="37" t="s">
+      <c r="J595" s="9"/>
+      <c r="K595" s="38" t="s">
         <v>470</v>
       </c>
-      <c r="L595" s="37" t="s">
+      <c r="L595" s="38" t="s">
         <v>471</v>
       </c>
-      <c r="M595" s="37" t="s">
+      <c r="M595" s="38" t="s">
         <v>470</v>
       </c>
-      <c r="N595" s="37" t="s">
+      <c r="N595" s="38" t="s">
         <v>471</v>
       </c>
-      <c r="O595" s="37" t="s">
+      <c r="O595" s="38" t="s">
         <v>470</v>
       </c>
-      <c r="P595" s="37" t="s">
+      <c r="P595" s="38" t="s">
         <v>471</v>
       </c>
-      <c r="Q595" s="37" t="s">
+      <c r="Q595" s="38" t="s">
         <v>470</v>
       </c>
-      <c r="R595" s="37" t="s">
+      <c r="R595" s="38" t="s">
         <v>471</v>
       </c>
-      <c r="S595" s="13"/>
-      <c r="T595" s="13"/>
+      <c r="S595" s="14"/>
+      <c r="T595" s="14"/>
     </row>
     <row r="596" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B596" s="20" t="s">
+      <c r="B596" s="21" t="s">
         <v>489</v>
       </c>
       <c r="C596" s="1"/>
@@ -36984,38 +37013,38 @@
       <c r="H596" s="1">
         <v>90</v>
       </c>
-      <c r="I596" s="26">
+      <c r="I596" s="27">
         <v>86</v>
       </c>
-      <c r="K596" s="52">
+      <c r="K596" s="53">
         <v>131</v>
       </c>
-      <c r="L596" s="7">
+      <c r="L596" s="8">
         <v>52</v>
       </c>
-      <c r="M596" s="7">
+      <c r="M596" s="8">
         <v>123</v>
       </c>
-      <c r="N596" s="7">
+      <c r="N596" s="8">
         <v>71</v>
       </c>
-      <c r="O596" s="7">
+      <c r="O596" s="8">
         <v>111</v>
       </c>
-      <c r="P596" s="7">
+      <c r="P596" s="8">
         <v>52</v>
       </c>
-      <c r="Q596" s="7">
+      <c r="Q596" s="8">
         <v>123</v>
       </c>
-      <c r="R596" s="7">
+      <c r="R596" s="8">
         <v>79</v>
       </c>
-      <c r="S596" s="23"/>
-      <c r="T596" s="13"/>
+      <c r="S596" s="24"/>
+      <c r="T596" s="14"/>
     </row>
     <row r="597" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B597" s="21" t="s">
+      <c r="B597" s="22" t="s">
         <v>486</v>
       </c>
       <c r="C597" s="1"/>
@@ -37028,264 +37057,378 @@
       <c r="H597" s="1">
         <v>31</v>
       </c>
-      <c r="I597" s="27">
+      <c r="I597" s="28">
         <v>63</v>
       </c>
-      <c r="K597" s="49">
+      <c r="K597" s="50">
         <v>18</v>
       </c>
-      <c r="L597" s="7">
+      <c r="L597" s="8">
         <v>97</v>
       </c>
-      <c r="M597" s="7">
+      <c r="M597" s="8">
         <v>27</v>
       </c>
-      <c r="N597" s="7">
+      <c r="N597" s="8">
         <v>79</v>
       </c>
-      <c r="O597" s="7">
+      <c r="O597" s="8">
         <v>38</v>
       </c>
-      <c r="P597" s="7">
+      <c r="P597" s="8">
         <v>97</v>
       </c>
-      <c r="Q597" s="7">
+      <c r="Q597" s="8">
         <v>26</v>
       </c>
-      <c r="R597" s="7">
+      <c r="R597" s="8">
         <v>70</v>
       </c>
-      <c r="S597" s="23"/>
-      <c r="T597" s="13"/>
+      <c r="S597" s="24"/>
+      <c r="T597" s="14"/>
     </row>
     <row r="598" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B598" s="22" t="s">
+      <c r="B598" s="23" t="s">
         <v>482</v>
       </c>
-      <c r="C598" s="17"/>
-      <c r="D598" s="17">
+      <c r="C598" s="18"/>
+      <c r="D598" s="18">
         <v>22</v>
       </c>
-      <c r="E598" s="17"/>
-      <c r="F598" s="17"/>
-      <c r="G598" s="17"/>
-      <c r="H598" s="17">
+      <c r="E598" s="18"/>
+      <c r="F598" s="18"/>
+      <c r="G598" s="18"/>
+      <c r="H598" s="18">
         <v>6</v>
       </c>
-      <c r="I598" s="28">
+      <c r="I598" s="29">
         <v>11</v>
       </c>
-      <c r="K598" s="53">
+      <c r="K598" s="54">
         <v>34</v>
       </c>
-      <c r="L598" s="54">
-        <v>2</v>
-      </c>
-      <c r="M598" s="54">
+      <c r="L598" s="55">
+        <v>2</v>
+      </c>
+      <c r="M598" s="55">
         <v>26</v>
       </c>
-      <c r="N598" s="54">
+      <c r="N598" s="55">
         <v>3</v>
       </c>
-      <c r="O598" s="14">
+      <c r="O598" s="15">
         <v>31</v>
       </c>
-      <c r="P598" s="54">
-        <v>2</v>
-      </c>
-      <c r="Q598" s="14">
+      <c r="P598" s="55">
+        <v>2</v>
+      </c>
+      <c r="Q598" s="15">
         <v>14</v>
       </c>
-      <c r="R598" s="15">
+      <c r="R598" s="16">
         <v>3</v>
       </c>
-      <c r="S598" s="23"/>
-      <c r="T598" s="13"/>
+      <c r="S598" s="24"/>
+      <c r="T598" s="14"/>
     </row>
     <row r="599" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B599" s="21" t="s">
+      <c r="B599" s="22" t="s">
         <v>498</v>
       </c>
-      <c r="C599" s="16"/>
-      <c r="D599" s="31">
+      <c r="C599" s="17"/>
+      <c r="D599" s="32">
         <f>D596/(D596+D598)</f>
         <v>0.77777777777777779</v>
       </c>
-      <c r="E599" s="31"/>
-      <c r="F599" s="31"/>
-      <c r="G599" s="31"/>
-      <c r="H599" s="31">
+      <c r="E599" s="32"/>
+      <c r="F599" s="32"/>
+      <c r="G599" s="32"/>
+      <c r="H599" s="32">
         <f t="shared" ref="E599:K599" si="141">H596/(H596+H598)</f>
         <v>0.9375</v>
       </c>
-      <c r="I599" s="32">
+      <c r="I599" s="33">
         <f t="shared" si="141"/>
         <v>0.88659793814432986</v>
       </c>
-      <c r="K599" s="50">
+      <c r="K599" s="51">
         <f t="shared" si="141"/>
         <v>0.79393939393939394</v>
       </c>
-      <c r="L599" s="39">
+      <c r="L599" s="40">
         <f t="shared" ref="L599" si="142">L596/(L596+L598)</f>
         <v>0.96296296296296291</v>
       </c>
-      <c r="M599" s="39">
+      <c r="M599" s="40">
         <f t="shared" ref="M599" si="143">M596/(M596+M598)</f>
         <v>0.82550335570469802</v>
       </c>
-      <c r="N599" s="39">
+      <c r="N599" s="40">
         <f t="shared" ref="N599" si="144">N596/(N596+N598)</f>
         <v>0.95945945945945943</v>
       </c>
-      <c r="O599" s="39">
+      <c r="O599" s="40">
         <f t="shared" ref="O599" si="145">O596/(O596+O598)</f>
         <v>0.78169014084507038</v>
       </c>
-      <c r="P599" s="39">
+      <c r="P599" s="40">
         <f t="shared" ref="P599" si="146">P596/(P596+P598)</f>
         <v>0.96296296296296291</v>
       </c>
-      <c r="Q599" s="39">
+      <c r="Q599" s="40">
         <f t="shared" ref="Q599" si="147">Q596/(Q596+Q598)</f>
         <v>0.8978102189781022</v>
       </c>
-      <c r="R599" s="39">
+      <c r="R599" s="40">
         <f t="shared" ref="R599" si="148">R596/(R596+R598)</f>
         <v>0.96341463414634143</v>
       </c>
-      <c r="S599" s="50"/>
-      <c r="T599" s="39"/>
+      <c r="S599" s="51"/>
+      <c r="T599" s="40"/>
     </row>
     <row r="600" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B600" s="21" t="s">
+      <c r="B600" s="22" t="s">
         <v>499</v>
       </c>
-      <c r="C600" s="16"/>
-      <c r="D600" s="31">
+      <c r="C600" s="17"/>
+      <c r="D600" s="32">
         <f>D596/(D596+D597)</f>
         <v>0.51677852348993292</v>
       </c>
-      <c r="E600" s="31"/>
-      <c r="F600" s="31"/>
-      <c r="G600" s="31"/>
-      <c r="H600" s="31">
+      <c r="E600" s="32"/>
+      <c r="F600" s="32"/>
+      <c r="G600" s="32"/>
+      <c r="H600" s="32">
         <f t="shared" ref="E600:K600" si="149">H596/(H596+H597)</f>
         <v>0.74380165289256195</v>
       </c>
-      <c r="I600" s="33">
+      <c r="I600" s="34">
         <f t="shared" si="149"/>
         <v>0.57718120805369133</v>
       </c>
-      <c r="K600" s="50">
+      <c r="K600" s="51">
         <f t="shared" si="149"/>
         <v>0.87919463087248317</v>
       </c>
-      <c r="L600" s="39">
+      <c r="L600" s="40">
         <f t="shared" ref="L600:T600" si="150">L596/(L596+L597)</f>
         <v>0.34899328859060402</v>
       </c>
-      <c r="M600" s="39">
+      <c r="M600" s="40">
         <f t="shared" ref="M600:R600" si="151">M596/(M596+M597)</f>
         <v>0.82</v>
       </c>
-      <c r="N600" s="39">
+      <c r="N600" s="40">
         <f t="shared" si="151"/>
         <v>0.47333333333333333</v>
       </c>
-      <c r="O600" s="39">
+      <c r="O600" s="40">
         <f t="shared" si="151"/>
         <v>0.74496644295302017</v>
       </c>
-      <c r="P600" s="39">
+      <c r="P600" s="40">
         <f t="shared" si="151"/>
         <v>0.34899328859060402</v>
       </c>
-      <c r="Q600" s="39">
+      <c r="Q600" s="40">
         <f t="shared" si="151"/>
         <v>0.82550335570469802</v>
       </c>
-      <c r="R600" s="39">
+      <c r="R600" s="40">
         <f t="shared" si="151"/>
         <v>0.53020134228187921</v>
       </c>
-      <c r="S600" s="50"/>
-      <c r="T600" s="39"/>
+      <c r="S600" s="51"/>
+      <c r="T600" s="40"/>
     </row>
     <row r="601" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B601" s="25" t="s">
+      <c r="B601" s="26" t="s">
         <v>500</v>
       </c>
-      <c r="C601" s="18"/>
-      <c r="D601" s="34">
+      <c r="C601" s="19"/>
+      <c r="D601" s="35">
         <f>(2*D596)/((2*D596)+D598+D597)</f>
         <v>0.62096774193548387</v>
       </c>
-      <c r="E601" s="34"/>
-      <c r="F601" s="34"/>
-      <c r="G601" s="34"/>
-      <c r="H601" s="34">
+      <c r="E601" s="35"/>
+      <c r="F601" s="35"/>
+      <c r="G601" s="35"/>
+      <c r="H601" s="35">
         <f t="shared" ref="E601:K601" si="152">(2*H596)/((2*H596)+H598+H597)</f>
         <v>0.82949308755760365</v>
       </c>
-      <c r="I601" s="35">
+      <c r="I601" s="36">
         <f t="shared" si="152"/>
         <v>0.69918699186991873</v>
       </c>
-      <c r="K601" s="51">
+      <c r="K601" s="52">
         <f t="shared" si="152"/>
         <v>0.83439490445859876</v>
       </c>
-      <c r="L601" s="34">
+      <c r="L601" s="35">
         <f t="shared" ref="L601:T601" si="153">(2*L596)/((2*L596)+L598+L597)</f>
         <v>0.51231527093596063</v>
       </c>
-      <c r="M601" s="34">
+      <c r="M601" s="35">
         <f t="shared" ref="M601:R601" si="154">(2*M596)/((2*M596)+M598+M597)</f>
         <v>0.82274247491638797</v>
       </c>
-      <c r="N601" s="34">
+      <c r="N601" s="35">
         <f t="shared" si="154"/>
         <v>0.6339285714285714</v>
       </c>
-      <c r="O601" s="34">
+      <c r="O601" s="35">
         <f t="shared" si="154"/>
         <v>0.76288659793814428</v>
       </c>
-      <c r="P601" s="34">
+      <c r="P601" s="35">
         <f t="shared" si="154"/>
         <v>0.51231527093596063</v>
       </c>
-      <c r="Q601" s="34">
+      <c r="Q601" s="35">
         <f t="shared" si="154"/>
         <v>0.8601398601398601</v>
       </c>
-      <c r="R601" s="34">
+      <c r="R601" s="35">
         <f t="shared" si="154"/>
         <v>0.68398268398268403</v>
       </c>
-      <c r="S601" s="50"/>
-      <c r="T601" s="39"/>
+      <c r="S601" s="51"/>
+      <c r="T601" s="40"/>
     </row>
     <row r="602" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B602" s="13"/>
-      <c r="C602" s="13"/>
-      <c r="D602" s="13"/>
-      <c r="E602" s="13"/>
-      <c r="F602" s="13"/>
-      <c r="G602" s="13"/>
-      <c r="H602" s="13"/>
-      <c r="I602" s="13"/>
+      <c r="B602" s="14"/>
+      <c r="C602" s="14"/>
+      <c r="D602" s="14"/>
+      <c r="E602" s="14"/>
+      <c r="F602" s="14"/>
+      <c r="G602" s="14"/>
+      <c r="H602" s="14"/>
+      <c r="I602" s="14"/>
     </row>
     <row r="603" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B603" s="13"/>
-      <c r="C603" s="13"/>
-      <c r="D603" s="13"/>
-      <c r="E603" s="13"/>
-      <c r="F603" s="13"/>
-      <c r="G603" s="13"/>
-      <c r="H603" s="13"/>
-      <c r="I603" s="13"/>
+      <c r="B603" s="14"/>
+      <c r="C603" s="14"/>
+      <c r="D603" s="14"/>
+      <c r="E603" s="14"/>
+      <c r="F603" s="14"/>
+      <c r="G603" s="14"/>
+      <c r="H603" s="14"/>
+      <c r="I603" s="14"/>
+    </row>
+    <row r="610" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J610" s="7"/>
+      <c r="K610" s="57" t="s">
+        <v>512</v>
+      </c>
+      <c r="L610" s="7"/>
+      <c r="M610" s="7"/>
+      <c r="N610" s="7"/>
+    </row>
+    <row r="611" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J611" s="7"/>
+      <c r="K611" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="L611" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="M611" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="N611" s="58" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="612" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J612" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="K612" s="7">
+        <v>178</v>
+      </c>
+      <c r="L612" s="7">
+        <v>331</v>
+      </c>
+      <c r="M612" s="7">
+        <v>123</v>
+      </c>
+      <c r="N612" s="58">
+        <f>SUM(K612:M612)</f>
+        <v>632</v>
+      </c>
+    </row>
+    <row r="613" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J613" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="K613" s="7">
+        <v>4</v>
+      </c>
+      <c r="L613" s="7">
+        <v>54</v>
+      </c>
+      <c r="M613" s="59">
+        <v>26</v>
+      </c>
+      <c r="N613" s="58">
+        <f>SUM(K613:M613)</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="614" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J614" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="K614" s="7">
+        <v>5</v>
+      </c>
+      <c r="L614" s="7">
+        <v>29</v>
+      </c>
+      <c r="M614" s="59">
+        <v>14</v>
+      </c>
+      <c r="N614" s="58">
+        <f>SUM(K614:M614)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="615" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J615" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="K615" s="60"/>
+      <c r="L615" s="60"/>
+      <c r="M615" s="60"/>
+      <c r="N615" s="61">
+        <f>N612/(N612+N614)</f>
+        <v>0.92941176470588238</v>
+      </c>
+    </row>
+    <row r="616" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J616" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="K616" s="60"/>
+      <c r="L616" s="60"/>
+      <c r="M616" s="60"/>
+      <c r="N616" s="61">
+        <f>N612/(N612+N613)</f>
+        <v>0.88268156424581001</v>
+      </c>
+    </row>
+    <row r="617" spans="10:14" x14ac:dyDescent="0.2">
+      <c r="J617" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="K617" s="62"/>
+      <c r="L617" s="62"/>
+      <c r="M617" s="62"/>
+      <c r="N617" s="63">
+        <f>(2*N612)/((2*N612)+N614+N613)</f>
+        <v>0.90544412607449853</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>